<commit_message>
add ALU two operands micro routines with addresses
</commit_message>
<xml_diff>
--- a/Microroutines.xlsx
+++ b/Microroutines.xlsx
@@ -24,14 +24,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="121">
   <si>
     <t>Micro instruction</t>
   </si>
   <si>
-    <t>fetch &amp; decode:</t>
-  </si>
-  <si>
     <t>F0</t>
   </si>
   <si>
@@ -270,6 +267,126 @@
   </si>
   <si>
     <t>272</t>
+  </si>
+  <si>
+    <t>300</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SOURCE_out Y_in </t>
+  </si>
+  <si>
+    <t>304</t>
+  </si>
+  <si>
+    <t>314</t>
+  </si>
+  <si>
+    <t>310</t>
+  </si>
+  <si>
+    <t>ALU operations</t>
+  </si>
+  <si>
+    <t>DESTINATION</t>
+  </si>
+  <si>
+    <t>SOURCE</t>
+  </si>
+  <si>
+    <t>fetch &amp; decode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SOURCE_out Z_in Y_clear Add </t>
+  </si>
+  <si>
+    <t>DEST_out add Z_in FLAGS_in</t>
+  </si>
+  <si>
+    <t>MOV:</t>
+  </si>
+  <si>
+    <t>ADD:</t>
+  </si>
+  <si>
+    <t>ADC:</t>
+  </si>
+  <si>
+    <t>SUB:</t>
+  </si>
+  <si>
+    <t>SUBC:</t>
+  </si>
+  <si>
+    <t>DEST_out adc Z_in FLAGS_in</t>
+  </si>
+  <si>
+    <t>320</t>
+  </si>
+  <si>
+    <t>AND:</t>
+  </si>
+  <si>
+    <t>324</t>
+  </si>
+  <si>
+    <t>330</t>
+  </si>
+  <si>
+    <t>377</t>
+  </si>
+  <si>
+    <t>OR:</t>
+  </si>
+  <si>
+    <t>XOR:</t>
+  </si>
+  <si>
+    <t>334</t>
+  </si>
+  <si>
+    <t>DEST_out sub Z_in FLAGS_in</t>
+  </si>
+  <si>
+    <t>DEST_out sbc Z_in FLAGS_in</t>
+  </si>
+  <si>
+    <t>DEST_out and Z_in FLAGS_in</t>
+  </si>
+  <si>
+    <t>DEST_out or Z_in FLAGS_in</t>
+  </si>
+  <si>
+    <t>DEST_out xor Z_in FLAGS_in</t>
+  </si>
+  <si>
+    <t>CMP:</t>
+  </si>
+  <si>
+    <t>340</t>
+  </si>
+  <si>
+    <t>SAVE:</t>
+  </si>
+  <si>
+    <t>372</t>
+  </si>
+  <si>
+    <t>370</t>
+  </si>
+  <si>
+    <t>MDR_in Z_out</t>
+  </si>
+  <si>
+    <t>Write</t>
+  </si>
+  <si>
+    <t>371</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rdst_in Z_out </t>
+  </si>
+  <si>
+    <t>OR_res or bit 1</t>
   </si>
 </sst>
 </file>
@@ -357,7 +474,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
@@ -385,6 +502,17 @@
     <xf numFmtId="49" fontId="4" fillId="5" borderId="0" xfId="4" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="4" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Accent2" xfId="4" builtinId="33"/>
@@ -669,11 +797,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB44"/>
+  <dimension ref="A1:AB68"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A28" sqref="A28"/>
+      <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="V62" sqref="V62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -712,344 +840,370 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="L1" s="11"/>
+      <c r="M1" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="N1" s="12"/>
+      <c r="O1" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="P1" s="11"/>
+      <c r="Q1" s="11"/>
+      <c r="R1" s="11"/>
+      <c r="S1" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="T1" s="12"/>
+      <c r="U1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="L1" s="4"/>
-      <c r="M1" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="N1" s="5"/>
-      <c r="O1" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="P1" s="4"/>
-      <c r="Q1" s="4"/>
-      <c r="R1" s="4"/>
-      <c r="S1" s="5" t="s">
+      <c r="V1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="W1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="X1" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="T1" s="5"/>
-      <c r="U1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="V1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="W1" s="3" t="s">
+      <c r="Y1" s="12"/>
+      <c r="Z1" s="12"/>
+      <c r="AA1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="X1" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="Y1" s="5"/>
-      <c r="Z1" s="5"/>
-      <c r="AA1" s="3" t="s">
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
+      <c r="O2" s="11"/>
+      <c r="P2" s="11"/>
+      <c r="Q2" s="11"/>
+      <c r="R2" s="11"/>
+      <c r="S2" s="12"/>
+      <c r="T2" s="12"/>
+      <c r="X2" s="12"/>
+      <c r="Y2" s="12"/>
+      <c r="Z2" s="12"/>
+    </row>
+    <row r="3" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="14"/>
+      <c r="M3" s="14"/>
+      <c r="N3" s="14"/>
+      <c r="O3" s="14"/>
+      <c r="P3" s="14"/>
+      <c r="Q3" s="14"/>
+      <c r="R3" s="14"/>
+      <c r="S3" s="14"/>
+      <c r="T3" s="14"/>
+      <c r="U3" s="14"/>
+      <c r="V3" s="14"/>
+      <c r="W3" s="14"/>
+      <c r="X3" s="14"/>
+      <c r="Y3" s="14"/>
+      <c r="Z3" s="14"/>
+      <c r="AA3" s="14"/>
+    </row>
+    <row r="4" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="O2" s="4"/>
-      <c r="P2" s="4"/>
-      <c r="Q2" s="4"/>
-      <c r="R2" s="4"/>
-      <c r="S2" s="5"/>
-      <c r="T2" s="5"/>
-      <c r="X2" s="5"/>
-      <c r="Y2" s="5"/>
-      <c r="Z2" s="5"/>
-    </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+      <c r="B4" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0</v>
+      </c>
+      <c r="F4" s="3">
+        <v>0</v>
+      </c>
+      <c r="G4" s="3">
+        <v>1</v>
+      </c>
+      <c r="H4" s="2">
+        <v>0</v>
+      </c>
+      <c r="I4" s="2">
+        <v>1</v>
+      </c>
+      <c r="J4" s="2">
+        <v>1</v>
+      </c>
+      <c r="K4" s="3">
+        <v>0</v>
+      </c>
+      <c r="L4" s="3">
+        <v>1</v>
+      </c>
+      <c r="M4" s="2">
+        <v>0</v>
+      </c>
+      <c r="N4" s="2">
+        <v>1</v>
+      </c>
+      <c r="O4" s="3">
+        <v>0</v>
+      </c>
+      <c r="P4" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="3">
+        <v>0</v>
+      </c>
+      <c r="R4" s="3">
+        <v>0</v>
+      </c>
+      <c r="S4" s="2">
+        <v>0</v>
+      </c>
+      <c r="T4" s="2">
+        <v>1</v>
+      </c>
+      <c r="U4" s="3">
+        <v>1</v>
+      </c>
+      <c r="V4" s="2">
+        <v>1</v>
+      </c>
+      <c r="W4" s="3">
+        <v>0</v>
+      </c>
+      <c r="X4" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y4" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z4" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA4" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0</v>
+      </c>
+      <c r="F5" s="3">
+        <v>1</v>
+      </c>
+      <c r="G5" s="3">
+        <v>1</v>
+      </c>
+      <c r="H5" s="2">
+        <v>0</v>
+      </c>
+      <c r="I5" s="2">
+        <v>0</v>
+      </c>
+      <c r="J5" s="2">
+        <v>1</v>
+      </c>
+      <c r="K5" s="3">
+        <v>0</v>
+      </c>
+      <c r="L5" s="3">
+        <v>0</v>
+      </c>
+      <c r="M5" s="2">
+        <v>0</v>
+      </c>
+      <c r="N5" s="2">
+        <v>0</v>
+      </c>
+      <c r="O5" s="3">
+        <v>0</v>
+      </c>
+      <c r="P5" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="3">
+        <v>0</v>
+      </c>
+      <c r="R5" s="3">
+        <v>0</v>
+      </c>
+      <c r="S5" s="2">
+        <v>0</v>
+      </c>
+      <c r="T5" s="2">
+        <v>0</v>
+      </c>
+      <c r="U5" s="3">
+        <v>0</v>
+      </c>
+      <c r="V5" s="2">
+        <v>0</v>
+      </c>
+      <c r="W5" s="3">
+        <v>0</v>
+      </c>
+      <c r="X5" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y5" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z5" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA5" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0</v>
+      </c>
+      <c r="F6" s="3">
+        <v>1</v>
+      </c>
+      <c r="G6" s="3">
+        <v>0</v>
+      </c>
+      <c r="H6" s="2">
+        <v>0</v>
+      </c>
+      <c r="I6" s="2">
+        <v>1</v>
+      </c>
+      <c r="J6" s="2">
+        <v>0</v>
+      </c>
+      <c r="K6" s="3">
+        <v>0</v>
+      </c>
+      <c r="L6" s="3">
+        <v>0</v>
+      </c>
+      <c r="M6" s="2">
+        <v>0</v>
+      </c>
+      <c r="N6" s="2">
+        <v>0</v>
+      </c>
+      <c r="O6" s="3">
+        <v>0</v>
+      </c>
+      <c r="P6" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="3">
+        <v>0</v>
+      </c>
+      <c r="R6" s="3">
+        <v>0</v>
+      </c>
+      <c r="S6" s="2">
+        <v>0</v>
+      </c>
+      <c r="T6" s="2">
+        <v>0</v>
+      </c>
+      <c r="U6" s="3">
+        <v>0</v>
+      </c>
+      <c r="V6" s="2">
+        <v>0</v>
+      </c>
+      <c r="W6" s="3">
+        <v>0</v>
+      </c>
+      <c r="X6" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y6" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z6" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA6" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" s="3">
-        <v>0</v>
-      </c>
-      <c r="F4" s="3">
-        <v>0</v>
-      </c>
-      <c r="G4" s="3">
-        <v>1</v>
-      </c>
-      <c r="H4" s="2">
-        <v>0</v>
-      </c>
-      <c r="I4" s="2">
-        <v>1</v>
-      </c>
-      <c r="J4" s="2">
-        <v>1</v>
-      </c>
-      <c r="K4" s="3">
-        <v>0</v>
-      </c>
-      <c r="L4" s="3">
-        <v>1</v>
-      </c>
-      <c r="M4" s="2">
-        <v>0</v>
-      </c>
-      <c r="N4" s="2">
-        <v>1</v>
-      </c>
-      <c r="O4" s="3">
-        <v>0</v>
-      </c>
-      <c r="P4" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="3">
-        <v>0</v>
-      </c>
-      <c r="R4" s="3">
-        <v>0</v>
-      </c>
-      <c r="S4" s="2">
-        <v>0</v>
-      </c>
-      <c r="T4" s="2">
-        <v>1</v>
-      </c>
-      <c r="U4" s="3">
-        <v>1</v>
-      </c>
-      <c r="V4" s="2">
-        <v>1</v>
-      </c>
-      <c r="W4" s="3">
-        <v>0</v>
-      </c>
-      <c r="X4" s="2">
-        <v>0</v>
-      </c>
-      <c r="Y4" s="2">
-        <v>0</v>
-      </c>
-      <c r="Z4" s="2">
-        <v>0</v>
-      </c>
-      <c r="AA4" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="7" t="s">
+      <c r="B7" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="3">
-        <v>0</v>
-      </c>
-      <c r="F5" s="3">
-        <v>1</v>
-      </c>
-      <c r="G5" s="3">
-        <v>1</v>
-      </c>
-      <c r="H5" s="2">
-        <v>0</v>
-      </c>
-      <c r="I5" s="2">
-        <v>0</v>
-      </c>
-      <c r="J5" s="2">
-        <v>1</v>
-      </c>
-      <c r="K5" s="3">
-        <v>0</v>
-      </c>
-      <c r="L5" s="3">
-        <v>0</v>
-      </c>
-      <c r="M5" s="2">
-        <v>0</v>
-      </c>
-      <c r="N5" s="2">
-        <v>0</v>
-      </c>
-      <c r="O5" s="3">
-        <v>0</v>
-      </c>
-      <c r="P5" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="3">
-        <v>0</v>
-      </c>
-      <c r="R5" s="3">
-        <v>0</v>
-      </c>
-      <c r="S5" s="2">
-        <v>0</v>
-      </c>
-      <c r="T5" s="2">
-        <v>0</v>
-      </c>
-      <c r="U5" s="3">
-        <v>0</v>
-      </c>
-      <c r="V5" s="2">
-        <v>0</v>
-      </c>
-      <c r="W5" s="3">
-        <v>0</v>
-      </c>
-      <c r="X5" s="2">
-        <v>0</v>
-      </c>
-      <c r="Y5" s="2">
-        <v>0</v>
-      </c>
-      <c r="Z5" s="2">
-        <v>0</v>
-      </c>
-      <c r="AA5" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" s="3">
-        <v>0</v>
-      </c>
-      <c r="F6" s="3">
-        <v>1</v>
-      </c>
-      <c r="G6" s="3">
-        <v>0</v>
-      </c>
-      <c r="H6" s="2">
-        <v>0</v>
-      </c>
-      <c r="I6" s="2">
-        <v>1</v>
-      </c>
-      <c r="J6" s="2">
-        <v>0</v>
-      </c>
-      <c r="K6" s="3">
-        <v>0</v>
-      </c>
-      <c r="L6" s="3">
-        <v>0</v>
-      </c>
-      <c r="M6" s="2">
-        <v>0</v>
-      </c>
-      <c r="N6" s="2">
-        <v>0</v>
-      </c>
-      <c r="O6" s="3">
-        <v>0</v>
-      </c>
-      <c r="P6" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q6" s="3">
-        <v>0</v>
-      </c>
-      <c r="R6" s="3">
-        <v>0</v>
-      </c>
-      <c r="S6" s="2">
-        <v>0</v>
-      </c>
-      <c r="T6" s="2">
-        <v>0</v>
-      </c>
-      <c r="U6" s="3">
-        <v>0</v>
-      </c>
-      <c r="V6" s="2">
-        <v>0</v>
-      </c>
-      <c r="W6" s="3">
-        <v>0</v>
-      </c>
-      <c r="X6" s="2">
-        <v>0</v>
-      </c>
-      <c r="Y6" s="2">
-        <v>0</v>
-      </c>
-      <c r="Z6" s="2">
-        <v>0</v>
-      </c>
-      <c r="AA6" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>16</v>
-      </c>
       <c r="C7" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E7" s="3">
         <v>0</v>
@@ -1120,15 +1274,46 @@
       <c r="AA7" s="3">
         <v>1</v>
       </c>
+    </row>
+    <row r="8" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="14"/>
+      <c r="L8" s="14"/>
+      <c r="M8" s="14"/>
+      <c r="N8" s="14"/>
+      <c r="O8" s="14"/>
+      <c r="P8" s="14"/>
+      <c r="Q8" s="14"/>
+      <c r="R8" s="14"/>
+      <c r="S8" s="14"/>
+      <c r="T8" s="14"/>
+      <c r="U8" s="14"/>
+      <c r="V8" s="14"/>
+      <c r="W8" s="14"/>
+      <c r="X8" s="14"/>
+      <c r="Y8" s="14"/>
+      <c r="Z8" s="14"/>
+      <c r="AA8" s="14"/>
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B10" s="6">
         <v>101</v>
@@ -1137,90 +1322,90 @@
         <v>201</v>
       </c>
       <c r="D10" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="E10" s="8" t="s">
-        <v>18</v>
-      </c>
       <c r="F10" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="I10" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="J10" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="K10" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="L10" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="M10" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="G10" s="8" t="s">
+      <c r="N10" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="O10" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="P10" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q10" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="R10" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="S10" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="T10" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="U10" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="V10" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="W10" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="X10" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y10" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="Z10" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="H10" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="I10" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="J10" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="K10" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="L10" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="M10" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="N10" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="O10" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="P10" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q10" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="R10" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="S10" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="T10" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="U10" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="V10" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="W10" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="X10" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="Y10" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="Z10" s="7" t="s">
-        <v>18</v>
-      </c>
       <c r="AA10" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>22</v>
-      </c>
       <c r="D11" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E11" s="3">
         <v>1</v>
@@ -1294,16 +1479,16 @@
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E12" s="3">
         <v>0</v>
@@ -1377,16 +1562,16 @@
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B13" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="7" t="s">
-        <v>26</v>
-      </c>
       <c r="D13" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E13" s="3">
         <v>1</v>
@@ -1460,16 +1645,16 @@
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E14" s="3">
         <v>0</v>
@@ -1543,16 +1728,16 @@
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B15" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>31</v>
-      </c>
       <c r="D15" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E15" s="3">
         <v>1</v>
@@ -1626,13 +1811,13 @@
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" s="7" t="s">
         <v>32</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>33</v>
       </c>
       <c r="D16" s="3">
         <v>0</v>
@@ -1709,13 +1894,13 @@
     </row>
     <row r="17" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D17" s="3">
         <v>0</v>
@@ -1792,16 +1977,16 @@
     </row>
     <row r="18" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B18" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C18" s="7" t="s">
-        <v>35</v>
-      </c>
       <c r="D18" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E18" s="3">
         <v>0</v>
@@ -1875,16 +2060,16 @@
     </row>
     <row r="19" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E19" s="3">
         <v>0</v>
@@ -1958,16 +2143,16 @@
     </row>
     <row r="20" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C20" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="B20" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>40</v>
-      </c>
       <c r="D20" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E20" s="3">
         <v>0</v>
@@ -2041,16 +2226,16 @@
     </row>
     <row r="21" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C21" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="B21" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>42</v>
-      </c>
       <c r="D21" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E21" s="3">
         <v>1</v>
@@ -2124,16 +2309,16 @@
     </row>
     <row r="22" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E22" s="3">
         <v>0</v>
@@ -2207,16 +2392,16 @@
     </row>
     <row r="23" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E23" s="3">
         <v>0</v>
@@ -2290,16 +2475,16 @@
     </row>
     <row r="24" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E24" s="3">
         <v>0</v>
@@ -2371,21 +2556,21 @@
         <v>0</v>
       </c>
       <c r="AB24" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="25" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E25" s="3">
         <v>0</v>
@@ -2459,16 +2644,16 @@
     </row>
     <row r="26" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E26" s="3">
         <v>0</v>
@@ -2541,6 +2726,9 @@
       </c>
     </row>
     <row r="27" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="9" t="s">
+        <v>87</v>
+      </c>
       <c r="B27" s="10"/>
       <c r="C27" s="10"/>
       <c r="D27" s="10"/>
@@ -2570,1414 +2758,1860 @@
     </row>
     <row r="28" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>102</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F28" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G28" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H28" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I28" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J28" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K28" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L28" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M28" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="N28" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O28" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="P28" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="Q28" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="R28" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="S28" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="T28" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="U28" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="V28" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="W28" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="X28" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="Y28" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="Z28" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AA28" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="29" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
+        <v>58</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C29" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="B29" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="C29" s="7" t="s">
-        <v>60</v>
-      </c>
       <c r="D29" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F29" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G29" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H29" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I29" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J29" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K29" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L29" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M29" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="N29" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O29" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="P29" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="Q29" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="R29" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="S29" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="T29" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="U29" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="V29" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="W29" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="X29" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="Y29" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="Z29" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AA29" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="30" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E30" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F30" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G30" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H30" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I30" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J30" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K30" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L30" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M30" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="N30" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O30" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="P30" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="Q30" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="R30" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="S30" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="T30" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="U30" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="V30" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="W30" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="X30" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="Y30" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="Z30" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AA30" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="31" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B31" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C31" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="C31" s="7" t="s">
-        <v>69</v>
-      </c>
       <c r="D31" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E31" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F31" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G31" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H31" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I31" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J31" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K31" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L31" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M31" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="N31" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O31" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="P31" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="Q31" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="R31" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="S31" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="T31" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="U31" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="V31" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="W31" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="X31" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="Y31" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="Z31" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AA31" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="32" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E32" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F32" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G32" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H32" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I32" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J32" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K32" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L32" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M32" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="N32" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O32" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="P32" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="Q32" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="R32" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="S32" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="T32" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="U32" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="V32" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="W32" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="X32" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="Y32" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="Z32" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AA32" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="33" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B33" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C33" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="C33" s="7" t="s">
-        <v>71</v>
-      </c>
       <c r="D33" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E33" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F33" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G33" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H33" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I33" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J33" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K33" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L33" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M33" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="N33" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O33" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="P33" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="Q33" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="R33" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="S33" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="T33" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="U33" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="V33" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="W33" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="X33" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="Y33" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="Z33" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AA33" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="34" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B34" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C34" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="C34" s="7" t="s">
-        <v>72</v>
-      </c>
       <c r="D34" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E34" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F34" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G34" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H34" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I34" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J34" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K34" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L34" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M34" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="N34" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O34" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="P34" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="Q34" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="R34" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="S34" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="T34" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="U34" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="V34" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="W34" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="X34" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="Y34" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="Z34" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AA34" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="35" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E35" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F35" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G35" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H35" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I35" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J35" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K35" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L35" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M35" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="N35" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O35" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="P35" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="Q35" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="R35" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="S35" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="T35" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="U35" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="V35" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="W35" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="X35" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="Y35" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="Z35" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AA35" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="36" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B36" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C36" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="C36" s="7" t="s">
-        <v>74</v>
-      </c>
       <c r="D36" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E36" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F36" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G36" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H36" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I36" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J36" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K36" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L36" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M36" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="N36" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O36" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="P36" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="Q36" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="R36" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="S36" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="T36" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="U36" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="V36" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="W36" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="X36" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="Y36" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="Z36" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AA36" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="37" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B37" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C37" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="C37" s="7" t="s">
-        <v>75</v>
-      </c>
       <c r="D37" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E37" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F37" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G37" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H37" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I37" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J37" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K37" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L37" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M37" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="N37" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O37" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="P37" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="Q37" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="R37" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="S37" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="T37" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="U37" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="V37" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="W37" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="X37" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="Y37" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="Z37" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AA37" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="38" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B38" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="C38" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="C38" s="7" t="s">
-        <v>76</v>
-      </c>
       <c r="D38" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E38" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F38" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G38" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H38" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I38" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J38" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K38" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L38" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M38" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="N38" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O38" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="P38" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="Q38" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="R38" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="S38" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="T38" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="U38" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="V38" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="W38" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="X38" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="Y38" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="Z38" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AA38" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="39" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B39" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="C39" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="C39" s="7" t="s">
-        <v>77</v>
-      </c>
       <c r="D39" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E39" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F39" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G39" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H39" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I39" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J39" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K39" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L39" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M39" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="N39" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O39" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="P39" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="Q39" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="R39" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="S39" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="T39" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="U39" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="V39" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="W39" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="X39" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="Y39" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="Z39" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AA39" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="40" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B40" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C40" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="C40" s="7" t="s">
-        <v>78</v>
-      </c>
       <c r="D40" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E40" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F40" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G40" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H40" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I40" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J40" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K40" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L40" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M40" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="N40" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O40" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="P40" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="Q40" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="R40" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="S40" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="T40" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="U40" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="V40" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="W40" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="X40" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="Y40" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="Z40" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AA40" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="41" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B41" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="C41" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="C41" s="7" t="s">
-        <v>79</v>
-      </c>
       <c r="D41" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E41" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F41" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G41" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H41" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I41" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J41" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K41" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L41" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M41" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="N41" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O41" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="P41" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="Q41" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="R41" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="S41" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="T41" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="U41" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="V41" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="W41" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="X41" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="Y41" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="Z41" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AA41" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="42" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B42" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="C42" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="C42" s="7" t="s">
-        <v>80</v>
-      </c>
       <c r="D42" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E42" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F42" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G42" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H42" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I42" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J42" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K42" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L42" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M42" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="N42" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O42" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="P42" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="Q42" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="R42" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="S42" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="T42" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="U42" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="V42" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="W42" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="X42" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="Y42" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="Z42" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AA42" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AB42" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="43" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B43" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C43" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="C43" s="7" t="s">
-        <v>81</v>
-      </c>
       <c r="D43" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E43" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F43" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G43" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H43" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I43" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J43" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K43" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L43" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M43" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="N43" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O43" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="P43" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="Q43" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="R43" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="S43" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="T43" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="U43" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="V43" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="W43" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="X43" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="Y43" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="Z43" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AA43" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="44" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>48</v>
+        <v>80</v>
+      </c>
+      <c r="C44" s="7" t="s">
+        <v>102</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E44" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F44" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G44" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H44" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I44" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J44" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K44" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L44" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M44" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="N44" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O44" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="P44" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="Q44" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="R44" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="S44" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="T44" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="U44" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="V44" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="W44" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="X44" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="Y44" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="Z44" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AA44" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="45" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="B45" s="10"/>
+      <c r="C45" s="10"/>
+      <c r="D45" s="10"/>
+      <c r="E45" s="14"/>
+      <c r="F45" s="14"/>
+      <c r="G45" s="14"/>
+      <c r="H45" s="14"/>
+      <c r="I45" s="14"/>
+      <c r="J45" s="14"/>
+      <c r="K45" s="14"/>
+      <c r="L45" s="14"/>
+      <c r="M45" s="14"/>
+      <c r="N45" s="14"/>
+      <c r="O45" s="14"/>
+      <c r="P45" s="14"/>
+      <c r="Q45" s="14"/>
+      <c r="R45" s="14"/>
+      <c r="S45" s="14"/>
+      <c r="T45" s="14"/>
+      <c r="U45" s="14"/>
+      <c r="V45" s="14"/>
+      <c r="W45" s="14"/>
+      <c r="X45" s="14"/>
+      <c r="Y45" s="14"/>
+      <c r="Z45" s="14"/>
+      <c r="AA45" s="14"/>
+    </row>
+    <row r="46" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A46" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="B46" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="C46" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="X46" s="2">
+        <v>1</v>
+      </c>
+      <c r="Y46" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z46" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A47" s="15" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="48" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A48" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="B48" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C48" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="X48" s="2">
+        <v>1</v>
+      </c>
+      <c r="Y48" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z48" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A49" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="E49" s="4"/>
+      <c r="F49" s="4"/>
+      <c r="G49" s="4"/>
+      <c r="H49" s="5"/>
+      <c r="I49" s="5"/>
+      <c r="J49" s="5"/>
+      <c r="K49" s="4"/>
+      <c r="L49" s="4"/>
+      <c r="M49" s="5"/>
+      <c r="N49" s="5"/>
+      <c r="O49" s="4"/>
+      <c r="P49" s="4"/>
+      <c r="Q49" s="4"/>
+      <c r="R49" s="4"/>
+      <c r="S49" s="5"/>
+      <c r="T49" s="5"/>
+      <c r="U49" s="4"/>
+      <c r="V49" s="5"/>
+      <c r="W49" s="4"/>
+      <c r="X49" s="5"/>
+      <c r="Y49" s="5"/>
+      <c r="Z49" s="5"/>
+      <c r="AA49" s="4"/>
+    </row>
+    <row r="50" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A50" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="B50" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="C50" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="X50" s="2">
+        <v>1</v>
+      </c>
+      <c r="Y50" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z50" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A51" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="E51" s="4"/>
+      <c r="F51" s="4"/>
+      <c r="G51" s="4"/>
+      <c r="H51" s="5"/>
+      <c r="I51" s="5"/>
+      <c r="J51" s="5"/>
+      <c r="K51" s="4"/>
+      <c r="L51" s="4"/>
+      <c r="M51" s="5"/>
+      <c r="N51" s="5"/>
+      <c r="O51" s="4"/>
+      <c r="P51" s="4"/>
+      <c r="Q51" s="4"/>
+      <c r="R51" s="4"/>
+      <c r="S51" s="5"/>
+      <c r="T51" s="5"/>
+      <c r="U51" s="4"/>
+      <c r="V51" s="5"/>
+      <c r="W51" s="4"/>
+      <c r="X51" s="5"/>
+      <c r="Y51" s="5"/>
+      <c r="Z51" s="5"/>
+      <c r="AA51" s="4"/>
+    </row>
+    <row r="52" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A52" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="B52" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="C52" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="X52" s="2">
+        <v>1</v>
+      </c>
+      <c r="Y52" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z52" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A53" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="E53" s="4"/>
+      <c r="F53" s="4"/>
+      <c r="G53" s="4"/>
+      <c r="H53" s="5"/>
+      <c r="I53" s="5"/>
+      <c r="J53" s="5"/>
+      <c r="K53" s="4"/>
+      <c r="L53" s="4"/>
+      <c r="M53" s="5"/>
+      <c r="N53" s="5"/>
+      <c r="O53" s="4"/>
+      <c r="P53" s="4"/>
+      <c r="Q53" s="4"/>
+      <c r="R53" s="4"/>
+      <c r="S53" s="5"/>
+      <c r="T53" s="5"/>
+      <c r="U53" s="4"/>
+      <c r="V53" s="5"/>
+      <c r="W53" s="4"/>
+      <c r="X53" s="5"/>
+      <c r="Y53" s="5"/>
+      <c r="Z53" s="5"/>
+      <c r="AA53" s="4"/>
+    </row>
+    <row r="54" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A54" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="B54" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="C54" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="X54" s="2">
+        <v>1</v>
+      </c>
+      <c r="Y54" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z54" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A55" s="15" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="56" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A56" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="B56" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C56" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="X56" s="2">
+        <v>1</v>
+      </c>
+      <c r="Y56" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z56" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A57" s="13" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="58" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A58" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="B58" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="C58" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="X58" s="2">
+        <v>1</v>
+      </c>
+      <c r="Y58" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z58" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A59" s="15" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="60" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A60" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="B60" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="C60" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="X60" s="2">
+        <v>1</v>
+      </c>
+      <c r="Y60" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z60" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A61" s="13" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="62" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A62" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="B62" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="C62" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="X62" s="2">
+        <v>1</v>
+      </c>
+      <c r="Y62" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z62" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A63" s="15" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="64" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A64" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="B64" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="C64" s="5">
+        <v>0</v>
+      </c>
+      <c r="D64" s="4"/>
+      <c r="E64" s="4"/>
+      <c r="F64" s="4"/>
+      <c r="G64" s="4"/>
+      <c r="H64" s="5"/>
+      <c r="I64" s="5"/>
+      <c r="J64" s="5"/>
+      <c r="K64" s="4"/>
+      <c r="L64" s="4"/>
+      <c r="M64" s="5"/>
+      <c r="N64" s="5"/>
+      <c r="O64" s="4"/>
+      <c r="P64" s="4"/>
+      <c r="Q64" s="4"/>
+      <c r="R64" s="4"/>
+      <c r="S64" s="5"/>
+      <c r="T64" s="5"/>
+      <c r="U64" s="4"/>
+      <c r="V64" s="5"/>
+      <c r="W64" s="4"/>
+      <c r="X64" s="5"/>
+      <c r="Y64" s="5"/>
+      <c r="AA64" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="B65" s="10"/>
+      <c r="C65" s="10"/>
+      <c r="D65" s="10"/>
+      <c r="E65" s="14"/>
+      <c r="F65" s="14"/>
+      <c r="G65" s="14"/>
+      <c r="H65" s="14"/>
+      <c r="I65" s="14"/>
+      <c r="J65" s="14"/>
+      <c r="K65" s="14"/>
+      <c r="L65" s="14"/>
+      <c r="M65" s="14"/>
+      <c r="N65" s="14"/>
+      <c r="O65" s="14"/>
+      <c r="P65" s="14"/>
+      <c r="Q65" s="14"/>
+      <c r="R65" s="14"/>
+      <c r="S65" s="14"/>
+      <c r="T65" s="14"/>
+      <c r="U65" s="14"/>
+      <c r="V65" s="14"/>
+      <c r="W65" s="14"/>
+      <c r="X65" s="14"/>
+      <c r="Y65" s="14"/>
+      <c r="Z65" s="14"/>
+      <c r="AA65" s="14"/>
+    </row>
+    <row r="66" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>116</v>
+      </c>
+      <c r="B66" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="C66" s="7" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="67" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>117</v>
+      </c>
+      <c r="B67" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="C67" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA67" s="3">
+        <v>1</v>
+      </c>
+      <c r="AB67" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="68" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>119</v>
+      </c>
+      <c r="B68" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="C68" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA68" s="3">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="D2:G2"/>
+    <mergeCell ref="O2:R2"/>
+    <mergeCell ref="S2:T2"/>
+    <mergeCell ref="X2:Z2"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="K2:L2"/>
     <mergeCell ref="D1:G1"/>
     <mergeCell ref="M1:N1"/>
     <mergeCell ref="X1:Z1"/>
@@ -3985,12 +4619,6 @@
     <mergeCell ref="O1:R1"/>
     <mergeCell ref="K1:L1"/>
     <mergeCell ref="H1:J1"/>
-    <mergeCell ref="O2:R2"/>
-    <mergeCell ref="S2:T2"/>
-    <mergeCell ref="X2:Z2"/>
-    <mergeCell ref="H2:J2"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="D2:G2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
add: single operand alu operations.
</commit_message>
<xml_diff>
--- a/Microroutines.xlsx
+++ b/Microroutines.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="155">
   <si>
     <t>Micro instruction</t>
   </si>
@@ -173,9 +173,6 @@
     <t>SOURCE_in MDR_out</t>
   </si>
   <si>
-    <t>Oring with bit 1</t>
-  </si>
-  <si>
     <t>F1: 4-bit</t>
   </si>
   <si>
@@ -269,27 +266,9 @@
     <t>272</t>
   </si>
   <si>
-    <t>300</t>
-  </si>
-  <si>
     <t xml:space="preserve">SOURCE_out Y_in </t>
   </si>
   <si>
-    <t>304</t>
-  </si>
-  <si>
-    <t>314</t>
-  </si>
-  <si>
-    <t>310</t>
-  </si>
-  <si>
-    <t>ALU operations</t>
-  </si>
-  <si>
-    <t>DESTINATION</t>
-  </si>
-  <si>
     <t>SOURCE</t>
   </si>
   <si>
@@ -320,30 +299,15 @@
     <t>DEST_out adc Z_in FLAGS_in</t>
   </si>
   <si>
-    <t>320</t>
-  </si>
-  <si>
     <t>AND:</t>
   </si>
   <si>
-    <t>324</t>
-  </si>
-  <si>
-    <t>330</t>
-  </si>
-  <si>
-    <t>377</t>
-  </si>
-  <si>
     <t>OR:</t>
   </si>
   <si>
     <t>XOR:</t>
   </si>
   <si>
-    <t>334</t>
-  </si>
-  <si>
     <t>DEST_out sub Z_in FLAGS_in</t>
   </si>
   <si>
@@ -362,31 +326,169 @@
     <t>CMP:</t>
   </si>
   <si>
-    <t>340</t>
-  </si>
-  <si>
     <t>SAVE:</t>
   </si>
   <si>
-    <t>372</t>
-  </si>
-  <si>
-    <t>370</t>
-  </si>
-  <si>
     <t>MDR_in Z_out</t>
   </si>
   <si>
     <t>Write</t>
   </si>
   <si>
-    <t>371</t>
-  </si>
-  <si>
     <t xml:space="preserve">Rdst_in Z_out </t>
   </si>
   <si>
     <t>OR_res or bit 1</t>
+  </si>
+  <si>
+    <t>ALU operations (2 Operands)</t>
+  </si>
+  <si>
+    <t>OR_indsrc or bit 1</t>
+  </si>
+  <si>
+    <t>OR_indst or bit 1</t>
+  </si>
+  <si>
+    <t>DESTINATION; base address of single operands</t>
+  </si>
+  <si>
+    <t>400</t>
+  </si>
+  <si>
+    <t>477</t>
+  </si>
+  <si>
+    <t>470</t>
+  </si>
+  <si>
+    <t>410</t>
+  </si>
+  <si>
+    <t>404</t>
+  </si>
+  <si>
+    <t>414</t>
+  </si>
+  <si>
+    <t>420</t>
+  </si>
+  <si>
+    <t>424</t>
+  </si>
+  <si>
+    <t>430</t>
+  </si>
+  <si>
+    <t>434</t>
+  </si>
+  <si>
+    <t>440</t>
+  </si>
+  <si>
+    <t>471</t>
+  </si>
+  <si>
+    <t>472</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>OR_sng or bit 6</t>
+  </si>
+  <si>
+    <t>577</t>
+  </si>
+  <si>
+    <t>500</t>
+  </si>
+  <si>
+    <t>INC:</t>
+  </si>
+  <si>
+    <t>DEC:</t>
+  </si>
+  <si>
+    <t>CLR:</t>
+  </si>
+  <si>
+    <t>Z_in clr</t>
+  </si>
+  <si>
+    <t>INV:</t>
+  </si>
+  <si>
+    <t>NOTES</t>
+  </si>
+  <si>
+    <t>LSR:</t>
+  </si>
+  <si>
+    <t>DEST_out Z_in clear_Y Carry_in add FLAGS_in</t>
+  </si>
+  <si>
+    <t>DEST_out Z_in clear_Y sub FLAGS_in</t>
+  </si>
+  <si>
+    <t>DEST_out Z_in NOT FLAGS_in</t>
+  </si>
+  <si>
+    <t>ALU: Op on the Operand on the bus</t>
+  </si>
+  <si>
+    <t>ROR:</t>
+  </si>
+  <si>
+    <t>DEST_out Z_in ROR FLAG_in</t>
+  </si>
+  <si>
+    <t>DEST_out Z_in LSR FLAG_in</t>
+  </si>
+  <si>
+    <t>ASR:</t>
+  </si>
+  <si>
+    <t>DEST_out Z_in ASR FLAG_in</t>
+  </si>
+  <si>
+    <t>LSL:</t>
+  </si>
+  <si>
+    <t>DEST_out Z_in LSL FLAG_in</t>
+  </si>
+  <si>
+    <t>ROL:</t>
+  </si>
+  <si>
+    <t>DEST_out Z_in ROL FLAG_in</t>
+  </si>
+  <si>
+    <t>504</t>
+  </si>
+  <si>
+    <t>520</t>
+  </si>
+  <si>
+    <t>514</t>
+  </si>
+  <si>
+    <t>510</t>
+  </si>
+  <si>
+    <t>524</t>
+  </si>
+  <si>
+    <t>530</t>
+  </si>
+  <si>
+    <t>534</t>
+  </si>
+  <si>
+    <t>540</t>
+  </si>
+  <si>
+    <t>ALU operations (Single Operand)</t>
   </si>
 </sst>
 </file>
@@ -474,7 +576,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
@@ -502,17 +604,35 @@
     <xf numFmtId="49" fontId="4" fillId="5" borderId="0" xfId="4" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="4" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="4" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="4" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Accent2" xfId="4" builtinId="33"/>
@@ -797,11 +917,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB68"/>
+  <dimension ref="A1:AB88"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="V62" sqref="V62"/>
+      <pane ySplit="1" topLeftCell="A66" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AB73" sqref="AB73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -832,10 +952,10 @@
     <col min="25" max="25" width="3.5546875" style="2" customWidth="1"/>
     <col min="26" max="26" width="3.6640625" style="2" customWidth="1"/>
     <col min="27" max="27" width="3.44140625" style="3" customWidth="1"/>
-    <col min="28" max="28" width="13.44140625" customWidth="1"/>
+    <col min="28" max="28" width="30.5546875" style="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -845,35 +965,35 @@
       <c r="C1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="L1" s="16"/>
+      <c r="M1" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="12" t="s">
+      <c r="N1" s="17"/>
+      <c r="O1" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="L1" s="11"/>
-      <c r="M1" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="N1" s="12"/>
-      <c r="O1" s="11" t="s">
+      <c r="P1" s="16"/>
+      <c r="Q1" s="16"/>
+      <c r="R1" s="16"/>
+      <c r="S1" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="P1" s="11"/>
-      <c r="Q1" s="11"/>
-      <c r="R1" s="11"/>
-      <c r="S1" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="T1" s="12"/>
+      <c r="T1" s="17"/>
       <c r="U1" s="3" t="s">
         <v>2</v>
       </c>
@@ -883,67 +1003,71 @@
       <c r="W1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="X1" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="Y1" s="12"/>
-      <c r="Z1" s="12"/>
+      <c r="X1" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="Y1" s="17"/>
+      <c r="Z1" s="17"/>
       <c r="AA1" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="11"/>
-      <c r="L2" s="11"/>
-      <c r="O2" s="11"/>
-      <c r="P2" s="11"/>
-      <c r="Q2" s="11"/>
-      <c r="R2" s="11"/>
-      <c r="S2" s="12"/>
-      <c r="T2" s="12"/>
-      <c r="X2" s="12"/>
-      <c r="Y2" s="12"/>
-      <c r="Z2" s="12"/>
-    </row>
-    <row r="3" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="AB1" s="18" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="16"/>
+      <c r="L2" s="16"/>
+      <c r="O2" s="16"/>
+      <c r="P2" s="16"/>
+      <c r="Q2" s="16"/>
+      <c r="R2" s="16"/>
+      <c r="S2" s="17"/>
+      <c r="T2" s="17"/>
+      <c r="X2" s="17"/>
+      <c r="Y2" s="17"/>
+      <c r="Z2" s="17"/>
+    </row>
+    <row r="3" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="B3" s="10"/>
       <c r="C3" s="10"/>
       <c r="D3" s="10"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="14"/>
-      <c r="L3" s="14"/>
-      <c r="M3" s="14"/>
-      <c r="N3" s="14"/>
-      <c r="O3" s="14"/>
-      <c r="P3" s="14"/>
-      <c r="Q3" s="14"/>
-      <c r="R3" s="14"/>
-      <c r="S3" s="14"/>
-      <c r="T3" s="14"/>
-      <c r="U3" s="14"/>
-      <c r="V3" s="14"/>
-      <c r="W3" s="14"/>
-      <c r="X3" s="14"/>
-      <c r="Y3" s="14"/>
-      <c r="Z3" s="14"/>
-      <c r="AA3" s="14"/>
-    </row>
-    <row r="4" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="12"/>
+      <c r="L3" s="12"/>
+      <c r="M3" s="12"/>
+      <c r="N3" s="12"/>
+      <c r="O3" s="12"/>
+      <c r="P3" s="12"/>
+      <c r="Q3" s="12"/>
+      <c r="R3" s="12"/>
+      <c r="S3" s="12"/>
+      <c r="T3" s="12"/>
+      <c r="U3" s="12"/>
+      <c r="V3" s="12"/>
+      <c r="W3" s="12"/>
+      <c r="X3" s="12"/>
+      <c r="Y3" s="12"/>
+      <c r="Z3" s="12"/>
+      <c r="AA3" s="12"/>
+      <c r="AB3" s="20"/>
+    </row>
+    <row r="4" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1025,8 +1149,9 @@
       <c r="AA4" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="AB4" s="21"/>
+    </row>
+    <row r="5" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -1108,8 +1233,9 @@
       <c r="AA5" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="AB5" s="21"/>
+    </row>
+    <row r="6" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -1191,8 +1317,9 @@
       <c r="AA6" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="AB6" s="21"/>
+    </row>
+    <row r="7" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1274,44 +1401,46 @@
       <c r="AA7" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="AB7" s="21"/>
+    </row>
+    <row r="8" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="B8" s="10"/>
       <c r="C8" s="10"/>
       <c r="D8" s="10"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="14"/>
-      <c r="L8" s="14"/>
-      <c r="M8" s="14"/>
-      <c r="N8" s="14"/>
-      <c r="O8" s="14"/>
-      <c r="P8" s="14"/>
-      <c r="Q8" s="14"/>
-      <c r="R8" s="14"/>
-      <c r="S8" s="14"/>
-      <c r="T8" s="14"/>
-      <c r="U8" s="14"/>
-      <c r="V8" s="14"/>
-      <c r="W8" s="14"/>
-      <c r="X8" s="14"/>
-      <c r="Y8" s="14"/>
-      <c r="Z8" s="14"/>
-      <c r="AA8" s="14"/>
-    </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="12"/>
+      <c r="L8" s="12"/>
+      <c r="M8" s="12"/>
+      <c r="N8" s="12"/>
+      <c r="O8" s="12"/>
+      <c r="P8" s="12"/>
+      <c r="Q8" s="12"/>
+      <c r="R8" s="12"/>
+      <c r="S8" s="12"/>
+      <c r="T8" s="12"/>
+      <c r="U8" s="12"/>
+      <c r="V8" s="12"/>
+      <c r="W8" s="12"/>
+      <c r="X8" s="12"/>
+      <c r="Y8" s="12"/>
+      <c r="Z8" s="12"/>
+      <c r="AA8" s="12"/>
+      <c r="AB8" s="20"/>
+    </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -1394,7 +1523,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -1477,7 +1606,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -1560,7 +1689,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>26</v>
       </c>
@@ -1643,7 +1772,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>23</v>
       </c>
@@ -1726,7 +1855,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>29</v>
       </c>
@@ -1809,7 +1938,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>31</v>
       </c>
@@ -2472,6 +2601,9 @@
       <c r="AA23" s="3">
         <v>0</v>
       </c>
+      <c r="AB23" s="19" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="24" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
@@ -2555,9 +2687,6 @@
       <c r="AA24" s="3">
         <v>0</v>
       </c>
-      <c r="AB24" t="s">
-        <v>49</v>
-      </c>
     </row>
     <row r="25" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
@@ -2727,7 +2856,7 @@
     </row>
     <row r="27" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="9" t="s">
-        <v>87</v>
+        <v>108</v>
       </c>
       <c r="B27" s="10"/>
       <c r="C27" s="10"/>
@@ -2755,82 +2884,42 @@
       <c r="Y27" s="10"/>
       <c r="Z27" s="10"/>
       <c r="AA27" s="10"/>
+      <c r="AB27" s="20"/>
     </row>
     <row r="28" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B28" s="6" t="s">
         <v>46</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="D28" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="E28" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F28" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="G28" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="H28" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="I28" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="J28" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="K28" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="L28" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="M28" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="N28" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="O28" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="P28" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q28" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="R28" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="S28" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="T28" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="U28" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="V28" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="W28" s="8" t="s">
-        <v>16</v>
-      </c>
+        <v>110</v>
+      </c>
+      <c r="E28" s="8"/>
+      <c r="F28" s="8"/>
+      <c r="G28" s="8"/>
+      <c r="H28" s="7"/>
+      <c r="I28" s="7"/>
+      <c r="J28" s="7"/>
+      <c r="K28" s="8"/>
+      <c r="L28" s="8"/>
+      <c r="M28" s="7"/>
+      <c r="N28" s="7"/>
+      <c r="O28" s="8"/>
+      <c r="P28" s="8"/>
+      <c r="Q28" s="8"/>
+      <c r="R28" s="8"/>
+      <c r="S28" s="7"/>
+      <c r="T28" s="7"/>
+      <c r="U28" s="8"/>
+      <c r="V28" s="7"/>
+      <c r="W28" s="8"/>
       <c r="X28" s="7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="Y28" s="7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="Z28" s="7" t="s">
         <v>16</v>
@@ -2841,74 +2930,33 @@
     </row>
     <row r="29" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
+        <v>57</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C29" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="B29" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="C29" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="D29" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="E29" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F29" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="G29" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="H29" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="I29" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="J29" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="K29" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="L29" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="M29" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="N29" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="O29" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="P29" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q29" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="R29" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="S29" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="T29" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="U29" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="V29" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="W29" s="8" t="s">
-        <v>16</v>
-      </c>
+      <c r="E29" s="8"/>
+      <c r="F29" s="8"/>
+      <c r="G29" s="8"/>
+      <c r="H29" s="7"/>
+      <c r="I29" s="7"/>
+      <c r="J29" s="7"/>
+      <c r="K29" s="8"/>
+      <c r="L29" s="8"/>
+      <c r="M29" s="7"/>
+      <c r="N29" s="7"/>
+      <c r="O29" s="8"/>
+      <c r="P29" s="8"/>
+      <c r="Q29" s="8"/>
+      <c r="R29" s="8"/>
+      <c r="S29" s="7"/>
+      <c r="T29" s="7"/>
+      <c r="U29" s="8"/>
+      <c r="V29" s="7"/>
+      <c r="W29" s="8"/>
       <c r="X29" s="7" t="s">
         <v>16</v>
       </c>
@@ -2927,71 +2975,30 @@
         <v>22</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="D30" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="E30" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F30" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="G30" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="H30" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="I30" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="J30" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="K30" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="L30" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="M30" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="N30" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="O30" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="P30" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q30" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="R30" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="S30" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="T30" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="U30" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="V30" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="W30" s="8" t="s">
-        <v>16</v>
-      </c>
+        <v>78</v>
+      </c>
+      <c r="E30" s="8"/>
+      <c r="F30" s="8"/>
+      <c r="G30" s="8"/>
+      <c r="H30" s="7"/>
+      <c r="I30" s="7"/>
+      <c r="J30" s="7"/>
+      <c r="K30" s="8"/>
+      <c r="L30" s="8"/>
+      <c r="M30" s="7"/>
+      <c r="N30" s="7"/>
+      <c r="O30" s="8"/>
+      <c r="P30" s="8"/>
+      <c r="Q30" s="8"/>
+      <c r="R30" s="8"/>
+      <c r="S30" s="7"/>
+      <c r="T30" s="7"/>
+      <c r="U30" s="8"/>
+      <c r="V30" s="7"/>
+      <c r="W30" s="8"/>
       <c r="X30" s="7" t="s">
         <v>16</v>
       </c>
@@ -3007,74 +3014,33 @@
     </row>
     <row r="31" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B31" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C31" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="C31" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="D31" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="E31" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F31" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="G31" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="H31" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="I31" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="J31" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="K31" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="L31" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="M31" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="N31" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="O31" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="P31" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q31" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="R31" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="S31" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="T31" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="U31" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="V31" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="W31" s="8" t="s">
-        <v>16</v>
-      </c>
+      <c r="E31" s="8"/>
+      <c r="F31" s="8"/>
+      <c r="G31" s="8"/>
+      <c r="H31" s="7"/>
+      <c r="I31" s="7"/>
+      <c r="J31" s="7"/>
+      <c r="K31" s="8"/>
+      <c r="L31" s="8"/>
+      <c r="M31" s="7"/>
+      <c r="N31" s="7"/>
+      <c r="O31" s="8"/>
+      <c r="P31" s="8"/>
+      <c r="Q31" s="8"/>
+      <c r="R31" s="8"/>
+      <c r="S31" s="7"/>
+      <c r="T31" s="7"/>
+      <c r="U31" s="8"/>
+      <c r="V31" s="7"/>
+      <c r="W31" s="8"/>
       <c r="X31" s="7" t="s">
         <v>16</v>
       </c>
@@ -3090,82 +3056,41 @@
     </row>
     <row r="32" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="D32" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="E32" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F32" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="G32" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="H32" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="I32" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="J32" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="K32" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="L32" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="M32" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="N32" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="O32" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="P32" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q32" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="R32" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="S32" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="T32" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="U32" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="V32" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="W32" s="8" t="s">
-        <v>16</v>
-      </c>
+        <v>77</v>
+      </c>
+      <c r="E32" s="8"/>
+      <c r="F32" s="8"/>
+      <c r="G32" s="8"/>
+      <c r="H32" s="7"/>
+      <c r="I32" s="7"/>
+      <c r="J32" s="7"/>
+      <c r="K32" s="8"/>
+      <c r="L32" s="8"/>
+      <c r="M32" s="7"/>
+      <c r="N32" s="7"/>
+      <c r="O32" s="8"/>
+      <c r="P32" s="8"/>
+      <c r="Q32" s="8"/>
+      <c r="R32" s="8"/>
+      <c r="S32" s="7"/>
+      <c r="T32" s="7"/>
+      <c r="U32" s="8"/>
+      <c r="V32" s="7"/>
+      <c r="W32" s="8"/>
       <c r="X32" s="7" t="s">
         <v>16</v>
       </c>
       <c r="Y32" s="7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="Z32" s="7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="AA32" s="8" t="s">
         <v>16</v>
@@ -3173,74 +3098,33 @@
     </row>
     <row r="33" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B33" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C33" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="C33" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="D33" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="E33" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F33" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="G33" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="H33" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="I33" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="J33" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="K33" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="L33" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="M33" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="N33" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="O33" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="P33" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q33" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="R33" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="S33" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="T33" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="U33" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="V33" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="W33" s="8" t="s">
-        <v>16</v>
-      </c>
+      <c r="E33" s="8"/>
+      <c r="F33" s="8"/>
+      <c r="G33" s="8"/>
+      <c r="H33" s="7"/>
+      <c r="I33" s="7"/>
+      <c r="J33" s="7"/>
+      <c r="K33" s="8"/>
+      <c r="L33" s="8"/>
+      <c r="M33" s="7"/>
+      <c r="N33" s="7"/>
+      <c r="O33" s="8"/>
+      <c r="P33" s="8"/>
+      <c r="Q33" s="8"/>
+      <c r="R33" s="8"/>
+      <c r="S33" s="7"/>
+      <c r="T33" s="7"/>
+      <c r="U33" s="8"/>
+      <c r="V33" s="7"/>
+      <c r="W33" s="8"/>
       <c r="X33" s="7" t="s">
         <v>16</v>
       </c>
@@ -3256,74 +3140,33 @@
     </row>
     <row r="34" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B34" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C34" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="C34" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="D34" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="E34" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F34" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="G34" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="H34" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="I34" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="J34" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="K34" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="L34" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="M34" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="N34" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="O34" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="P34" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q34" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="R34" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="S34" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="T34" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="U34" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="V34" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="W34" s="8" t="s">
-        <v>16</v>
-      </c>
+      <c r="E34" s="8"/>
+      <c r="F34" s="8"/>
+      <c r="G34" s="8"/>
+      <c r="H34" s="7"/>
+      <c r="I34" s="7"/>
+      <c r="J34" s="7"/>
+      <c r="K34" s="8"/>
+      <c r="L34" s="8"/>
+      <c r="M34" s="7"/>
+      <c r="N34" s="7"/>
+      <c r="O34" s="8"/>
+      <c r="P34" s="8"/>
+      <c r="Q34" s="8"/>
+      <c r="R34" s="8"/>
+      <c r="S34" s="7"/>
+      <c r="T34" s="7"/>
+      <c r="U34" s="8"/>
+      <c r="V34" s="7"/>
+      <c r="W34" s="8"/>
       <c r="X34" s="7" t="s">
         <v>16</v>
       </c>
@@ -3342,79 +3185,38 @@
         <v>22</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="D35" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="E35" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F35" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="G35" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="H35" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="I35" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="J35" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="K35" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="L35" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="M35" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="N35" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="O35" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="P35" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q35" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="R35" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="S35" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="T35" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="U35" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="V35" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="W35" s="8" t="s">
-        <v>16</v>
-      </c>
+        <v>77</v>
+      </c>
+      <c r="E35" s="8"/>
+      <c r="F35" s="8"/>
+      <c r="G35" s="8"/>
+      <c r="H35" s="7"/>
+      <c r="I35" s="7"/>
+      <c r="J35" s="7"/>
+      <c r="K35" s="8"/>
+      <c r="L35" s="8"/>
+      <c r="M35" s="7"/>
+      <c r="N35" s="7"/>
+      <c r="O35" s="8"/>
+      <c r="P35" s="8"/>
+      <c r="Q35" s="8"/>
+      <c r="R35" s="8"/>
+      <c r="S35" s="7"/>
+      <c r="T35" s="7"/>
+      <c r="U35" s="8"/>
+      <c r="V35" s="7"/>
+      <c r="W35" s="8"/>
       <c r="X35" s="7" t="s">
         <v>16</v>
       </c>
       <c r="Y35" s="7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="Z35" s="7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="AA35" s="8" t="s">
         <v>16</v>
@@ -3425,71 +3227,30 @@
         <v>36</v>
       </c>
       <c r="B36" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C36" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="C36" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="D36" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="E36" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F36" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="G36" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="H36" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="I36" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="J36" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="K36" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="L36" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="M36" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="N36" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="O36" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="P36" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q36" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="R36" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="S36" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="T36" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="U36" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="V36" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="W36" s="8" t="s">
-        <v>16</v>
-      </c>
+      <c r="E36" s="8"/>
+      <c r="F36" s="8"/>
+      <c r="G36" s="8"/>
+      <c r="H36" s="7"/>
+      <c r="I36" s="7"/>
+      <c r="J36" s="7"/>
+      <c r="K36" s="8"/>
+      <c r="L36" s="8"/>
+      <c r="M36" s="7"/>
+      <c r="N36" s="7"/>
+      <c r="O36" s="8"/>
+      <c r="P36" s="8"/>
+      <c r="Q36" s="8"/>
+      <c r="R36" s="8"/>
+      <c r="S36" s="7"/>
+      <c r="T36" s="7"/>
+      <c r="U36" s="8"/>
+      <c r="V36" s="7"/>
+      <c r="W36" s="8"/>
       <c r="X36" s="7" t="s">
         <v>16</v>
       </c>
@@ -3508,71 +3269,30 @@
         <v>35</v>
       </c>
       <c r="B37" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C37" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="C37" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="D37" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="E37" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F37" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="G37" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="H37" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="I37" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="J37" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="K37" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="L37" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="M37" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="N37" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="O37" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="P37" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q37" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="R37" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="S37" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="T37" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="U37" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="V37" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="W37" s="8" t="s">
-        <v>16</v>
-      </c>
+      <c r="E37" s="8"/>
+      <c r="F37" s="8"/>
+      <c r="G37" s="8"/>
+      <c r="H37" s="7"/>
+      <c r="I37" s="7"/>
+      <c r="J37" s="7"/>
+      <c r="K37" s="8"/>
+      <c r="L37" s="8"/>
+      <c r="M37" s="7"/>
+      <c r="N37" s="7"/>
+      <c r="O37" s="8"/>
+      <c r="P37" s="8"/>
+      <c r="Q37" s="8"/>
+      <c r="R37" s="8"/>
+      <c r="S37" s="7"/>
+      <c r="T37" s="7"/>
+      <c r="U37" s="8"/>
+      <c r="V37" s="7"/>
+      <c r="W37" s="8"/>
       <c r="X37" s="7" t="s">
         <v>16</v>
       </c>
@@ -3591,71 +3311,30 @@
         <v>38</v>
       </c>
       <c r="B38" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C38" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="C38" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="D38" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="E38" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F38" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="G38" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="H38" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="I38" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="J38" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="K38" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="L38" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="M38" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="N38" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="O38" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="P38" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q38" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="R38" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="S38" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="T38" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="U38" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="V38" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="W38" s="8" t="s">
-        <v>16</v>
-      </c>
+      <c r="E38" s="8"/>
+      <c r="F38" s="8"/>
+      <c r="G38" s="8"/>
+      <c r="H38" s="7"/>
+      <c r="I38" s="7"/>
+      <c r="J38" s="7"/>
+      <c r="K38" s="8"/>
+      <c r="L38" s="8"/>
+      <c r="M38" s="7"/>
+      <c r="N38" s="7"/>
+      <c r="O38" s="8"/>
+      <c r="P38" s="8"/>
+      <c r="Q38" s="8"/>
+      <c r="R38" s="8"/>
+      <c r="S38" s="7"/>
+      <c r="T38" s="7"/>
+      <c r="U38" s="8"/>
+      <c r="V38" s="7"/>
+      <c r="W38" s="8"/>
       <c r="X38" s="7" t="s">
         <v>16</v>
       </c>
@@ -3671,74 +3350,33 @@
     </row>
     <row r="39" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B39" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="C39" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="C39" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="D39" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="E39" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F39" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="G39" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="H39" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="I39" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="J39" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="K39" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="L39" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="M39" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="N39" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="O39" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="P39" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q39" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="R39" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="S39" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="T39" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="U39" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="V39" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="W39" s="8" t="s">
-        <v>16</v>
-      </c>
+      <c r="E39" s="8"/>
+      <c r="F39" s="8"/>
+      <c r="G39" s="8"/>
+      <c r="H39" s="7"/>
+      <c r="I39" s="7"/>
+      <c r="J39" s="7"/>
+      <c r="K39" s="8"/>
+      <c r="L39" s="8"/>
+      <c r="M39" s="7"/>
+      <c r="N39" s="7"/>
+      <c r="O39" s="8"/>
+      <c r="P39" s="8"/>
+      <c r="Q39" s="8"/>
+      <c r="R39" s="8"/>
+      <c r="S39" s="7"/>
+      <c r="T39" s="7"/>
+      <c r="U39" s="8"/>
+      <c r="V39" s="7"/>
+      <c r="W39" s="8"/>
       <c r="X39" s="7" t="s">
         <v>16</v>
       </c>
@@ -3757,71 +3395,30 @@
         <v>42</v>
       </c>
       <c r="B40" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="C40" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="C40" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="D40" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="E40" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F40" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="G40" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="H40" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="I40" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="J40" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="K40" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="L40" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="M40" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="N40" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="O40" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="P40" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q40" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="R40" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="S40" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="T40" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="U40" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="V40" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="W40" s="8" t="s">
-        <v>16</v>
-      </c>
+      <c r="E40" s="8"/>
+      <c r="F40" s="8"/>
+      <c r="G40" s="8"/>
+      <c r="H40" s="7"/>
+      <c r="I40" s="7"/>
+      <c r="J40" s="7"/>
+      <c r="K40" s="8"/>
+      <c r="L40" s="8"/>
+      <c r="M40" s="7"/>
+      <c r="N40" s="7"/>
+      <c r="O40" s="8"/>
+      <c r="P40" s="8"/>
+      <c r="Q40" s="8"/>
+      <c r="R40" s="8"/>
+      <c r="S40" s="7"/>
+      <c r="T40" s="7"/>
+      <c r="U40" s="8"/>
+      <c r="V40" s="7"/>
+      <c r="W40" s="8"/>
       <c r="X40" s="7" t="s">
         <v>16</v>
       </c>
@@ -3840,82 +3437,44 @@
         <v>22</v>
       </c>
       <c r="B41" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C41" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="C41" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="D41" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="E41" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F41" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="G41" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="H41" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="I41" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="J41" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="K41" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="L41" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="M41" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="N41" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="O41" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="P41" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q41" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="R41" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="S41" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="T41" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="U41" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="V41" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="W41" s="8" t="s">
-        <v>16</v>
-      </c>
+      <c r="E41" s="8"/>
+      <c r="F41" s="8"/>
+      <c r="G41" s="8"/>
+      <c r="H41" s="7"/>
+      <c r="I41" s="7"/>
+      <c r="J41" s="7"/>
+      <c r="K41" s="8"/>
+      <c r="L41" s="8"/>
+      <c r="M41" s="7"/>
+      <c r="N41" s="7"/>
+      <c r="O41" s="8"/>
+      <c r="P41" s="8"/>
+      <c r="Q41" s="8"/>
+      <c r="R41" s="8"/>
+      <c r="S41" s="7"/>
+      <c r="T41" s="7"/>
+      <c r="U41" s="8"/>
+      <c r="V41" s="7"/>
+      <c r="W41" s="8"/>
       <c r="X41" s="7" t="s">
         <v>16</v>
       </c>
       <c r="Y41" s="7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="Z41" s="7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="AA41" s="8" t="s">
         <v>16</v>
+      </c>
+      <c r="AB41" s="19" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="42" spans="1:28" x14ac:dyDescent="0.3">
@@ -3923,71 +3482,30 @@
         <v>45</v>
       </c>
       <c r="B42" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="C42" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="C42" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="D42" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="E42" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F42" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="G42" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="H42" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="I42" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="J42" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="K42" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="L42" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="M42" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="N42" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="O42" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="P42" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q42" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="R42" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="S42" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="T42" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="U42" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="V42" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="W42" s="8" t="s">
-        <v>16</v>
-      </c>
+      <c r="E42" s="8"/>
+      <c r="F42" s="8"/>
+      <c r="G42" s="8"/>
+      <c r="H42" s="7"/>
+      <c r="I42" s="7"/>
+      <c r="J42" s="7"/>
+      <c r="K42" s="8"/>
+      <c r="L42" s="8"/>
+      <c r="M42" s="7"/>
+      <c r="N42" s="7"/>
+      <c r="O42" s="8"/>
+      <c r="P42" s="8"/>
+      <c r="Q42" s="8"/>
+      <c r="R42" s="8"/>
+      <c r="S42" s="7"/>
+      <c r="T42" s="7"/>
+      <c r="U42" s="8"/>
+      <c r="V42" s="7"/>
+      <c r="W42" s="8"/>
       <c r="X42" s="7" t="s">
         <v>16</v>
       </c>
@@ -3999,9 +3517,6 @@
       </c>
       <c r="AA42" s="8" t="s">
         <v>16</v>
-      </c>
-      <c r="AB42" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="43" spans="1:28" x14ac:dyDescent="0.3">
@@ -4009,71 +3524,30 @@
         <v>22</v>
       </c>
       <c r="B43" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="C43" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="C43" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="D43" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="E43" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F43" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="G43" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="H43" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="I43" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="J43" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="K43" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="L43" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="M43" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="N43" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="O43" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="P43" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q43" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="R43" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="S43" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="T43" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="U43" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="V43" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="W43" s="8" t="s">
-        <v>16</v>
-      </c>
+      <c r="E43" s="8"/>
+      <c r="F43" s="8"/>
+      <c r="G43" s="8"/>
+      <c r="H43" s="7"/>
+      <c r="I43" s="7"/>
+      <c r="J43" s="7"/>
+      <c r="K43" s="8"/>
+      <c r="L43" s="8"/>
+      <c r="M43" s="7"/>
+      <c r="N43" s="7"/>
+      <c r="O43" s="8"/>
+      <c r="P43" s="8"/>
+      <c r="Q43" s="8"/>
+      <c r="R43" s="8"/>
+      <c r="S43" s="7"/>
+      <c r="T43" s="7"/>
+      <c r="U43" s="8"/>
+      <c r="V43" s="7"/>
+      <c r="W43" s="8"/>
       <c r="X43" s="7" t="s">
         <v>16</v>
       </c>
@@ -4089,127 +3563,90 @@
     </row>
     <row r="44" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="D44" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="E44" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F44" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="G44" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="H44" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="I44" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="J44" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="K44" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="L44" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="M44" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="N44" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="O44" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="P44" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q44" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="R44" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="S44" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="T44" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="U44" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="V44" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="W44" s="8" t="s">
-        <v>16</v>
-      </c>
+        <v>110</v>
+      </c>
+      <c r="E44" s="8"/>
+      <c r="F44" s="8"/>
+      <c r="G44" s="8"/>
+      <c r="H44" s="7"/>
+      <c r="I44" s="7"/>
+      <c r="J44" s="7"/>
+      <c r="K44" s="8"/>
+      <c r="L44" s="8"/>
+      <c r="M44" s="7"/>
+      <c r="N44" s="7"/>
+      <c r="O44" s="8"/>
+      <c r="P44" s="8"/>
+      <c r="Q44" s="8"/>
+      <c r="R44" s="8"/>
+      <c r="S44" s="7"/>
+      <c r="T44" s="7"/>
+      <c r="U44" s="8"/>
+      <c r="V44" s="7"/>
+      <c r="W44" s="8"/>
       <c r="X44" s="7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="Y44" s="7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="Z44" s="7" t="s">
         <v>16</v>
       </c>
       <c r="AA44" s="8" t="s">
-        <v>16</v>
+        <v>122</v>
+      </c>
+      <c r="AB44" s="19" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="45" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A45" s="9" t="s">
-        <v>86</v>
+        <v>105</v>
       </c>
       <c r="B45" s="10"/>
       <c r="C45" s="10"/>
       <c r="D45" s="10"/>
-      <c r="E45" s="14"/>
-      <c r="F45" s="14"/>
-      <c r="G45" s="14"/>
-      <c r="H45" s="14"/>
-      <c r="I45" s="14"/>
-      <c r="J45" s="14"/>
-      <c r="K45" s="14"/>
-      <c r="L45" s="14"/>
-      <c r="M45" s="14"/>
-      <c r="N45" s="14"/>
-      <c r="O45" s="14"/>
-      <c r="P45" s="14"/>
-      <c r="Q45" s="14"/>
-      <c r="R45" s="14"/>
-      <c r="S45" s="14"/>
-      <c r="T45" s="14"/>
-      <c r="U45" s="14"/>
-      <c r="V45" s="14"/>
-      <c r="W45" s="14"/>
-      <c r="X45" s="14"/>
-      <c r="Y45" s="14"/>
-      <c r="Z45" s="14"/>
-      <c r="AA45" s="14"/>
+      <c r="E45" s="12"/>
+      <c r="F45" s="12"/>
+      <c r="G45" s="12"/>
+      <c r="H45" s="12"/>
+      <c r="I45" s="12"/>
+      <c r="J45" s="12"/>
+      <c r="K45" s="12"/>
+      <c r="L45" s="12"/>
+      <c r="M45" s="12"/>
+      <c r="N45" s="12"/>
+      <c r="O45" s="12"/>
+      <c r="P45" s="12"/>
+      <c r="Q45" s="12"/>
+      <c r="R45" s="12"/>
+      <c r="S45" s="12"/>
+      <c r="T45" s="12"/>
+      <c r="U45" s="12"/>
+      <c r="V45" s="12"/>
+      <c r="W45" s="12"/>
+      <c r="X45" s="12"/>
+      <c r="Y45" s="12"/>
+      <c r="Z45" s="12"/>
+      <c r="AA45" s="12"/>
+      <c r="AB45" s="20"/>
     </row>
     <row r="46" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A46" s="13" t="s">
-        <v>82</v>
+      <c r="A46" s="11" t="s">
+        <v>80</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>81</v>
+        <v>109</v>
       </c>
       <c r="X46" s="2">
         <v>1</v>
@@ -4222,19 +3659,19 @@
       </c>
     </row>
     <row r="47" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A47" s="15" t="s">
-        <v>92</v>
+      <c r="A47" s="13" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="48" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A48" s="15" t="s">
-        <v>90</v>
+      <c r="A48" s="13" t="s">
+        <v>83</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>81</v>
+        <v>109</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="X48" s="2">
         <v>1</v>
@@ -4247,8 +3684,8 @@
       </c>
     </row>
     <row r="49" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A49" s="13" t="s">
-        <v>93</v>
+      <c r="A49" s="11" t="s">
+        <v>86</v>
       </c>
       <c r="E49" s="4"/>
       <c r="F49" s="4"/>
@@ -4275,14 +3712,14 @@
       <c r="AA49" s="4"/>
     </row>
     <row r="50" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A50" s="13" t="s">
-        <v>91</v>
+      <c r="A50" s="11" t="s">
+        <v>84</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>83</v>
+        <v>113</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="X50" s="2">
         <v>1</v>
@@ -4295,8 +3732,8 @@
       </c>
     </row>
     <row r="51" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A51" s="15" t="s">
-        <v>94</v>
+      <c r="A51" s="13" t="s">
+        <v>87</v>
       </c>
       <c r="E51" s="4"/>
       <c r="F51" s="4"/>
@@ -4323,14 +3760,14 @@
       <c r="AA51" s="4"/>
     </row>
     <row r="52" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A52" s="15" t="s">
-        <v>97</v>
+      <c r="A52" s="13" t="s">
+        <v>90</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>85</v>
+        <v>112</v>
       </c>
       <c r="C52" s="7" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="X52" s="2">
         <v>1</v>
@@ -4343,8 +3780,8 @@
       </c>
     </row>
     <row r="53" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A53" s="13" t="s">
-        <v>95</v>
+      <c r="A53" s="11" t="s">
+        <v>88</v>
       </c>
       <c r="E53" s="4"/>
       <c r="F53" s="4"/>
@@ -4371,136 +3808,136 @@
       <c r="AA53" s="4"/>
     </row>
     <row r="54" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A54" s="13" t="s">
-        <v>106</v>
+      <c r="A54" s="11" t="s">
+        <v>94</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>84</v>
+        <v>114</v>
       </c>
       <c r="C54" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="X54" s="2">
+        <v>1</v>
+      </c>
+      <c r="Y54" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z54" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A55" s="13" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="56" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A56" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="B56" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="X54" s="2">
-        <v>1</v>
-      </c>
-      <c r="Y54" s="2">
-        <v>0</v>
-      </c>
-      <c r="Z54" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A55" s="15" t="s">
+      <c r="C56" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="X56" s="2">
+        <v>1</v>
+      </c>
+      <c r="Y56" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z56" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A57" s="11" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="58" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A58" s="11" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="56" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A56" s="15" t="s">
-        <v>107</v>
-      </c>
-      <c r="B56" s="6" t="s">
+      <c r="B58" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="C58" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="X58" s="2">
+        <v>1</v>
+      </c>
+      <c r="Y58" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z58" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A59" s="13" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="60" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A60" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="B60" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="C60" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="X60" s="2">
+        <v>1</v>
+      </c>
+      <c r="Y60" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z60" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A61" s="11" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="62" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A62" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="C56" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="X56" s="2">
-        <v>1</v>
-      </c>
-      <c r="Y56" s="2">
-        <v>0</v>
-      </c>
-      <c r="Z56" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A57" s="13" t="s">
+      <c r="B62" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="C62" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="X62" s="2">
+        <v>1</v>
+      </c>
+      <c r="Y62" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z62" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A63" s="13" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="58" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A58" s="13" t="s">
-        <v>108</v>
-      </c>
-      <c r="B58" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="C58" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="X58" s="2">
-        <v>1</v>
-      </c>
-      <c r="Y58" s="2">
-        <v>0</v>
-      </c>
-      <c r="Z58" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A59" s="15" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="60" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A60" s="15" t="s">
-        <v>109</v>
-      </c>
-      <c r="B60" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="C60" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="X60" s="2">
-        <v>1</v>
-      </c>
-      <c r="Y60" s="2">
-        <v>0</v>
-      </c>
-      <c r="Z60" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A61" s="13" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="62" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A62" s="13" t="s">
-        <v>110</v>
-      </c>
-      <c r="B62" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="C62" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="X62" s="2">
-        <v>1</v>
-      </c>
-      <c r="Y62" s="2">
-        <v>0</v>
-      </c>
-      <c r="Z62" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A63" s="15" t="s">
-        <v>111</v>
-      </c>
-    </row>
     <row r="64" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A64" s="15" t="s">
-        <v>106</v>
+      <c r="A64" s="13" t="s">
+        <v>94</v>
       </c>
       <c r="B64" s="6" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
       <c r="C64" s="5">
         <v>0</v>
@@ -4533,74 +3970,347 @@
     </row>
     <row r="65" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A65" s="9" t="s">
-        <v>113</v>
+        <v>154</v>
       </c>
       <c r="B65" s="10"/>
       <c r="C65" s="10"/>
       <c r="D65" s="10"/>
-      <c r="E65" s="14"/>
-      <c r="F65" s="14"/>
-      <c r="G65" s="14"/>
-      <c r="H65" s="14"/>
-      <c r="I65" s="14"/>
-      <c r="J65" s="14"/>
-      <c r="K65" s="14"/>
-      <c r="L65" s="14"/>
-      <c r="M65" s="14"/>
-      <c r="N65" s="14"/>
-      <c r="O65" s="14"/>
-      <c r="P65" s="14"/>
-      <c r="Q65" s="14"/>
-      <c r="R65" s="14"/>
-      <c r="S65" s="14"/>
-      <c r="T65" s="14"/>
-      <c r="U65" s="14"/>
-      <c r="V65" s="14"/>
-      <c r="W65" s="14"/>
-      <c r="X65" s="14"/>
-      <c r="Y65" s="14"/>
-      <c r="Z65" s="14"/>
-      <c r="AA65" s="14"/>
+      <c r="E65" s="12"/>
+      <c r="F65" s="12"/>
+      <c r="G65" s="12"/>
+      <c r="H65" s="12"/>
+      <c r="I65" s="12"/>
+      <c r="J65" s="12"/>
+      <c r="K65" s="12"/>
+      <c r="L65" s="12"/>
+      <c r="M65" s="12"/>
+      <c r="N65" s="12"/>
+      <c r="O65" s="12"/>
+      <c r="P65" s="12"/>
+      <c r="Q65" s="12"/>
+      <c r="R65" s="12"/>
+      <c r="S65" s="12"/>
+      <c r="T65" s="12"/>
+      <c r="U65" s="12"/>
+      <c r="V65" s="12"/>
+      <c r="W65" s="12"/>
+      <c r="X65" s="12"/>
+      <c r="Y65" s="12"/>
+      <c r="Z65" s="12"/>
+      <c r="AA65" s="12"/>
+      <c r="AB65" s="20"/>
     </row>
     <row r="66" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A66" t="s">
-        <v>116</v>
-      </c>
       <c r="B66" s="6" t="s">
-        <v>115</v>
+        <v>124</v>
       </c>
       <c r="C66" s="7" t="s">
-        <v>118</v>
+        <v>125</v>
+      </c>
+      <c r="X66" s="2">
+        <v>1</v>
+      </c>
+      <c r="Y66" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z66" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="67" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A67" t="s">
-        <v>117</v>
-      </c>
-      <c r="B67" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="C67" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="AA67" s="3">
-        <v>1</v>
-      </c>
-      <c r="AB67" t="s">
+      <c r="A67" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="E67" s="14"/>
+      <c r="F67" s="14"/>
+      <c r="G67" s="14"/>
+      <c r="H67" s="15"/>
+      <c r="I67" s="15"/>
+      <c r="J67" s="15"/>
+      <c r="K67" s="14"/>
+      <c r="L67" s="14"/>
+      <c r="M67" s="15"/>
+      <c r="N67" s="15"/>
+      <c r="O67" s="14"/>
+      <c r="P67" s="14"/>
+      <c r="Q67" s="14"/>
+      <c r="R67" s="14"/>
+      <c r="S67" s="15"/>
+      <c r="T67" s="15"/>
+      <c r="U67" s="14"/>
+      <c r="V67" s="15"/>
+      <c r="W67" s="14"/>
+      <c r="X67" s="15"/>
+      <c r="Y67" s="15"/>
+      <c r="Z67" s="15"/>
+      <c r="AA67" s="14"/>
+    </row>
+    <row r="68" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A68" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="B68" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="C68" s="7" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="69" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A69" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="E69" s="14"/>
+      <c r="F69" s="14"/>
+      <c r="G69" s="14"/>
+      <c r="H69" s="15"/>
+      <c r="I69" s="15"/>
+      <c r="J69" s="15"/>
+      <c r="K69" s="14"/>
+      <c r="L69" s="14"/>
+      <c r="M69" s="15"/>
+      <c r="N69" s="15"/>
+      <c r="O69" s="14"/>
+      <c r="P69" s="14"/>
+      <c r="Q69" s="14"/>
+      <c r="R69" s="14"/>
+      <c r="S69" s="15"/>
+      <c r="T69" s="15"/>
+      <c r="U69" s="14"/>
+      <c r="V69" s="15"/>
+      <c r="W69" s="14"/>
+      <c r="X69" s="15"/>
+      <c r="Y69" s="15"/>
+      <c r="Z69" s="15"/>
+      <c r="AA69" s="14"/>
+    </row>
+    <row r="70" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A70" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="B70" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="C70" s="7" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="71" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A71" s="11" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="72" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A72" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="B72" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="C72" s="7" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="73" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A73" s="13" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="74" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A74" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="B74" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="C74" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="AB74" s="19" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="75" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A75" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="AB75" s="19" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="76" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A76" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="B76" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="C76" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="AB76" s="19" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="77" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A77" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="AB77" s="19" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="78" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A78" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="B78" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="C78" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="AB78" s="19" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="79" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A79" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="AB79" s="19" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="80" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A80" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="B80" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="C80" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="AB80" s="19" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="81" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A81" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="AB81" s="19" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="82" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A82" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="B82" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="C82" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="AB82" s="19" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="83" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A83" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="AB83" s="19" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="84" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A84" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="B84" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="C84" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="AB84" s="19" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="85" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A85" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="B85" s="10"/>
+      <c r="C85" s="10"/>
+      <c r="D85" s="10"/>
+      <c r="E85" s="12"/>
+      <c r="F85" s="12"/>
+      <c r="G85" s="12"/>
+      <c r="H85" s="12"/>
+      <c r="I85" s="12"/>
+      <c r="J85" s="12"/>
+      <c r="K85" s="12"/>
+      <c r="L85" s="12"/>
+      <c r="M85" s="12"/>
+      <c r="N85" s="12"/>
+      <c r="O85" s="12"/>
+      <c r="P85" s="12"/>
+      <c r="Q85" s="12"/>
+      <c r="R85" s="12"/>
+      <c r="S85" s="12"/>
+      <c r="T85" s="12"/>
+      <c r="U85" s="12"/>
+      <c r="V85" s="12"/>
+      <c r="W85" s="12"/>
+      <c r="X85" s="12"/>
+      <c r="Y85" s="12"/>
+      <c r="Z85" s="12"/>
+      <c r="AA85" s="12"/>
+      <c r="AB85" s="20"/>
+    </row>
+    <row r="86" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>101</v>
+      </c>
+      <c r="B86" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="C86" s="7" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="68" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A68" t="s">
-        <v>119</v>
-      </c>
-      <c r="B68" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="C68" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="AA68" s="3">
+    <row r="87" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>102</v>
+      </c>
+      <c r="B87" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="C87" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA87" s="3">
+        <v>1</v>
+      </c>
+      <c r="AB87" s="19" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="88" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>103</v>
+      </c>
+      <c r="B88" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="C88" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA88" s="3">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added control words for destination fetching and ALU operations for 2 operands
</commit_message>
<xml_diff>
--- a/Microroutines.xlsx
+++ b/Microroutines.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\college\arch\Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study\Third Year\arch\PDP11\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B3C5A8B-A60C-4C7B-9106-639657580226}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384"/>
+    <workbookView xWindow="13716" yWindow="3732" windowWidth="9324" windowHeight="8616" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="166">
   <si>
     <t>Micro instruction</t>
   </si>
@@ -527,8 +528,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -560,6 +561,12 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -609,7 +616,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
@@ -666,7 +673,22 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -952,12 +974,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AC99"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B99" sqref="B99"/>
+    <sheetView tabSelected="1" zoomScale="82" zoomScaleNormal="82" zoomScaleSheetLayoutView="86" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1002,35 +1024,35 @@
       <c r="C1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="22" t="s">
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="21" t="s">
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="L1" s="21"/>
-      <c r="M1" s="22" t="s">
+      <c r="L1" s="22"/>
+      <c r="M1" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="N1" s="22"/>
-      <c r="O1" s="21" t="s">
+      <c r="N1" s="23"/>
+      <c r="O1" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="P1" s="21"/>
-      <c r="Q1" s="21"/>
-      <c r="R1" s="21"/>
-      <c r="S1" s="22" t="s">
+      <c r="P1" s="22"/>
+      <c r="Q1" s="22"/>
+      <c r="R1" s="22"/>
+      <c r="S1" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="T1" s="22"/>
+      <c r="T1" s="23"/>
       <c r="U1" s="3" t="s">
         <v>2</v>
       </c>
@@ -1040,11 +1062,11 @@
       <c r="W1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="X1" s="22" t="s">
+      <c r="X1" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="Y1" s="22"/>
-      <c r="Z1" s="22"/>
+      <c r="Y1" s="23"/>
+      <c r="Z1" s="23"/>
       <c r="AA1" s="3" t="s">
         <v>5</v>
       </c>
@@ -1056,24 +1078,24 @@
       </c>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="22"/>
-      <c r="I2" s="22"/>
-      <c r="J2" s="22"/>
-      <c r="K2" s="21"/>
-      <c r="L2" s="21"/>
-      <c r="O2" s="21"/>
-      <c r="P2" s="21"/>
-      <c r="Q2" s="21"/>
-      <c r="R2" s="21"/>
-      <c r="S2" s="22"/>
-      <c r="T2" s="22"/>
-      <c r="X2" s="22"/>
-      <c r="Y2" s="22"/>
-      <c r="Z2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23"/>
+      <c r="K2" s="22"/>
+      <c r="L2" s="22"/>
+      <c r="O2" s="22"/>
+      <c r="P2" s="22"/>
+      <c r="Q2" s="22"/>
+      <c r="R2" s="22"/>
+      <c r="S2" s="23"/>
+      <c r="T2" s="23"/>
+      <c r="X2" s="23"/>
+      <c r="Y2" s="23"/>
+      <c r="Z2" s="23"/>
     </row>
     <row r="3" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
@@ -3002,25 +3024,38 @@
       <c r="C28" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="E28" s="8"/>
-      <c r="F28" s="8"/>
-      <c r="G28" s="8"/>
-      <c r="H28" s="7"/>
-      <c r="I28" s="7"/>
-      <c r="J28" s="7"/>
-      <c r="K28" s="8"/>
-      <c r="L28" s="8"/>
-      <c r="M28" s="7"/>
-      <c r="N28" s="7"/>
-      <c r="O28" s="8"/>
-      <c r="P28" s="8"/>
-      <c r="Q28" s="8"/>
-      <c r="R28" s="8"/>
-      <c r="S28" s="7"/>
-      <c r="T28" s="7"/>
-      <c r="U28" s="8"/>
-      <c r="V28" s="7"/>
-      <c r="W28" s="8"/>
+      <c r="D28" s="24">
+        <v>0</v>
+      </c>
+      <c r="E28" s="24">
+        <v>1</v>
+      </c>
+      <c r="F28" s="24">
+        <v>0</v>
+      </c>
+      <c r="G28" s="24">
+        <v>1</v>
+      </c>
+      <c r="H28" s="27"/>
+      <c r="I28" s="27"/>
+      <c r="J28" s="27"/>
+      <c r="K28" s="26"/>
+      <c r="L28" s="26"/>
+      <c r="M28" s="25">
+        <v>1</v>
+      </c>
+      <c r="N28" s="25">
+        <v>1</v>
+      </c>
+      <c r="O28" s="26"/>
+      <c r="P28" s="26"/>
+      <c r="Q28" s="26"/>
+      <c r="R28" s="26"/>
+      <c r="S28" s="27"/>
+      <c r="T28" s="27"/>
+      <c r="U28" s="26"/>
+      <c r="V28" s="27"/>
+      <c r="W28" s="26"/>
       <c r="X28" s="7" t="s">
         <v>17</v>
       </c>
@@ -3047,25 +3082,38 @@
       <c r="C29" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="E29" s="8"/>
-      <c r="F29" s="8"/>
-      <c r="G29" s="8"/>
-      <c r="H29" s="7"/>
-      <c r="I29" s="7"/>
-      <c r="J29" s="7"/>
-      <c r="K29" s="8"/>
-      <c r="L29" s="8"/>
-      <c r="M29" s="7"/>
-      <c r="N29" s="7"/>
-      <c r="O29" s="8"/>
-      <c r="P29" s="8"/>
-      <c r="Q29" s="8"/>
-      <c r="R29" s="8"/>
-      <c r="S29" s="7"/>
-      <c r="T29" s="7"/>
-      <c r="U29" s="8"/>
-      <c r="V29" s="7"/>
-      <c r="W29" s="8"/>
+      <c r="D29" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="E29" s="24">
+        <v>1</v>
+      </c>
+      <c r="F29" s="24">
+        <v>0</v>
+      </c>
+      <c r="G29" s="24">
+        <v>1</v>
+      </c>
+      <c r="H29" s="27"/>
+      <c r="I29" s="27"/>
+      <c r="J29" s="27"/>
+      <c r="K29" s="24">
+        <v>0</v>
+      </c>
+      <c r="L29" s="24">
+        <v>1</v>
+      </c>
+      <c r="M29" s="27"/>
+      <c r="N29" s="27"/>
+      <c r="O29" s="26"/>
+      <c r="P29" s="26"/>
+      <c r="Q29" s="26"/>
+      <c r="R29" s="26"/>
+      <c r="S29" s="27"/>
+      <c r="T29" s="27"/>
+      <c r="U29" s="26"/>
+      <c r="V29" s="27"/>
+      <c r="W29" s="26"/>
       <c r="X29" s="7" t="s">
         <v>16</v>
       </c>
@@ -3092,25 +3140,34 @@
       <c r="C30" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="E30" s="8"/>
-      <c r="F30" s="8"/>
-      <c r="G30" s="8"/>
-      <c r="H30" s="7"/>
-      <c r="I30" s="7"/>
-      <c r="J30" s="7"/>
-      <c r="K30" s="8"/>
-      <c r="L30" s="8"/>
-      <c r="M30" s="7"/>
-      <c r="N30" s="7"/>
-      <c r="O30" s="8"/>
-      <c r="P30" s="8"/>
-      <c r="Q30" s="8"/>
-      <c r="R30" s="8"/>
-      <c r="S30" s="7"/>
-      <c r="T30" s="7"/>
-      <c r="U30" s="8"/>
-      <c r="V30" s="7"/>
-      <c r="W30" s="8"/>
+      <c r="D30" s="26"/>
+      <c r="E30" s="26"/>
+      <c r="F30" s="26"/>
+      <c r="G30" s="26"/>
+      <c r="H30" s="27"/>
+      <c r="I30" s="27"/>
+      <c r="J30" s="27"/>
+      <c r="K30" s="24">
+        <v>1</v>
+      </c>
+      <c r="L30" s="24">
+        <v>0</v>
+      </c>
+      <c r="M30" s="27"/>
+      <c r="N30" s="27"/>
+      <c r="O30" s="26"/>
+      <c r="P30" s="26"/>
+      <c r="Q30" s="26"/>
+      <c r="R30" s="26"/>
+      <c r="S30" s="25">
+        <v>0</v>
+      </c>
+      <c r="T30" s="25">
+        <v>1</v>
+      </c>
+      <c r="U30" s="26"/>
+      <c r="V30" s="27"/>
+      <c r="W30" s="26"/>
       <c r="X30" s="7" t="s">
         <v>16</v>
       </c>
@@ -3137,25 +3194,56 @@
       <c r="C31" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="E31" s="8"/>
-      <c r="F31" s="8"/>
-      <c r="G31" s="8"/>
-      <c r="H31" s="7"/>
-      <c r="I31" s="7"/>
-      <c r="J31" s="7"/>
-      <c r="K31" s="8"/>
-      <c r="L31" s="8"/>
-      <c r="M31" s="7"/>
-      <c r="N31" s="7"/>
-      <c r="O31" s="8"/>
-      <c r="P31" s="8"/>
-      <c r="Q31" s="8"/>
-      <c r="R31" s="8"/>
-      <c r="S31" s="7"/>
-      <c r="T31" s="7"/>
-      <c r="U31" s="8"/>
-      <c r="V31" s="7"/>
-      <c r="W31" s="8"/>
+      <c r="D31" s="24">
+        <v>0</v>
+      </c>
+      <c r="E31" s="24">
+        <v>1</v>
+      </c>
+      <c r="F31" s="24">
+        <v>0</v>
+      </c>
+      <c r="G31" s="24">
+        <v>1</v>
+      </c>
+      <c r="H31" s="25">
+        <v>0</v>
+      </c>
+      <c r="I31" s="25">
+        <v>1</v>
+      </c>
+      <c r="J31" s="25">
+        <v>1</v>
+      </c>
+      <c r="K31" s="24">
+        <v>0</v>
+      </c>
+      <c r="L31" s="24">
+        <v>1</v>
+      </c>
+      <c r="M31" s="27"/>
+      <c r="N31" s="27"/>
+      <c r="O31" s="24">
+        <v>0</v>
+      </c>
+      <c r="P31" s="24">
+        <v>0</v>
+      </c>
+      <c r="Q31" s="24">
+        <v>0</v>
+      </c>
+      <c r="R31" s="24">
+        <v>0</v>
+      </c>
+      <c r="S31" s="27"/>
+      <c r="T31" s="27"/>
+      <c r="U31" s="24">
+        <v>1</v>
+      </c>
+      <c r="V31" s="25">
+        <v>1</v>
+      </c>
+      <c r="W31" s="26"/>
       <c r="X31" s="7" t="s">
         <v>16</v>
       </c>
@@ -3182,25 +3270,48 @@
       <c r="C32" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="E32" s="8"/>
-      <c r="F32" s="8"/>
-      <c r="G32" s="8"/>
-      <c r="H32" s="7"/>
-      <c r="I32" s="7"/>
-      <c r="J32" s="7"/>
-      <c r="K32" s="8"/>
-      <c r="L32" s="8"/>
-      <c r="M32" s="7"/>
-      <c r="N32" s="7"/>
-      <c r="O32" s="8"/>
-      <c r="P32" s="8"/>
-      <c r="Q32" s="8"/>
-      <c r="R32" s="8"/>
-      <c r="S32" s="7"/>
-      <c r="T32" s="7"/>
-      <c r="U32" s="8"/>
-      <c r="V32" s="7"/>
-      <c r="W32" s="8"/>
+      <c r="D32" s="24">
+        <v>0</v>
+      </c>
+      <c r="E32" s="24">
+        <v>0</v>
+      </c>
+      <c r="F32" s="24">
+        <v>1</v>
+      </c>
+      <c r="G32" s="24">
+        <v>1</v>
+      </c>
+      <c r="H32" s="25">
+        <v>1</v>
+      </c>
+      <c r="I32" s="25">
+        <v>0</v>
+      </c>
+      <c r="J32" s="25">
+        <v>1</v>
+      </c>
+      <c r="K32" s="24">
+        <v>1</v>
+      </c>
+      <c r="L32" s="24">
+        <v>0</v>
+      </c>
+      <c r="M32" s="27"/>
+      <c r="N32" s="27"/>
+      <c r="O32" s="26"/>
+      <c r="P32" s="26"/>
+      <c r="Q32" s="26"/>
+      <c r="R32" s="26"/>
+      <c r="S32" s="25">
+        <v>0</v>
+      </c>
+      <c r="T32" s="25">
+        <v>1</v>
+      </c>
+      <c r="U32" s="26"/>
+      <c r="V32" s="27"/>
+      <c r="W32" s="26"/>
       <c r="X32" s="7" t="s">
         <v>16</v>
       </c>
@@ -3227,25 +3338,50 @@
       <c r="C33" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="E33" s="8"/>
-      <c r="F33" s="8"/>
-      <c r="G33" s="8"/>
-      <c r="H33" s="7"/>
-      <c r="I33" s="7"/>
-      <c r="J33" s="7"/>
-      <c r="K33" s="8"/>
-      <c r="L33" s="8"/>
-      <c r="M33" s="7"/>
-      <c r="N33" s="7"/>
-      <c r="O33" s="8"/>
-      <c r="P33" s="8"/>
-      <c r="Q33" s="8"/>
-      <c r="R33" s="8"/>
-      <c r="S33" s="7"/>
-      <c r="T33" s="7"/>
-      <c r="U33" s="8"/>
-      <c r="V33" s="7"/>
-      <c r="W33" s="8"/>
+      <c r="D33" s="24">
+        <v>0</v>
+      </c>
+      <c r="E33" s="24">
+        <v>1</v>
+      </c>
+      <c r="F33" s="24">
+        <v>0</v>
+      </c>
+      <c r="G33" s="24">
+        <v>1</v>
+      </c>
+      <c r="H33" s="25">
+        <v>0</v>
+      </c>
+      <c r="I33" s="25">
+        <v>1</v>
+      </c>
+      <c r="J33" s="25">
+        <v>1</v>
+      </c>
+      <c r="K33" s="26"/>
+      <c r="L33" s="26"/>
+      <c r="M33" s="27"/>
+      <c r="N33" s="27"/>
+      <c r="O33" s="24">
+        <v>0</v>
+      </c>
+      <c r="P33" s="24">
+        <v>0</v>
+      </c>
+      <c r="Q33" s="24">
+        <v>0</v>
+      </c>
+      <c r="R33" s="24">
+        <v>1</v>
+      </c>
+      <c r="S33" s="27"/>
+      <c r="T33" s="27"/>
+      <c r="U33" s="24">
+        <v>1</v>
+      </c>
+      <c r="V33" s="27"/>
+      <c r="W33" s="26"/>
       <c r="X33" s="7" t="s">
         <v>16</v>
       </c>
@@ -3272,25 +3408,44 @@
       <c r="C34" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="E34" s="8"/>
-      <c r="F34" s="8"/>
-      <c r="G34" s="8"/>
-      <c r="H34" s="7"/>
-      <c r="I34" s="7"/>
-      <c r="J34" s="7"/>
-      <c r="K34" s="8"/>
-      <c r="L34" s="8"/>
-      <c r="M34" s="7"/>
-      <c r="N34" s="7"/>
-      <c r="O34" s="8"/>
-      <c r="P34" s="8"/>
-      <c r="Q34" s="8"/>
-      <c r="R34" s="8"/>
-      <c r="S34" s="7"/>
-      <c r="T34" s="7"/>
-      <c r="U34" s="8"/>
-      <c r="V34" s="7"/>
-      <c r="W34" s="8"/>
+      <c r="D34" s="24">
+        <v>0</v>
+      </c>
+      <c r="E34" s="24">
+        <v>0</v>
+      </c>
+      <c r="F34" s="24">
+        <v>1</v>
+      </c>
+      <c r="G34" s="24">
+        <v>1</v>
+      </c>
+      <c r="H34" s="25">
+        <v>1</v>
+      </c>
+      <c r="I34" s="25">
+        <v>0</v>
+      </c>
+      <c r="J34" s="25">
+        <v>1</v>
+      </c>
+      <c r="K34" s="24">
+        <v>0</v>
+      </c>
+      <c r="L34" s="24">
+        <v>1</v>
+      </c>
+      <c r="M34" s="27"/>
+      <c r="N34" s="27"/>
+      <c r="O34" s="26"/>
+      <c r="P34" s="26"/>
+      <c r="Q34" s="26"/>
+      <c r="R34" s="26"/>
+      <c r="S34" s="27"/>
+      <c r="T34" s="27"/>
+      <c r="U34" s="26"/>
+      <c r="V34" s="27"/>
+      <c r="W34" s="26"/>
       <c r="X34" s="7" t="s">
         <v>16</v>
       </c>
@@ -3317,25 +3472,34 @@
       <c r="C35" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="E35" s="8"/>
-      <c r="F35" s="8"/>
-      <c r="G35" s="8"/>
-      <c r="H35" s="7"/>
-      <c r="I35" s="7"/>
-      <c r="J35" s="7"/>
-      <c r="K35" s="8"/>
-      <c r="L35" s="8"/>
-      <c r="M35" s="7"/>
-      <c r="N35" s="7"/>
-      <c r="O35" s="8"/>
-      <c r="P35" s="8"/>
-      <c r="Q35" s="8"/>
-      <c r="R35" s="8"/>
-      <c r="S35" s="7"/>
-      <c r="T35" s="7"/>
-      <c r="U35" s="8"/>
-      <c r="V35" s="7"/>
-      <c r="W35" s="8"/>
+      <c r="D35" s="26"/>
+      <c r="E35" s="26"/>
+      <c r="F35" s="26"/>
+      <c r="G35" s="26"/>
+      <c r="H35" s="27"/>
+      <c r="I35" s="27"/>
+      <c r="J35" s="27"/>
+      <c r="K35" s="24">
+        <v>1</v>
+      </c>
+      <c r="L35" s="24">
+        <v>0</v>
+      </c>
+      <c r="M35" s="27"/>
+      <c r="N35" s="27"/>
+      <c r="O35" s="26"/>
+      <c r="P35" s="26"/>
+      <c r="Q35" s="26"/>
+      <c r="R35" s="26"/>
+      <c r="S35" s="25">
+        <v>0</v>
+      </c>
+      <c r="T35" s="25">
+        <v>1</v>
+      </c>
+      <c r="U35" s="26"/>
+      <c r="V35" s="27"/>
+      <c r="W35" s="26"/>
       <c r="X35" s="7" t="s">
         <v>16</v>
       </c>
@@ -3362,25 +3526,56 @@
       <c r="C36" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="E36" s="8"/>
-      <c r="F36" s="8"/>
-      <c r="G36" s="8"/>
-      <c r="H36" s="7"/>
-      <c r="I36" s="7"/>
-      <c r="J36" s="7"/>
-      <c r="K36" s="8"/>
-      <c r="L36" s="8"/>
-      <c r="M36" s="7"/>
-      <c r="N36" s="7"/>
-      <c r="O36" s="8"/>
-      <c r="P36" s="8"/>
-      <c r="Q36" s="8"/>
-      <c r="R36" s="8"/>
-      <c r="S36" s="7"/>
-      <c r="T36" s="7"/>
-      <c r="U36" s="8"/>
-      <c r="V36" s="7"/>
-      <c r="W36" s="8"/>
+      <c r="D36" s="24">
+        <v>0</v>
+      </c>
+      <c r="E36" s="24">
+        <v>0</v>
+      </c>
+      <c r="F36" s="24">
+        <v>0</v>
+      </c>
+      <c r="G36" s="24">
+        <v>1</v>
+      </c>
+      <c r="H36" s="25">
+        <v>0</v>
+      </c>
+      <c r="I36" s="25">
+        <v>1</v>
+      </c>
+      <c r="J36" s="25">
+        <v>1</v>
+      </c>
+      <c r="K36" s="24">
+        <v>0</v>
+      </c>
+      <c r="L36" s="24">
+        <v>1</v>
+      </c>
+      <c r="M36" s="27"/>
+      <c r="N36" s="27"/>
+      <c r="O36" s="24">
+        <v>0</v>
+      </c>
+      <c r="P36" s="24">
+        <v>0</v>
+      </c>
+      <c r="Q36" s="24">
+        <v>0</v>
+      </c>
+      <c r="R36" s="24">
+        <v>0</v>
+      </c>
+      <c r="S36" s="27"/>
+      <c r="T36" s="27"/>
+      <c r="U36" s="24">
+        <v>1</v>
+      </c>
+      <c r="V36" s="25">
+        <v>1</v>
+      </c>
+      <c r="W36" s="26"/>
       <c r="X36" s="7" t="s">
         <v>16</v>
       </c>
@@ -3407,25 +3602,48 @@
       <c r="C37" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="E37" s="8"/>
-      <c r="F37" s="8"/>
-      <c r="G37" s="8"/>
-      <c r="H37" s="7"/>
-      <c r="I37" s="7"/>
-      <c r="J37" s="7"/>
-      <c r="K37" s="8"/>
-      <c r="L37" s="8"/>
-      <c r="M37" s="7"/>
-      <c r="N37" s="7"/>
-      <c r="O37" s="8"/>
-      <c r="P37" s="8"/>
-      <c r="Q37" s="8"/>
-      <c r="R37" s="8"/>
-      <c r="S37" s="7"/>
-      <c r="T37" s="7"/>
-      <c r="U37" s="8"/>
-      <c r="V37" s="7"/>
-      <c r="W37" s="8"/>
+      <c r="D37" s="24">
+        <v>0</v>
+      </c>
+      <c r="E37" s="24">
+        <v>0</v>
+      </c>
+      <c r="F37" s="24">
+        <v>1</v>
+      </c>
+      <c r="G37" s="24">
+        <v>1</v>
+      </c>
+      <c r="H37" s="25">
+        <v>0</v>
+      </c>
+      <c r="I37" s="25">
+        <v>0</v>
+      </c>
+      <c r="J37" s="25">
+        <v>1</v>
+      </c>
+      <c r="K37" s="24">
+        <v>1</v>
+      </c>
+      <c r="L37" s="24">
+        <v>0</v>
+      </c>
+      <c r="M37" s="27"/>
+      <c r="N37" s="27"/>
+      <c r="O37" s="26"/>
+      <c r="P37" s="26"/>
+      <c r="Q37" s="26"/>
+      <c r="R37" s="26"/>
+      <c r="S37" s="25">
+        <v>0</v>
+      </c>
+      <c r="T37" s="25">
+        <v>1</v>
+      </c>
+      <c r="U37" s="26"/>
+      <c r="V37" s="27"/>
+      <c r="W37" s="26"/>
       <c r="X37" s="7" t="s">
         <v>16</v>
       </c>
@@ -3452,25 +3670,38 @@
       <c r="C38" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="E38" s="8"/>
-      <c r="F38" s="8"/>
-      <c r="G38" s="8"/>
-      <c r="H38" s="7"/>
-      <c r="I38" s="7"/>
-      <c r="J38" s="7"/>
-      <c r="K38" s="8"/>
-      <c r="L38" s="8"/>
-      <c r="M38" s="7"/>
-      <c r="N38" s="7"/>
-      <c r="O38" s="8"/>
-      <c r="P38" s="8"/>
-      <c r="Q38" s="8"/>
-      <c r="R38" s="8"/>
-      <c r="S38" s="7"/>
-      <c r="T38" s="7"/>
-      <c r="U38" s="8"/>
-      <c r="V38" s="7"/>
-      <c r="W38" s="8"/>
+      <c r="D38" s="24">
+        <v>0</v>
+      </c>
+      <c r="E38" s="24">
+        <v>0</v>
+      </c>
+      <c r="F38" s="24">
+        <v>1</v>
+      </c>
+      <c r="G38" s="24">
+        <v>0</v>
+      </c>
+      <c r="H38" s="27"/>
+      <c r="I38" s="27"/>
+      <c r="J38" s="27"/>
+      <c r="K38" s="26"/>
+      <c r="L38" s="26"/>
+      <c r="M38" s="25">
+        <v>0</v>
+      </c>
+      <c r="N38" s="25">
+        <v>1</v>
+      </c>
+      <c r="O38" s="26"/>
+      <c r="P38" s="26"/>
+      <c r="Q38" s="26"/>
+      <c r="R38" s="26"/>
+      <c r="S38" s="27"/>
+      <c r="T38" s="27"/>
+      <c r="U38" s="26"/>
+      <c r="V38" s="27"/>
+      <c r="W38" s="26"/>
       <c r="X38" s="7" t="s">
         <v>16</v>
       </c>
@@ -3497,25 +3728,48 @@
       <c r="C39" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="E39" s="8"/>
-      <c r="F39" s="8"/>
-      <c r="G39" s="8"/>
-      <c r="H39" s="7"/>
-      <c r="I39" s="7"/>
-      <c r="J39" s="7"/>
-      <c r="K39" s="8"/>
-      <c r="L39" s="8"/>
-      <c r="M39" s="7"/>
-      <c r="N39" s="7"/>
-      <c r="O39" s="8"/>
-      <c r="P39" s="8"/>
-      <c r="Q39" s="8"/>
-      <c r="R39" s="8"/>
-      <c r="S39" s="7"/>
-      <c r="T39" s="7"/>
-      <c r="U39" s="8"/>
-      <c r="V39" s="7"/>
-      <c r="W39" s="8"/>
+      <c r="D39" s="24">
+        <v>0</v>
+      </c>
+      <c r="E39" s="24">
+        <v>1</v>
+      </c>
+      <c r="F39" s="24">
+        <v>0</v>
+      </c>
+      <c r="G39" s="24">
+        <v>1</v>
+      </c>
+      <c r="H39" s="25">
+        <v>0</v>
+      </c>
+      <c r="I39" s="25">
+        <v>1</v>
+      </c>
+      <c r="J39" s="25">
+        <v>1</v>
+      </c>
+      <c r="K39" s="26"/>
+      <c r="L39" s="26"/>
+      <c r="M39" s="27"/>
+      <c r="N39" s="27"/>
+      <c r="O39" s="24">
+        <v>0</v>
+      </c>
+      <c r="P39" s="24">
+        <v>0</v>
+      </c>
+      <c r="Q39" s="24">
+        <v>0</v>
+      </c>
+      <c r="R39" s="24">
+        <v>0</v>
+      </c>
+      <c r="S39" s="27"/>
+      <c r="T39" s="27"/>
+      <c r="U39" s="26"/>
+      <c r="V39" s="27"/>
+      <c r="W39" s="26"/>
       <c r="X39" s="7" t="s">
         <v>16</v>
       </c>
@@ -3542,25 +3796,38 @@
       <c r="C40" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="E40" s="8"/>
-      <c r="F40" s="8"/>
-      <c r="G40" s="8"/>
-      <c r="H40" s="7"/>
-      <c r="I40" s="7"/>
-      <c r="J40" s="7"/>
-      <c r="K40" s="8"/>
-      <c r="L40" s="8"/>
-      <c r="M40" s="7"/>
-      <c r="N40" s="7"/>
-      <c r="O40" s="8"/>
-      <c r="P40" s="8"/>
-      <c r="Q40" s="8"/>
-      <c r="R40" s="8"/>
-      <c r="S40" s="7"/>
-      <c r="T40" s="7"/>
-      <c r="U40" s="8"/>
-      <c r="V40" s="7"/>
-      <c r="W40" s="8"/>
+      <c r="D40" s="24">
+        <v>0</v>
+      </c>
+      <c r="E40" s="24">
+        <v>0</v>
+      </c>
+      <c r="F40" s="24">
+        <v>1</v>
+      </c>
+      <c r="G40" s="24">
+        <v>1</v>
+      </c>
+      <c r="H40" s="27"/>
+      <c r="I40" s="27"/>
+      <c r="J40" s="27"/>
+      <c r="K40" s="24">
+        <v>0</v>
+      </c>
+      <c r="L40" s="24">
+        <v>1</v>
+      </c>
+      <c r="M40" s="27"/>
+      <c r="N40" s="27"/>
+      <c r="O40" s="26"/>
+      <c r="P40" s="26"/>
+      <c r="Q40" s="26"/>
+      <c r="R40" s="26"/>
+      <c r="S40" s="27"/>
+      <c r="T40" s="27"/>
+      <c r="U40" s="26"/>
+      <c r="V40" s="27"/>
+      <c r="W40" s="26"/>
       <c r="X40" s="7" t="s">
         <v>16</v>
       </c>
@@ -3587,25 +3854,34 @@
       <c r="C41" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="E41" s="8"/>
-      <c r="F41" s="8"/>
-      <c r="G41" s="8"/>
-      <c r="H41" s="7"/>
-      <c r="I41" s="7"/>
-      <c r="J41" s="7"/>
-      <c r="K41" s="8"/>
-      <c r="L41" s="8"/>
-      <c r="M41" s="7"/>
-      <c r="N41" s="7"/>
-      <c r="O41" s="8"/>
-      <c r="P41" s="8"/>
-      <c r="Q41" s="8"/>
-      <c r="R41" s="8"/>
-      <c r="S41" s="7"/>
-      <c r="T41" s="7"/>
-      <c r="U41" s="8"/>
-      <c r="V41" s="7"/>
-      <c r="W41" s="8"/>
+      <c r="D41" s="26"/>
+      <c r="E41" s="26"/>
+      <c r="F41" s="26"/>
+      <c r="G41" s="26"/>
+      <c r="H41" s="27"/>
+      <c r="I41" s="27"/>
+      <c r="J41" s="27"/>
+      <c r="K41" s="24">
+        <v>1</v>
+      </c>
+      <c r="L41" s="24">
+        <v>0</v>
+      </c>
+      <c r="M41" s="27"/>
+      <c r="N41" s="27"/>
+      <c r="O41" s="26"/>
+      <c r="P41" s="26"/>
+      <c r="Q41" s="26"/>
+      <c r="R41" s="26"/>
+      <c r="S41" s="25">
+        <v>0</v>
+      </c>
+      <c r="T41" s="25">
+        <v>1</v>
+      </c>
+      <c r="U41" s="26"/>
+      <c r="V41" s="27"/>
+      <c r="W41" s="26"/>
       <c r="X41" s="7" t="s">
         <v>16</v>
       </c>
@@ -3635,25 +3911,38 @@
       <c r="C42" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="E42" s="8"/>
-      <c r="F42" s="8"/>
-      <c r="G42" s="8"/>
-      <c r="H42" s="7"/>
-      <c r="I42" s="7"/>
-      <c r="J42" s="7"/>
-      <c r="K42" s="8"/>
-      <c r="L42" s="8"/>
-      <c r="M42" s="7"/>
-      <c r="N42" s="7"/>
-      <c r="O42" s="8"/>
-      <c r="P42" s="8"/>
-      <c r="Q42" s="8"/>
-      <c r="R42" s="8"/>
-      <c r="S42" s="7"/>
-      <c r="T42" s="7"/>
-      <c r="U42" s="8"/>
-      <c r="V42" s="7"/>
-      <c r="W42" s="8"/>
+      <c r="D42" s="24">
+        <v>0</v>
+      </c>
+      <c r="E42" s="24">
+        <v>0</v>
+      </c>
+      <c r="F42" s="24">
+        <v>1</v>
+      </c>
+      <c r="G42" s="24">
+        <v>0</v>
+      </c>
+      <c r="H42" s="27"/>
+      <c r="I42" s="27"/>
+      <c r="J42" s="27"/>
+      <c r="K42" s="24">
+        <v>0</v>
+      </c>
+      <c r="L42" s="24">
+        <v>1</v>
+      </c>
+      <c r="M42" s="27"/>
+      <c r="N42" s="27"/>
+      <c r="O42" s="26"/>
+      <c r="P42" s="26"/>
+      <c r="Q42" s="26"/>
+      <c r="R42" s="26"/>
+      <c r="S42" s="27"/>
+      <c r="T42" s="27"/>
+      <c r="U42" s="26"/>
+      <c r="V42" s="27"/>
+      <c r="W42" s="26"/>
       <c r="X42" s="7" t="s">
         <v>16</v>
       </c>
@@ -3680,25 +3969,34 @@
       <c r="C43" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="E43" s="8"/>
-      <c r="F43" s="8"/>
-      <c r="G43" s="8"/>
-      <c r="H43" s="7"/>
-      <c r="I43" s="7"/>
-      <c r="J43" s="7"/>
-      <c r="K43" s="8"/>
-      <c r="L43" s="8"/>
-      <c r="M43" s="7"/>
-      <c r="N43" s="7"/>
-      <c r="O43" s="8"/>
-      <c r="P43" s="8"/>
-      <c r="Q43" s="8"/>
-      <c r="R43" s="8"/>
-      <c r="S43" s="7"/>
-      <c r="T43" s="7"/>
-      <c r="U43" s="8"/>
-      <c r="V43" s="7"/>
-      <c r="W43" s="8"/>
+      <c r="D43" s="26"/>
+      <c r="E43" s="26"/>
+      <c r="F43" s="26"/>
+      <c r="G43" s="26"/>
+      <c r="H43" s="27"/>
+      <c r="I43" s="27"/>
+      <c r="J43" s="27"/>
+      <c r="K43" s="24">
+        <v>1</v>
+      </c>
+      <c r="L43" s="24">
+        <v>0</v>
+      </c>
+      <c r="M43" s="27"/>
+      <c r="N43" s="27"/>
+      <c r="O43" s="26"/>
+      <c r="P43" s="26"/>
+      <c r="Q43" s="26"/>
+      <c r="R43" s="26"/>
+      <c r="S43" s="25">
+        <v>0</v>
+      </c>
+      <c r="T43" s="25">
+        <v>1</v>
+      </c>
+      <c r="U43" s="26"/>
+      <c r="V43" s="27"/>
+      <c r="W43" s="26"/>
       <c r="X43" s="7" t="s">
         <v>16</v>
       </c>
@@ -3725,25 +4023,38 @@
       <c r="C44" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="E44" s="8"/>
-      <c r="F44" s="8"/>
-      <c r="G44" s="8"/>
-      <c r="H44" s="7"/>
-      <c r="I44" s="7"/>
-      <c r="J44" s="7"/>
-      <c r="K44" s="8"/>
-      <c r="L44" s="8"/>
-      <c r="M44" s="7"/>
-      <c r="N44" s="7"/>
-      <c r="O44" s="8"/>
-      <c r="P44" s="8"/>
-      <c r="Q44" s="8"/>
-      <c r="R44" s="8"/>
-      <c r="S44" s="7"/>
-      <c r="T44" s="7"/>
-      <c r="U44" s="8"/>
-      <c r="V44" s="7"/>
-      <c r="W44" s="8"/>
+      <c r="D44" s="24">
+        <v>0</v>
+      </c>
+      <c r="E44" s="24">
+        <v>0</v>
+      </c>
+      <c r="F44" s="24">
+        <v>1</v>
+      </c>
+      <c r="G44" s="24">
+        <v>0</v>
+      </c>
+      <c r="H44" s="27"/>
+      <c r="I44" s="27"/>
+      <c r="J44" s="27"/>
+      <c r="K44" s="26"/>
+      <c r="L44" s="26"/>
+      <c r="M44" s="25">
+        <v>1</v>
+      </c>
+      <c r="N44" s="25">
+        <v>1</v>
+      </c>
+      <c r="O44" s="26"/>
+      <c r="P44" s="26"/>
+      <c r="Q44" s="26"/>
+      <c r="R44" s="26"/>
+      <c r="S44" s="27"/>
+      <c r="T44" s="27"/>
+      <c r="U44" s="26"/>
+      <c r="V44" s="27"/>
+      <c r="W44" s="26"/>
       <c r="X44" s="7" t="s">
         <v>17</v>
       </c>
@@ -3806,6 +4117,24 @@
       <c r="C46" s="7" t="s">
         <v>109</v>
       </c>
+      <c r="D46" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E46" s="3">
+        <v>0</v>
+      </c>
+      <c r="F46" s="3">
+        <v>0</v>
+      </c>
+      <c r="G46" s="3">
+        <v>0</v>
+      </c>
+      <c r="M46" s="2">
+        <v>0</v>
+      </c>
+      <c r="N46" s="2">
+        <v>1</v>
+      </c>
       <c r="X46" s="2">
         <v>1</v>
       </c>
@@ -3836,6 +4165,42 @@
       </c>
       <c r="C48" s="7" t="s">
         <v>111</v>
+      </c>
+      <c r="D48" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E48" s="3">
+        <v>0</v>
+      </c>
+      <c r="F48" s="3">
+        <v>0</v>
+      </c>
+      <c r="G48" s="3">
+        <v>0</v>
+      </c>
+      <c r="H48" s="2">
+        <v>0</v>
+      </c>
+      <c r="I48" s="2">
+        <v>1</v>
+      </c>
+      <c r="J48" s="2">
+        <v>1</v>
+      </c>
+      <c r="O48" s="3">
+        <v>0</v>
+      </c>
+      <c r="P48" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q48" s="3">
+        <v>0</v>
+      </c>
+      <c r="R48" s="3">
+        <v>0</v>
+      </c>
+      <c r="U48" s="3">
+        <v>1</v>
       </c>
       <c r="X48" s="2">
         <v>1</v>
@@ -3891,6 +4256,42 @@
       <c r="C50" s="7" t="s">
         <v>111</v>
       </c>
+      <c r="D50" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E50" s="3">
+        <v>0</v>
+      </c>
+      <c r="F50" s="3">
+        <v>0</v>
+      </c>
+      <c r="G50" s="3">
+        <v>1</v>
+      </c>
+      <c r="H50" s="2">
+        <v>0</v>
+      </c>
+      <c r="I50" s="2">
+        <v>1</v>
+      </c>
+      <c r="J50" s="2">
+        <v>1</v>
+      </c>
+      <c r="O50" s="3">
+        <v>0</v>
+      </c>
+      <c r="P50" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q50" s="3">
+        <v>0</v>
+      </c>
+      <c r="R50" s="3">
+        <v>0</v>
+      </c>
+      <c r="W50" s="3">
+        <v>1</v>
+      </c>
       <c r="X50" s="2">
         <v>1</v>
       </c>
@@ -3945,6 +4346,42 @@
       <c r="C52" s="7" t="s">
         <v>111</v>
       </c>
+      <c r="D52" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E52" s="21">
+        <v>0</v>
+      </c>
+      <c r="F52" s="21">
+        <v>0</v>
+      </c>
+      <c r="G52" s="21">
+        <v>1</v>
+      </c>
+      <c r="H52" s="2">
+        <v>0</v>
+      </c>
+      <c r="I52" s="2">
+        <v>1</v>
+      </c>
+      <c r="J52" s="2">
+        <v>1</v>
+      </c>
+      <c r="O52" s="3">
+        <v>1</v>
+      </c>
+      <c r="P52" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q52" s="3">
+        <v>0</v>
+      </c>
+      <c r="R52" s="3">
+        <v>0</v>
+      </c>
+      <c r="W52" s="3">
+        <v>1</v>
+      </c>
       <c r="X52" s="2">
         <v>1</v>
       </c>
@@ -3999,6 +4436,42 @@
       <c r="C54" s="7" t="s">
         <v>111</v>
       </c>
+      <c r="D54" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E54" s="21">
+        <v>0</v>
+      </c>
+      <c r="F54" s="21">
+        <v>0</v>
+      </c>
+      <c r="G54" s="21">
+        <v>1</v>
+      </c>
+      <c r="H54" s="2">
+        <v>0</v>
+      </c>
+      <c r="I54" s="2">
+        <v>1</v>
+      </c>
+      <c r="J54" s="2">
+        <v>1</v>
+      </c>
+      <c r="O54" s="3">
+        <v>0</v>
+      </c>
+      <c r="P54" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q54" s="3">
+        <v>0</v>
+      </c>
+      <c r="R54" s="3">
+        <v>1</v>
+      </c>
+      <c r="W54" s="3">
+        <v>1</v>
+      </c>
       <c r="X54" s="2">
         <v>1</v>
       </c>
@@ -4030,6 +4503,42 @@
       <c r="C56" s="7" t="s">
         <v>111</v>
       </c>
+      <c r="D56" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E56" s="21">
+        <v>0</v>
+      </c>
+      <c r="F56" s="21">
+        <v>0</v>
+      </c>
+      <c r="G56" s="21">
+        <v>1</v>
+      </c>
+      <c r="H56" s="2">
+        <v>0</v>
+      </c>
+      <c r="I56" s="2">
+        <v>1</v>
+      </c>
+      <c r="J56" s="2">
+        <v>1</v>
+      </c>
+      <c r="O56" s="3">
+        <v>1</v>
+      </c>
+      <c r="P56" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q56" s="3">
+        <v>0</v>
+      </c>
+      <c r="R56" s="3">
+        <v>1</v>
+      </c>
+      <c r="W56" s="3">
+        <v>1</v>
+      </c>
       <c r="X56" s="2">
         <v>1</v>
       </c>
@@ -4061,6 +4570,42 @@
       <c r="C58" s="7" t="s">
         <v>111</v>
       </c>
+      <c r="D58" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E58" s="21">
+        <v>0</v>
+      </c>
+      <c r="F58" s="21">
+        <v>0</v>
+      </c>
+      <c r="G58" s="21">
+        <v>1</v>
+      </c>
+      <c r="H58" s="2">
+        <v>0</v>
+      </c>
+      <c r="I58" s="2">
+        <v>1</v>
+      </c>
+      <c r="J58" s="2">
+        <v>1</v>
+      </c>
+      <c r="O58" s="3">
+        <v>0</v>
+      </c>
+      <c r="P58" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q58" s="3">
+        <v>1</v>
+      </c>
+      <c r="R58" s="3">
+        <v>0</v>
+      </c>
+      <c r="W58" s="3">
+        <v>1</v>
+      </c>
       <c r="X58" s="2">
         <v>1</v>
       </c>
@@ -4092,6 +4637,42 @@
       <c r="C60" s="7" t="s">
         <v>111</v>
       </c>
+      <c r="D60" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E60" s="21">
+        <v>0</v>
+      </c>
+      <c r="F60" s="21">
+        <v>0</v>
+      </c>
+      <c r="G60" s="21">
+        <v>1</v>
+      </c>
+      <c r="H60" s="2">
+        <v>0</v>
+      </c>
+      <c r="I60" s="2">
+        <v>1</v>
+      </c>
+      <c r="J60" s="2">
+        <v>1</v>
+      </c>
+      <c r="O60" s="3">
+        <v>0</v>
+      </c>
+      <c r="P60" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q60" s="3">
+        <v>1</v>
+      </c>
+      <c r="R60" s="3">
+        <v>1</v>
+      </c>
+      <c r="W60" s="3">
+        <v>1</v>
+      </c>
       <c r="X60" s="2">
         <v>1</v>
       </c>
@@ -4123,6 +4704,42 @@
       <c r="C62" s="7" t="s">
         <v>111</v>
       </c>
+      <c r="D62" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E62" s="21">
+        <v>0</v>
+      </c>
+      <c r="F62" s="21">
+        <v>0</v>
+      </c>
+      <c r="G62" s="21">
+        <v>1</v>
+      </c>
+      <c r="H62" s="2">
+        <v>0</v>
+      </c>
+      <c r="I62" s="2">
+        <v>1</v>
+      </c>
+      <c r="J62" s="2">
+        <v>1</v>
+      </c>
+      <c r="O62" s="3">
+        <v>0</v>
+      </c>
+      <c r="P62" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q62" s="3">
+        <v>0</v>
+      </c>
+      <c r="R62" s="3">
+        <v>0</v>
+      </c>
+      <c r="W62" s="3">
+        <v>1</v>
+      </c>
       <c r="X62" s="2">
         <v>1</v>
       </c>
@@ -4154,26 +4771,50 @@
       <c r="C64" s="5">
         <v>0</v>
       </c>
-      <c r="D64" s="4"/>
-      <c r="E64" s="4"/>
-      <c r="F64" s="4"/>
-      <c r="G64" s="4"/>
-      <c r="H64" s="5"/>
-      <c r="I64" s="5"/>
-      <c r="J64" s="5"/>
+      <c r="D64" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E64" s="21">
+        <v>0</v>
+      </c>
+      <c r="F64" s="21">
+        <v>0</v>
+      </c>
+      <c r="G64" s="21">
+        <v>1</v>
+      </c>
+      <c r="H64" s="5">
+        <v>0</v>
+      </c>
+      <c r="I64" s="5">
+        <v>1</v>
+      </c>
+      <c r="J64" s="5">
+        <v>1</v>
+      </c>
       <c r="K64" s="4"/>
       <c r="L64" s="4"/>
       <c r="M64" s="5"/>
       <c r="N64" s="5"/>
-      <c r="O64" s="4"/>
-      <c r="P64" s="4"/>
-      <c r="Q64" s="4"/>
-      <c r="R64" s="4"/>
+      <c r="O64" s="4">
+        <v>0</v>
+      </c>
+      <c r="P64" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q64" s="4">
+        <v>0</v>
+      </c>
+      <c r="R64" s="4">
+        <v>1</v>
+      </c>
       <c r="S64" s="5"/>
       <c r="T64" s="5"/>
       <c r="U64" s="4"/>
       <c r="V64" s="5"/>
-      <c r="W64" s="4"/>
+      <c r="W64" s="4">
+        <v>1</v>
+      </c>
       <c r="X64" s="5"/>
       <c r="Y64" s="5"/>
       <c r="AA64" s="3">
@@ -4767,7 +5408,11 @@
     <mergeCell ref="H2:J2"/>
     <mergeCell ref="K2:L2"/>
   </mergeCells>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="D29" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add 1 Op + Bakr review
</commit_message>
<xml_diff>
--- a/Microroutines.xlsx
+++ b/Microroutines.xlsx
@@ -1,23 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study\Third Year\arch\PDP11\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B3C5A8B-A60C-4C7B-9106-639657580226}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13716" yWindow="3732" windowWidth="9324" windowHeight="8616" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13710" yWindow="3735" windowWidth="9330" windowHeight="8610"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="125725"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="166">
   <si>
     <t>Micro instruction</t>
   </si>
@@ -276,9 +270,6 @@
     <t>fetch &amp; decode</t>
   </si>
   <si>
-    <t xml:space="preserve">SOURCE_out Z_in Y_clear Add </t>
-  </si>
-  <si>
     <t>DEST_out add Z_in FLAGS_in</t>
   </si>
   <si>
@@ -411,9 +402,6 @@
     <t>CLR:</t>
   </si>
   <si>
-    <t>Z_in clr</t>
-  </si>
-  <si>
     <t>INV:</t>
   </si>
   <si>
@@ -523,51 +511,104 @@
   </si>
   <si>
     <t xml:space="preserve">JST, RTS, IRET </t>
+  </si>
+  <si>
+    <r>
+      <t>Z_in clr</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Flags_in</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">SOURCE_out Z_in Y_clear Add </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Flags_in</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF9C0006"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -616,7 +657,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
@@ -673,12 +714,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -691,6 +726,19 @@
     <xf numFmtId="2" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Accent2" xfId="4" builtinId="33"/>
@@ -755,7 +803,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -790,7 +838,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -967,54 +1015,54 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AC99"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="82" zoomScaleNormal="82" zoomScaleSheetLayoutView="86" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A48" sqref="A48"/>
+      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="47.109375" customWidth="1"/>
-    <col min="2" max="2" width="8.77734375" style="6" customWidth="1"/>
-    <col min="3" max="3" width="7.33203125" style="7" customWidth="1"/>
-    <col min="4" max="4" width="2.6640625" style="8" customWidth="1"/>
+    <col min="1" max="1" width="47.125" customWidth="1"/>
+    <col min="2" max="2" width="8.75" style="6" customWidth="1"/>
+    <col min="3" max="3" width="7.375" style="7" customWidth="1"/>
+    <col min="4" max="4" width="2.625" style="8" customWidth="1"/>
     <col min="5" max="5" width="3" style="3" customWidth="1"/>
-    <col min="6" max="6" width="3.109375" style="3" customWidth="1"/>
-    <col min="7" max="7" width="3.77734375" style="3" customWidth="1"/>
+    <col min="6" max="6" width="3.125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="3.75" style="3" customWidth="1"/>
     <col min="8" max="8" width="3" style="2" customWidth="1"/>
-    <col min="9" max="9" width="3.44140625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="2.88671875" style="2" customWidth="1"/>
-    <col min="11" max="11" width="3.21875" style="3" customWidth="1"/>
-    <col min="12" max="12" width="3.6640625" style="3" customWidth="1"/>
-    <col min="13" max="13" width="3.6640625" style="2" customWidth="1"/>
-    <col min="14" max="14" width="3.109375" style="2" customWidth="1"/>
-    <col min="15" max="16" width="3.6640625" style="3" customWidth="1"/>
-    <col min="17" max="17" width="3.44140625" style="3" customWidth="1"/>
-    <col min="18" max="18" width="3.33203125" style="3" customWidth="1"/>
-    <col min="19" max="19" width="3.77734375" style="2" customWidth="1"/>
-    <col min="20" max="20" width="3.5546875" style="2" customWidth="1"/>
+    <col min="9" max="9" width="3.5" style="2" customWidth="1"/>
+    <col min="10" max="10" width="2.875" style="2" customWidth="1"/>
+    <col min="11" max="11" width="3.25" style="3" customWidth="1"/>
+    <col min="12" max="12" width="3.625" style="3" customWidth="1"/>
+    <col min="13" max="13" width="3.625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="3.125" style="2" customWidth="1"/>
+    <col min="15" max="16" width="3.625" style="3" customWidth="1"/>
+    <col min="17" max="17" width="3.5" style="3" customWidth="1"/>
+    <col min="18" max="18" width="3.375" style="3" customWidth="1"/>
+    <col min="19" max="19" width="3.75" style="2" customWidth="1"/>
+    <col min="20" max="20" width="3.5" style="2" customWidth="1"/>
     <col min="21" max="21" width="3" style="3" customWidth="1"/>
-    <col min="22" max="22" width="3.109375" style="2" customWidth="1"/>
-    <col min="23" max="23" width="3.44140625" style="3" customWidth="1"/>
+    <col min="22" max="22" width="3.125" style="2" customWidth="1"/>
+    <col min="23" max="23" width="3.5" style="3" customWidth="1"/>
     <col min="24" max="24" width="4" style="2" customWidth="1"/>
-    <col min="25" max="25" width="3.5546875" style="2" customWidth="1"/>
-    <col min="26" max="26" width="3.6640625" style="2" customWidth="1"/>
-    <col min="27" max="27" width="3.44140625" style="3" customWidth="1"/>
-    <col min="28" max="28" width="3.44140625" style="16" customWidth="1"/>
-    <col min="29" max="29" width="30.5546875" style="18" customWidth="1"/>
+    <col min="25" max="25" width="3.5" style="2" customWidth="1"/>
+    <col min="26" max="26" width="3.625" style="2" customWidth="1"/>
+    <col min="27" max="27" width="3.5" style="3" customWidth="1"/>
+    <col min="28" max="28" width="3.5" style="16" customWidth="1"/>
+    <col min="29" max="29" width="30.5" style="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:29">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1024,35 +1072,35 @@
       <c r="C1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="D1" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="23" t="s">
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-      <c r="K1" s="22" t="s">
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="L1" s="22"/>
-      <c r="M1" s="23" t="s">
+      <c r="L1" s="26"/>
+      <c r="M1" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="N1" s="23"/>
-      <c r="O1" s="22" t="s">
+      <c r="N1" s="27"/>
+      <c r="O1" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="P1" s="22"/>
-      <c r="Q1" s="22"/>
-      <c r="R1" s="22"/>
-      <c r="S1" s="23" t="s">
+      <c r="P1" s="26"/>
+      <c r="Q1" s="26"/>
+      <c r="R1" s="26"/>
+      <c r="S1" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="T1" s="23"/>
+      <c r="T1" s="27"/>
       <c r="U1" s="3" t="s">
         <v>2</v>
       </c>
@@ -1062,42 +1110,42 @@
       <c r="W1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="X1" s="23" t="s">
+      <c r="X1" s="27" t="s">
         <v>55</v>
       </c>
-      <c r="Y1" s="23"/>
-      <c r="Z1" s="23"/>
+      <c r="Y1" s="27"/>
+      <c r="Z1" s="27"/>
       <c r="AA1" s="3" t="s">
         <v>5</v>
       </c>
       <c r="AB1" s="16" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="AC1" s="17" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23"/>
-      <c r="J2" s="23"/>
-      <c r="K2" s="22"/>
-      <c r="L2" s="22"/>
-      <c r="O2" s="22"/>
-      <c r="P2" s="22"/>
-      <c r="Q2" s="22"/>
-      <c r="R2" s="22"/>
-      <c r="S2" s="23"/>
-      <c r="T2" s="23"/>
-      <c r="X2" s="23"/>
-      <c r="Y2" s="23"/>
-      <c r="Z2" s="23"/>
-    </row>
-    <row r="3" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.3">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="2" spans="1:29">
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="27"/>
+      <c r="J2" s="27"/>
+      <c r="K2" s="26"/>
+      <c r="L2" s="26"/>
+      <c r="O2" s="26"/>
+      <c r="P2" s="26"/>
+      <c r="Q2" s="26"/>
+      <c r="R2" s="26"/>
+      <c r="S2" s="27"/>
+      <c r="T2" s="27"/>
+      <c r="X2" s="27"/>
+      <c r="Y2" s="27"/>
+      <c r="Z2" s="27"/>
+    </row>
+    <row r="3" spans="1:29" s="9" customFormat="1">
       <c r="A3" s="9" t="s">
         <v>82</v>
       </c>
@@ -1130,7 +1178,7 @@
       <c r="AB3" s="12"/>
       <c r="AC3" s="19"/>
     </row>
-    <row r="4" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:29" s="1" customFormat="1">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1217,7 +1265,7 @@
       </c>
       <c r="AC4" s="20"/>
     </row>
-    <row r="5" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:29" s="1" customFormat="1">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -1304,7 +1352,7 @@
       </c>
       <c r="AC5" s="20"/>
     </row>
-    <row r="6" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:29" s="1" customFormat="1">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -1391,7 +1439,7 @@
       </c>
       <c r="AC6" s="20"/>
     </row>
-    <row r="7" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:29" s="1" customFormat="1">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1478,7 +1526,7 @@
       </c>
       <c r="AC7" s="20"/>
     </row>
-    <row r="8" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:29" s="9" customFormat="1">
       <c r="A8" s="9" t="s">
         <v>81</v>
       </c>
@@ -1511,12 +1559,12 @@
       <c r="AB8" s="12"/>
       <c r="AC8" s="19"/>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:29">
       <c r="A9" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:29">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -1602,7 +1650,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:29">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -1688,15 +1736,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:29">
       <c r="A12" t="s">
         <v>22</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="7" t="s">
-        <v>43</v>
+      <c r="C12" s="29" t="s">
+        <v>47</v>
       </c>
       <c r="D12" s="8" t="s">
         <v>16</v>
@@ -1774,7 +1822,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:29">
       <c r="A13" t="s">
         <v>26</v>
       </c>
@@ -1860,7 +1908,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:29">
       <c r="A14" t="s">
         <v>23</v>
       </c>
@@ -1946,7 +1994,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:29">
       <c r="A15" t="s">
         <v>29</v>
       </c>
@@ -2032,7 +2080,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:29">
       <c r="A16" t="s">
         <v>31</v>
       </c>
@@ -2118,7 +2166,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:29">
       <c r="A17" t="s">
         <v>22</v>
       </c>
@@ -2204,7 +2252,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:29">
       <c r="A18" t="s">
         <v>36</v>
       </c>
@@ -2290,7 +2338,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:29">
       <c r="A19" t="s">
         <v>35</v>
       </c>
@@ -2376,7 +2424,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:29">
       <c r="A20" t="s">
         <v>38</v>
       </c>
@@ -2462,7 +2510,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:29">
       <c r="A21" t="s">
         <v>40</v>
       </c>
@@ -2548,7 +2596,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:29">
       <c r="A22" t="s">
         <v>42</v>
       </c>
@@ -2634,7 +2682,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:29">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -2720,10 +2768,10 @@
         <v>0</v>
       </c>
       <c r="AC23" s="18" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="24" spans="1:29" x14ac:dyDescent="0.3">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="24" spans="1:29">
       <c r="A24" t="s">
         <v>45</v>
       </c>
@@ -2809,7 +2857,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:29">
       <c r="A25" t="s">
         <v>22</v>
       </c>
@@ -2895,7 +2943,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:29">
       <c r="A26" t="s">
         <v>48</v>
       </c>
@@ -2981,9 +3029,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:29" s="9" customFormat="1">
       <c r="A27" s="9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B27" s="10"/>
       <c r="C27" s="10"/>
@@ -3014,7 +3062,7 @@
       <c r="AB27" s="10"/>
       <c r="AC27" s="19"/>
     </row>
-    <row r="28" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:29">
       <c r="A28" t="s">
         <v>64</v>
       </c>
@@ -3022,40 +3070,40 @@
         <v>46</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="D28" s="24">
-        <v>0</v>
-      </c>
-      <c r="E28" s="24">
-        <v>1</v>
-      </c>
-      <c r="F28" s="24">
-        <v>0</v>
-      </c>
-      <c r="G28" s="24">
-        <v>1</v>
-      </c>
-      <c r="H28" s="27"/>
-      <c r="I28" s="27"/>
-      <c r="J28" s="27"/>
-      <c r="K28" s="26"/>
-      <c r="L28" s="26"/>
-      <c r="M28" s="25">
-        <v>1</v>
-      </c>
-      <c r="N28" s="25">
-        <v>1</v>
-      </c>
-      <c r="O28" s="26"/>
-      <c r="P28" s="26"/>
-      <c r="Q28" s="26"/>
-      <c r="R28" s="26"/>
-      <c r="S28" s="27"/>
-      <c r="T28" s="27"/>
-      <c r="U28" s="26"/>
-      <c r="V28" s="27"/>
-      <c r="W28" s="26"/>
+        <v>109</v>
+      </c>
+      <c r="D28" s="22">
+        <v>0</v>
+      </c>
+      <c r="E28" s="22">
+        <v>1</v>
+      </c>
+      <c r="F28" s="22">
+        <v>0</v>
+      </c>
+      <c r="G28" s="22">
+        <v>1</v>
+      </c>
+      <c r="H28" s="25"/>
+      <c r="I28" s="25"/>
+      <c r="J28" s="25"/>
+      <c r="K28" s="24"/>
+      <c r="L28" s="24"/>
+      <c r="M28" s="23">
+        <v>1</v>
+      </c>
+      <c r="N28" s="23">
+        <v>1</v>
+      </c>
+      <c r="O28" s="24"/>
+      <c r="P28" s="24"/>
+      <c r="Q28" s="24"/>
+      <c r="R28" s="24"/>
+      <c r="S28" s="25"/>
+      <c r="T28" s="25"/>
+      <c r="U28" s="24"/>
+      <c r="V28" s="25"/>
+      <c r="W28" s="24"/>
       <c r="X28" s="7" t="s">
         <v>17</v>
       </c>
@@ -3072,7 +3120,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="29" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:29">
       <c r="A29" t="s">
         <v>57</v>
       </c>
@@ -3082,38 +3130,38 @@
       <c r="C29" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="D29" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="E29" s="24">
-        <v>1</v>
-      </c>
-      <c r="F29" s="24">
-        <v>0</v>
-      </c>
-      <c r="G29" s="24">
-        <v>1</v>
-      </c>
-      <c r="H29" s="27"/>
-      <c r="I29" s="27"/>
-      <c r="J29" s="27"/>
-      <c r="K29" s="24">
-        <v>0</v>
-      </c>
-      <c r="L29" s="24">
-        <v>1</v>
-      </c>
-      <c r="M29" s="27"/>
-      <c r="N29" s="27"/>
-      <c r="O29" s="26"/>
-      <c r="P29" s="26"/>
-      <c r="Q29" s="26"/>
-      <c r="R29" s="26"/>
-      <c r="S29" s="27"/>
-      <c r="T29" s="27"/>
-      <c r="U29" s="26"/>
-      <c r="V29" s="27"/>
-      <c r="W29" s="26"/>
+      <c r="D29" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="E29" s="22">
+        <v>1</v>
+      </c>
+      <c r="F29" s="22">
+        <v>0</v>
+      </c>
+      <c r="G29" s="22">
+        <v>1</v>
+      </c>
+      <c r="H29" s="25"/>
+      <c r="I29" s="25"/>
+      <c r="J29" s="25"/>
+      <c r="K29" s="22">
+        <v>0</v>
+      </c>
+      <c r="L29" s="22">
+        <v>1</v>
+      </c>
+      <c r="M29" s="25"/>
+      <c r="N29" s="25"/>
+      <c r="O29" s="24"/>
+      <c r="P29" s="24"/>
+      <c r="Q29" s="24"/>
+      <c r="R29" s="24"/>
+      <c r="S29" s="25"/>
+      <c r="T29" s="25"/>
+      <c r="U29" s="24"/>
+      <c r="V29" s="25"/>
+      <c r="W29" s="24"/>
       <c r="X29" s="7" t="s">
         <v>16</v>
       </c>
@@ -3130,44 +3178,44 @@
         <v>16</v>
       </c>
     </row>
-    <row r="30" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:29">
       <c r="A30" t="s">
         <v>22</v>
       </c>
       <c r="B30" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="D30" s="26"/>
-      <c r="E30" s="26"/>
-      <c r="F30" s="26"/>
-      <c r="G30" s="26"/>
-      <c r="H30" s="27"/>
-      <c r="I30" s="27"/>
-      <c r="J30" s="27"/>
-      <c r="K30" s="24">
-        <v>1</v>
-      </c>
-      <c r="L30" s="24">
-        <v>0</v>
-      </c>
-      <c r="M30" s="27"/>
-      <c r="N30" s="27"/>
-      <c r="O30" s="26"/>
-      <c r="P30" s="26"/>
-      <c r="Q30" s="26"/>
-      <c r="R30" s="26"/>
-      <c r="S30" s="25">
-        <v>0</v>
-      </c>
-      <c r="T30" s="25">
-        <v>1</v>
-      </c>
-      <c r="U30" s="26"/>
-      <c r="V30" s="27"/>
-      <c r="W30" s="26"/>
+      <c r="C30" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="D30" s="24"/>
+      <c r="E30" s="24"/>
+      <c r="F30" s="24"/>
+      <c r="G30" s="24"/>
+      <c r="H30" s="25"/>
+      <c r="I30" s="25"/>
+      <c r="J30" s="25"/>
+      <c r="K30" s="22">
+        <v>1</v>
+      </c>
+      <c r="L30" s="22">
+        <v>0</v>
+      </c>
+      <c r="M30" s="25"/>
+      <c r="N30" s="25"/>
+      <c r="O30" s="24"/>
+      <c r="P30" s="24"/>
+      <c r="Q30" s="24"/>
+      <c r="R30" s="24"/>
+      <c r="S30" s="23">
+        <v>0</v>
+      </c>
+      <c r="T30" s="23">
+        <v>1</v>
+      </c>
+      <c r="U30" s="24"/>
+      <c r="V30" s="25"/>
+      <c r="W30" s="24"/>
       <c r="X30" s="7" t="s">
         <v>16</v>
       </c>
@@ -3184,7 +3232,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:29">
       <c r="A31" t="s">
         <v>59</v>
       </c>
@@ -3194,56 +3242,56 @@
       <c r="C31" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="D31" s="24">
-        <v>0</v>
-      </c>
-      <c r="E31" s="24">
-        <v>1</v>
-      </c>
-      <c r="F31" s="24">
-        <v>0</v>
-      </c>
-      <c r="G31" s="24">
-        <v>1</v>
-      </c>
-      <c r="H31" s="25">
-        <v>0</v>
-      </c>
-      <c r="I31" s="25">
-        <v>1</v>
-      </c>
-      <c r="J31" s="25">
-        <v>1</v>
-      </c>
-      <c r="K31" s="24">
-        <v>0</v>
-      </c>
-      <c r="L31" s="24">
-        <v>1</v>
-      </c>
-      <c r="M31" s="27"/>
-      <c r="N31" s="27"/>
-      <c r="O31" s="24">
-        <v>0</v>
-      </c>
-      <c r="P31" s="24">
-        <v>0</v>
-      </c>
-      <c r="Q31" s="24">
-        <v>0</v>
-      </c>
-      <c r="R31" s="24">
-        <v>0</v>
-      </c>
-      <c r="S31" s="27"/>
-      <c r="T31" s="27"/>
-      <c r="U31" s="24">
-        <v>1</v>
-      </c>
-      <c r="V31" s="25">
-        <v>1</v>
-      </c>
-      <c r="W31" s="26"/>
+      <c r="D31" s="22">
+        <v>0</v>
+      </c>
+      <c r="E31" s="22">
+        <v>1</v>
+      </c>
+      <c r="F31" s="22">
+        <v>0</v>
+      </c>
+      <c r="G31" s="22">
+        <v>1</v>
+      </c>
+      <c r="H31" s="23">
+        <v>0</v>
+      </c>
+      <c r="I31" s="23">
+        <v>1</v>
+      </c>
+      <c r="J31" s="23">
+        <v>1</v>
+      </c>
+      <c r="K31" s="22">
+        <v>0</v>
+      </c>
+      <c r="L31" s="22">
+        <v>1</v>
+      </c>
+      <c r="M31" s="25"/>
+      <c r="N31" s="25"/>
+      <c r="O31" s="22">
+        <v>0</v>
+      </c>
+      <c r="P31" s="22">
+        <v>0</v>
+      </c>
+      <c r="Q31" s="22">
+        <v>0</v>
+      </c>
+      <c r="R31" s="22">
+        <v>0</v>
+      </c>
+      <c r="S31" s="25"/>
+      <c r="T31" s="25"/>
+      <c r="U31" s="22">
+        <v>1</v>
+      </c>
+      <c r="V31" s="23">
+        <v>1</v>
+      </c>
+      <c r="W31" s="24"/>
       <c r="X31" s="7" t="s">
         <v>16</v>
       </c>
@@ -3260,7 +3308,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="32" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:29">
       <c r="A32" t="s">
         <v>60</v>
       </c>
@@ -3270,48 +3318,48 @@
       <c r="C32" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="D32" s="24">
-        <v>0</v>
-      </c>
-      <c r="E32" s="24">
-        <v>0</v>
-      </c>
-      <c r="F32" s="24">
-        <v>1</v>
-      </c>
-      <c r="G32" s="24">
-        <v>1</v>
-      </c>
-      <c r="H32" s="25">
-        <v>1</v>
-      </c>
-      <c r="I32" s="25">
-        <v>0</v>
-      </c>
-      <c r="J32" s="25">
-        <v>1</v>
-      </c>
-      <c r="K32" s="24">
-        <v>1</v>
-      </c>
-      <c r="L32" s="24">
-        <v>0</v>
-      </c>
-      <c r="M32" s="27"/>
-      <c r="N32" s="27"/>
-      <c r="O32" s="26"/>
-      <c r="P32" s="26"/>
-      <c r="Q32" s="26"/>
-      <c r="R32" s="26"/>
-      <c r="S32" s="25">
-        <v>0</v>
-      </c>
-      <c r="T32" s="25">
-        <v>1</v>
-      </c>
-      <c r="U32" s="26"/>
-      <c r="V32" s="27"/>
-      <c r="W32" s="26"/>
+      <c r="D32" s="22">
+        <v>0</v>
+      </c>
+      <c r="E32" s="22">
+        <v>0</v>
+      </c>
+      <c r="F32" s="22">
+        <v>1</v>
+      </c>
+      <c r="G32" s="22">
+        <v>1</v>
+      </c>
+      <c r="H32" s="23">
+        <v>1</v>
+      </c>
+      <c r="I32" s="23">
+        <v>0</v>
+      </c>
+      <c r="J32" s="23">
+        <v>1</v>
+      </c>
+      <c r="K32" s="22">
+        <v>1</v>
+      </c>
+      <c r="L32" s="22">
+        <v>0</v>
+      </c>
+      <c r="M32" s="25"/>
+      <c r="N32" s="25"/>
+      <c r="O32" s="24"/>
+      <c r="P32" s="24"/>
+      <c r="Q32" s="24"/>
+      <c r="R32" s="24"/>
+      <c r="S32" s="23">
+        <v>0</v>
+      </c>
+      <c r="T32" s="23">
+        <v>1</v>
+      </c>
+      <c r="U32" s="24"/>
+      <c r="V32" s="25"/>
+      <c r="W32" s="24"/>
       <c r="X32" s="7" t="s">
         <v>16</v>
       </c>
@@ -3328,7 +3376,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="33" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:29">
       <c r="A33" t="s">
         <v>61</v>
       </c>
@@ -3338,50 +3386,50 @@
       <c r="C33" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="D33" s="24">
-        <v>0</v>
-      </c>
-      <c r="E33" s="24">
-        <v>1</v>
-      </c>
-      <c r="F33" s="24">
-        <v>0</v>
-      </c>
-      <c r="G33" s="24">
-        <v>1</v>
-      </c>
-      <c r="H33" s="25">
-        <v>0</v>
-      </c>
-      <c r="I33" s="25">
-        <v>1</v>
-      </c>
-      <c r="J33" s="25">
-        <v>1</v>
-      </c>
-      <c r="K33" s="26"/>
-      <c r="L33" s="26"/>
-      <c r="M33" s="27"/>
-      <c r="N33" s="27"/>
-      <c r="O33" s="24">
-        <v>0</v>
-      </c>
-      <c r="P33" s="24">
-        <v>0</v>
-      </c>
-      <c r="Q33" s="24">
-        <v>0</v>
-      </c>
-      <c r="R33" s="24">
-        <v>1</v>
-      </c>
-      <c r="S33" s="27"/>
-      <c r="T33" s="27"/>
-      <c r="U33" s="24">
-        <v>1</v>
-      </c>
-      <c r="V33" s="27"/>
-      <c r="W33" s="26"/>
+      <c r="D33" s="22">
+        <v>0</v>
+      </c>
+      <c r="E33" s="22">
+        <v>1</v>
+      </c>
+      <c r="F33" s="22">
+        <v>0</v>
+      </c>
+      <c r="G33" s="22">
+        <v>1</v>
+      </c>
+      <c r="H33" s="23">
+        <v>0</v>
+      </c>
+      <c r="I33" s="23">
+        <v>1</v>
+      </c>
+      <c r="J33" s="23">
+        <v>1</v>
+      </c>
+      <c r="K33" s="24"/>
+      <c r="L33" s="24"/>
+      <c r="M33" s="25"/>
+      <c r="N33" s="25"/>
+      <c r="O33" s="22">
+        <v>0</v>
+      </c>
+      <c r="P33" s="22">
+        <v>0</v>
+      </c>
+      <c r="Q33" s="22">
+        <v>0</v>
+      </c>
+      <c r="R33" s="22">
+        <v>1</v>
+      </c>
+      <c r="S33" s="25"/>
+      <c r="T33" s="25"/>
+      <c r="U33" s="22">
+        <v>1</v>
+      </c>
+      <c r="V33" s="25"/>
+      <c r="W33" s="24"/>
       <c r="X33" s="7" t="s">
         <v>16</v>
       </c>
@@ -3398,7 +3446,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="34" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:29">
       <c r="A34" t="s">
         <v>62</v>
       </c>
@@ -3408,44 +3456,44 @@
       <c r="C34" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="D34" s="24">
-        <v>0</v>
-      </c>
-      <c r="E34" s="24">
-        <v>0</v>
-      </c>
-      <c r="F34" s="24">
-        <v>1</v>
-      </c>
-      <c r="G34" s="24">
-        <v>1</v>
-      </c>
-      <c r="H34" s="25">
-        <v>1</v>
-      </c>
-      <c r="I34" s="25">
-        <v>0</v>
-      </c>
-      <c r="J34" s="25">
-        <v>1</v>
-      </c>
-      <c r="K34" s="24">
-        <v>0</v>
-      </c>
-      <c r="L34" s="24">
-        <v>1</v>
-      </c>
-      <c r="M34" s="27"/>
-      <c r="N34" s="27"/>
-      <c r="O34" s="26"/>
-      <c r="P34" s="26"/>
-      <c r="Q34" s="26"/>
-      <c r="R34" s="26"/>
-      <c r="S34" s="27"/>
-      <c r="T34" s="27"/>
-      <c r="U34" s="26"/>
-      <c r="V34" s="27"/>
-      <c r="W34" s="26"/>
+      <c r="D34" s="22">
+        <v>0</v>
+      </c>
+      <c r="E34" s="22">
+        <v>0</v>
+      </c>
+      <c r="F34" s="22">
+        <v>1</v>
+      </c>
+      <c r="G34" s="22">
+        <v>1</v>
+      </c>
+      <c r="H34" s="23">
+        <v>1</v>
+      </c>
+      <c r="I34" s="23">
+        <v>0</v>
+      </c>
+      <c r="J34" s="23">
+        <v>1</v>
+      </c>
+      <c r="K34" s="22">
+        <v>0</v>
+      </c>
+      <c r="L34" s="22">
+        <v>1</v>
+      </c>
+      <c r="M34" s="25"/>
+      <c r="N34" s="25"/>
+      <c r="O34" s="24"/>
+      <c r="P34" s="24"/>
+      <c r="Q34" s="24"/>
+      <c r="R34" s="24"/>
+      <c r="S34" s="25"/>
+      <c r="T34" s="25"/>
+      <c r="U34" s="24"/>
+      <c r="V34" s="25"/>
+      <c r="W34" s="24"/>
       <c r="X34" s="7" t="s">
         <v>16</v>
       </c>
@@ -3462,7 +3510,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="35" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:29">
       <c r="A35" t="s">
         <v>22</v>
       </c>
@@ -3472,34 +3520,34 @@
       <c r="C35" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="D35" s="26"/>
-      <c r="E35" s="26"/>
-      <c r="F35" s="26"/>
-      <c r="G35" s="26"/>
-      <c r="H35" s="27"/>
-      <c r="I35" s="27"/>
-      <c r="J35" s="27"/>
-      <c r="K35" s="24">
-        <v>1</v>
-      </c>
-      <c r="L35" s="24">
-        <v>0</v>
-      </c>
-      <c r="M35" s="27"/>
-      <c r="N35" s="27"/>
-      <c r="O35" s="26"/>
-      <c r="P35" s="26"/>
-      <c r="Q35" s="26"/>
-      <c r="R35" s="26"/>
-      <c r="S35" s="25">
-        <v>0</v>
-      </c>
-      <c r="T35" s="25">
-        <v>1</v>
-      </c>
-      <c r="U35" s="26"/>
-      <c r="V35" s="27"/>
-      <c r="W35" s="26"/>
+      <c r="D35" s="24"/>
+      <c r="E35" s="24"/>
+      <c r="F35" s="24"/>
+      <c r="G35" s="24"/>
+      <c r="H35" s="25"/>
+      <c r="I35" s="25"/>
+      <c r="J35" s="25"/>
+      <c r="K35" s="22">
+        <v>1</v>
+      </c>
+      <c r="L35" s="22">
+        <v>0</v>
+      </c>
+      <c r="M35" s="25"/>
+      <c r="N35" s="25"/>
+      <c r="O35" s="24"/>
+      <c r="P35" s="24"/>
+      <c r="Q35" s="24"/>
+      <c r="R35" s="24"/>
+      <c r="S35" s="23">
+        <v>0</v>
+      </c>
+      <c r="T35" s="23">
+        <v>1</v>
+      </c>
+      <c r="U35" s="24"/>
+      <c r="V35" s="25"/>
+      <c r="W35" s="24"/>
       <c r="X35" s="7" t="s">
         <v>16</v>
       </c>
@@ -3516,7 +3564,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="36" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:29">
       <c r="A36" t="s">
         <v>36</v>
       </c>
@@ -3526,56 +3574,56 @@
       <c r="C36" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="D36" s="24">
-        <v>0</v>
-      </c>
-      <c r="E36" s="24">
-        <v>0</v>
-      </c>
-      <c r="F36" s="24">
-        <v>0</v>
-      </c>
-      <c r="G36" s="24">
-        <v>1</v>
-      </c>
-      <c r="H36" s="25">
-        <v>0</v>
-      </c>
-      <c r="I36" s="25">
-        <v>1</v>
-      </c>
-      <c r="J36" s="25">
-        <v>1</v>
-      </c>
-      <c r="K36" s="24">
-        <v>0</v>
-      </c>
-      <c r="L36" s="24">
-        <v>1</v>
-      </c>
-      <c r="M36" s="27"/>
-      <c r="N36" s="27"/>
-      <c r="O36" s="24">
-        <v>0</v>
-      </c>
-      <c r="P36" s="24">
-        <v>0</v>
-      </c>
-      <c r="Q36" s="24">
-        <v>0</v>
-      </c>
-      <c r="R36" s="24">
-        <v>0</v>
-      </c>
-      <c r="S36" s="27"/>
-      <c r="T36" s="27"/>
-      <c r="U36" s="24">
-        <v>1</v>
-      </c>
-      <c r="V36" s="25">
-        <v>1</v>
-      </c>
-      <c r="W36" s="26"/>
+      <c r="D36" s="22">
+        <v>0</v>
+      </c>
+      <c r="E36" s="22">
+        <v>0</v>
+      </c>
+      <c r="F36" s="22">
+        <v>0</v>
+      </c>
+      <c r="G36" s="22">
+        <v>1</v>
+      </c>
+      <c r="H36" s="23">
+        <v>0</v>
+      </c>
+      <c r="I36" s="23">
+        <v>1</v>
+      </c>
+      <c r="J36" s="23">
+        <v>1</v>
+      </c>
+      <c r="K36" s="22">
+        <v>0</v>
+      </c>
+      <c r="L36" s="22">
+        <v>1</v>
+      </c>
+      <c r="M36" s="25"/>
+      <c r="N36" s="25"/>
+      <c r="O36" s="22">
+        <v>0</v>
+      </c>
+      <c r="P36" s="22">
+        <v>0</v>
+      </c>
+      <c r="Q36" s="22">
+        <v>0</v>
+      </c>
+      <c r="R36" s="22">
+        <v>0</v>
+      </c>
+      <c r="S36" s="25"/>
+      <c r="T36" s="25"/>
+      <c r="U36" s="22">
+        <v>1</v>
+      </c>
+      <c r="V36" s="23">
+        <v>1</v>
+      </c>
+      <c r="W36" s="24"/>
       <c r="X36" s="7" t="s">
         <v>16</v>
       </c>
@@ -3592,7 +3640,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="37" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:29">
       <c r="A37" t="s">
         <v>35</v>
       </c>
@@ -3602,48 +3650,48 @@
       <c r="C37" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="D37" s="24">
-        <v>0</v>
-      </c>
-      <c r="E37" s="24">
-        <v>0</v>
-      </c>
-      <c r="F37" s="24">
-        <v>1</v>
-      </c>
-      <c r="G37" s="24">
-        <v>1</v>
-      </c>
-      <c r="H37" s="25">
-        <v>0</v>
-      </c>
-      <c r="I37" s="25">
-        <v>0</v>
-      </c>
-      <c r="J37" s="25">
-        <v>1</v>
-      </c>
-      <c r="K37" s="24">
-        <v>1</v>
-      </c>
-      <c r="L37" s="24">
-        <v>0</v>
-      </c>
-      <c r="M37" s="27"/>
-      <c r="N37" s="27"/>
-      <c r="O37" s="26"/>
-      <c r="P37" s="26"/>
-      <c r="Q37" s="26"/>
-      <c r="R37" s="26"/>
-      <c r="S37" s="25">
-        <v>0</v>
-      </c>
-      <c r="T37" s="25">
-        <v>1</v>
-      </c>
-      <c r="U37" s="26"/>
-      <c r="V37" s="27"/>
-      <c r="W37" s="26"/>
+      <c r="D37" s="22">
+        <v>0</v>
+      </c>
+      <c r="E37" s="22">
+        <v>0</v>
+      </c>
+      <c r="F37" s="22">
+        <v>1</v>
+      </c>
+      <c r="G37" s="22">
+        <v>1</v>
+      </c>
+      <c r="H37" s="23">
+        <v>0</v>
+      </c>
+      <c r="I37" s="23">
+        <v>0</v>
+      </c>
+      <c r="J37" s="23">
+        <v>1</v>
+      </c>
+      <c r="K37" s="22">
+        <v>1</v>
+      </c>
+      <c r="L37" s="22">
+        <v>0</v>
+      </c>
+      <c r="M37" s="25"/>
+      <c r="N37" s="25"/>
+      <c r="O37" s="24"/>
+      <c r="P37" s="24"/>
+      <c r="Q37" s="24"/>
+      <c r="R37" s="24"/>
+      <c r="S37" s="23">
+        <v>0</v>
+      </c>
+      <c r="T37" s="23">
+        <v>1</v>
+      </c>
+      <c r="U37" s="24"/>
+      <c r="V37" s="25"/>
+      <c r="W37" s="24"/>
       <c r="X37" s="7" t="s">
         <v>16</v>
       </c>
@@ -3660,7 +3708,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="38" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:29">
       <c r="A38" t="s">
         <v>38</v>
       </c>
@@ -3670,38 +3718,38 @@
       <c r="C38" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="D38" s="24">
-        <v>0</v>
-      </c>
-      <c r="E38" s="24">
-        <v>0</v>
-      </c>
-      <c r="F38" s="24">
-        <v>1</v>
-      </c>
-      <c r="G38" s="24">
-        <v>0</v>
-      </c>
-      <c r="H38" s="27"/>
-      <c r="I38" s="27"/>
-      <c r="J38" s="27"/>
-      <c r="K38" s="26"/>
-      <c r="L38" s="26"/>
-      <c r="M38" s="25">
-        <v>0</v>
-      </c>
-      <c r="N38" s="25">
-        <v>1</v>
-      </c>
-      <c r="O38" s="26"/>
-      <c r="P38" s="26"/>
-      <c r="Q38" s="26"/>
-      <c r="R38" s="26"/>
-      <c r="S38" s="27"/>
-      <c r="T38" s="27"/>
-      <c r="U38" s="26"/>
-      <c r="V38" s="27"/>
-      <c r="W38" s="26"/>
+      <c r="D38" s="22">
+        <v>0</v>
+      </c>
+      <c r="E38" s="22">
+        <v>0</v>
+      </c>
+      <c r="F38" s="22">
+        <v>1</v>
+      </c>
+      <c r="G38" s="22">
+        <v>0</v>
+      </c>
+      <c r="H38" s="25"/>
+      <c r="I38" s="25"/>
+      <c r="J38" s="25"/>
+      <c r="K38" s="24"/>
+      <c r="L38" s="24"/>
+      <c r="M38" s="23">
+        <v>0</v>
+      </c>
+      <c r="N38" s="23">
+        <v>1</v>
+      </c>
+      <c r="O38" s="24"/>
+      <c r="P38" s="24"/>
+      <c r="Q38" s="24"/>
+      <c r="R38" s="24"/>
+      <c r="S38" s="25"/>
+      <c r="T38" s="25"/>
+      <c r="U38" s="24"/>
+      <c r="V38" s="25"/>
+      <c r="W38" s="24"/>
       <c r="X38" s="7" t="s">
         <v>16</v>
       </c>
@@ -3718,7 +3766,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="39" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:29">
       <c r="A39" t="s">
         <v>63</v>
       </c>
@@ -3728,48 +3776,48 @@
       <c r="C39" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="D39" s="24">
-        <v>0</v>
-      </c>
-      <c r="E39" s="24">
-        <v>1</v>
-      </c>
-      <c r="F39" s="24">
-        <v>0</v>
-      </c>
-      <c r="G39" s="24">
-        <v>1</v>
-      </c>
-      <c r="H39" s="25">
-        <v>0</v>
-      </c>
-      <c r="I39" s="25">
-        <v>1</v>
-      </c>
-      <c r="J39" s="25">
-        <v>1</v>
-      </c>
-      <c r="K39" s="26"/>
-      <c r="L39" s="26"/>
-      <c r="M39" s="27"/>
-      <c r="N39" s="27"/>
-      <c r="O39" s="24">
-        <v>0</v>
-      </c>
-      <c r="P39" s="24">
-        <v>0</v>
-      </c>
-      <c r="Q39" s="24">
-        <v>0</v>
-      </c>
-      <c r="R39" s="24">
-        <v>0</v>
-      </c>
-      <c r="S39" s="27"/>
-      <c r="T39" s="27"/>
-      <c r="U39" s="26"/>
-      <c r="V39" s="27"/>
-      <c r="W39" s="26"/>
+      <c r="D39" s="22">
+        <v>0</v>
+      </c>
+      <c r="E39" s="22">
+        <v>1</v>
+      </c>
+      <c r="F39" s="22">
+        <v>0</v>
+      </c>
+      <c r="G39" s="22">
+        <v>1</v>
+      </c>
+      <c r="H39" s="23">
+        <v>0</v>
+      </c>
+      <c r="I39" s="23">
+        <v>1</v>
+      </c>
+      <c r="J39" s="23">
+        <v>1</v>
+      </c>
+      <c r="K39" s="24"/>
+      <c r="L39" s="24"/>
+      <c r="M39" s="25"/>
+      <c r="N39" s="25"/>
+      <c r="O39" s="22">
+        <v>0</v>
+      </c>
+      <c r="P39" s="22">
+        <v>0</v>
+      </c>
+      <c r="Q39" s="22">
+        <v>0</v>
+      </c>
+      <c r="R39" s="22">
+        <v>0</v>
+      </c>
+      <c r="S39" s="25"/>
+      <c r="T39" s="25"/>
+      <c r="U39" s="24"/>
+      <c r="V39" s="25"/>
+      <c r="W39" s="24"/>
       <c r="X39" s="7" t="s">
         <v>16</v>
       </c>
@@ -3786,7 +3834,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="40" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:29">
       <c r="A40" t="s">
         <v>42</v>
       </c>
@@ -3796,38 +3844,38 @@
       <c r="C40" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="D40" s="24">
-        <v>0</v>
-      </c>
-      <c r="E40" s="24">
-        <v>0</v>
-      </c>
-      <c r="F40" s="24">
-        <v>1</v>
-      </c>
-      <c r="G40" s="24">
-        <v>1</v>
-      </c>
-      <c r="H40" s="27"/>
-      <c r="I40" s="27"/>
-      <c r="J40" s="27"/>
-      <c r="K40" s="24">
-        <v>0</v>
-      </c>
-      <c r="L40" s="24">
-        <v>1</v>
-      </c>
-      <c r="M40" s="27"/>
-      <c r="N40" s="27"/>
-      <c r="O40" s="26"/>
-      <c r="P40" s="26"/>
-      <c r="Q40" s="26"/>
-      <c r="R40" s="26"/>
-      <c r="S40" s="27"/>
-      <c r="T40" s="27"/>
-      <c r="U40" s="26"/>
-      <c r="V40" s="27"/>
-      <c r="W40" s="26"/>
+      <c r="D40" s="22">
+        <v>0</v>
+      </c>
+      <c r="E40" s="22">
+        <v>0</v>
+      </c>
+      <c r="F40" s="22">
+        <v>1</v>
+      </c>
+      <c r="G40" s="22">
+        <v>1</v>
+      </c>
+      <c r="H40" s="25"/>
+      <c r="I40" s="25"/>
+      <c r="J40" s="25"/>
+      <c r="K40" s="22">
+        <v>0</v>
+      </c>
+      <c r="L40" s="22">
+        <v>1</v>
+      </c>
+      <c r="M40" s="25"/>
+      <c r="N40" s="25"/>
+      <c r="O40" s="24"/>
+      <c r="P40" s="24"/>
+      <c r="Q40" s="24"/>
+      <c r="R40" s="24"/>
+      <c r="S40" s="25"/>
+      <c r="T40" s="25"/>
+      <c r="U40" s="24"/>
+      <c r="V40" s="25"/>
+      <c r="W40" s="24"/>
       <c r="X40" s="7" t="s">
         <v>16</v>
       </c>
@@ -3844,7 +3892,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="41" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:29">
       <c r="A41" t="s">
         <v>22</v>
       </c>
@@ -3854,34 +3902,34 @@
       <c r="C41" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="D41" s="26"/>
-      <c r="E41" s="26"/>
-      <c r="F41" s="26"/>
-      <c r="G41" s="26"/>
-      <c r="H41" s="27"/>
-      <c r="I41" s="27"/>
-      <c r="J41" s="27"/>
-      <c r="K41" s="24">
-        <v>1</v>
-      </c>
-      <c r="L41" s="24">
-        <v>0</v>
-      </c>
-      <c r="M41" s="27"/>
-      <c r="N41" s="27"/>
-      <c r="O41" s="26"/>
-      <c r="P41" s="26"/>
-      <c r="Q41" s="26"/>
-      <c r="R41" s="26"/>
-      <c r="S41" s="25">
-        <v>0</v>
-      </c>
-      <c r="T41" s="25">
-        <v>1</v>
-      </c>
-      <c r="U41" s="26"/>
-      <c r="V41" s="27"/>
-      <c r="W41" s="26"/>
+      <c r="D41" s="24"/>
+      <c r="E41" s="24"/>
+      <c r="F41" s="24"/>
+      <c r="G41" s="24"/>
+      <c r="H41" s="25"/>
+      <c r="I41" s="25"/>
+      <c r="J41" s="25"/>
+      <c r="K41" s="22">
+        <v>1</v>
+      </c>
+      <c r="L41" s="22">
+        <v>0</v>
+      </c>
+      <c r="M41" s="25"/>
+      <c r="N41" s="25"/>
+      <c r="O41" s="24"/>
+      <c r="P41" s="24"/>
+      <c r="Q41" s="24"/>
+      <c r="R41" s="24"/>
+      <c r="S41" s="23">
+        <v>0</v>
+      </c>
+      <c r="T41" s="23">
+        <v>1</v>
+      </c>
+      <c r="U41" s="24"/>
+      <c r="V41" s="25"/>
+      <c r="W41" s="24"/>
       <c r="X41" s="7" t="s">
         <v>16</v>
       </c>
@@ -3898,10 +3946,10 @@
         <v>16</v>
       </c>
       <c r="AC41" s="18" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="42" spans="1:29" x14ac:dyDescent="0.3">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="42" spans="1:29">
       <c r="A42" t="s">
         <v>45</v>
       </c>
@@ -3911,38 +3959,38 @@
       <c r="C42" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="D42" s="24">
-        <v>0</v>
-      </c>
-      <c r="E42" s="24">
-        <v>0</v>
-      </c>
-      <c r="F42" s="24">
-        <v>1</v>
-      </c>
-      <c r="G42" s="24">
-        <v>0</v>
-      </c>
-      <c r="H42" s="27"/>
-      <c r="I42" s="27"/>
-      <c r="J42" s="27"/>
-      <c r="K42" s="24">
-        <v>0</v>
-      </c>
-      <c r="L42" s="24">
-        <v>1</v>
-      </c>
-      <c r="M42" s="27"/>
-      <c r="N42" s="27"/>
-      <c r="O42" s="26"/>
-      <c r="P42" s="26"/>
-      <c r="Q42" s="26"/>
-      <c r="R42" s="26"/>
-      <c r="S42" s="27"/>
-      <c r="T42" s="27"/>
-      <c r="U42" s="26"/>
-      <c r="V42" s="27"/>
-      <c r="W42" s="26"/>
+      <c r="D42" s="22">
+        <v>0</v>
+      </c>
+      <c r="E42" s="22">
+        <v>0</v>
+      </c>
+      <c r="F42" s="22">
+        <v>1</v>
+      </c>
+      <c r="G42" s="22">
+        <v>0</v>
+      </c>
+      <c r="H42" s="25"/>
+      <c r="I42" s="25"/>
+      <c r="J42" s="25"/>
+      <c r="K42" s="22">
+        <v>0</v>
+      </c>
+      <c r="L42" s="22">
+        <v>1</v>
+      </c>
+      <c r="M42" s="25"/>
+      <c r="N42" s="25"/>
+      <c r="O42" s="24"/>
+      <c r="P42" s="24"/>
+      <c r="Q42" s="24"/>
+      <c r="R42" s="24"/>
+      <c r="S42" s="25"/>
+      <c r="T42" s="25"/>
+      <c r="U42" s="24"/>
+      <c r="V42" s="25"/>
+      <c r="W42" s="24"/>
       <c r="X42" s="7" t="s">
         <v>16</v>
       </c>
@@ -3959,7 +4007,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="43" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:29">
       <c r="A43" t="s">
         <v>22</v>
       </c>
@@ -3969,34 +4017,34 @@
       <c r="C43" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="D43" s="26"/>
-      <c r="E43" s="26"/>
-      <c r="F43" s="26"/>
-      <c r="G43" s="26"/>
-      <c r="H43" s="27"/>
-      <c r="I43" s="27"/>
-      <c r="J43" s="27"/>
-      <c r="K43" s="24">
-        <v>1</v>
-      </c>
-      <c r="L43" s="24">
-        <v>0</v>
-      </c>
-      <c r="M43" s="27"/>
-      <c r="N43" s="27"/>
-      <c r="O43" s="26"/>
-      <c r="P43" s="26"/>
-      <c r="Q43" s="26"/>
-      <c r="R43" s="26"/>
-      <c r="S43" s="25">
-        <v>0</v>
-      </c>
-      <c r="T43" s="25">
-        <v>1</v>
-      </c>
-      <c r="U43" s="26"/>
-      <c r="V43" s="27"/>
-      <c r="W43" s="26"/>
+      <c r="D43" s="24"/>
+      <c r="E43" s="24"/>
+      <c r="F43" s="24"/>
+      <c r="G43" s="24"/>
+      <c r="H43" s="25"/>
+      <c r="I43" s="25"/>
+      <c r="J43" s="25"/>
+      <c r="K43" s="22">
+        <v>1</v>
+      </c>
+      <c r="L43" s="22">
+        <v>0</v>
+      </c>
+      <c r="M43" s="25"/>
+      <c r="N43" s="25"/>
+      <c r="O43" s="24"/>
+      <c r="P43" s="24"/>
+      <c r="Q43" s="24"/>
+      <c r="R43" s="24"/>
+      <c r="S43" s="23">
+        <v>0</v>
+      </c>
+      <c r="T43" s="23">
+        <v>1</v>
+      </c>
+      <c r="U43" s="24"/>
+      <c r="V43" s="25"/>
+      <c r="W43" s="24"/>
       <c r="X43" s="7" t="s">
         <v>16</v>
       </c>
@@ -4013,7 +4061,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="44" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:29">
       <c r="A44" t="s">
         <v>65</v>
       </c>
@@ -4021,40 +4069,40 @@
         <v>79</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="D44" s="24">
-        <v>0</v>
-      </c>
-      <c r="E44" s="24">
-        <v>0</v>
-      </c>
-      <c r="F44" s="24">
-        <v>1</v>
-      </c>
-      <c r="G44" s="24">
-        <v>0</v>
-      </c>
-      <c r="H44" s="27"/>
-      <c r="I44" s="27"/>
-      <c r="J44" s="27"/>
-      <c r="K44" s="26"/>
-      <c r="L44" s="26"/>
-      <c r="M44" s="25">
-        <v>1</v>
-      </c>
-      <c r="N44" s="25">
-        <v>1</v>
-      </c>
-      <c r="O44" s="26"/>
-      <c r="P44" s="26"/>
-      <c r="Q44" s="26"/>
-      <c r="R44" s="26"/>
-      <c r="S44" s="27"/>
-      <c r="T44" s="27"/>
-      <c r="U44" s="26"/>
-      <c r="V44" s="27"/>
-      <c r="W44" s="26"/>
+        <v>109</v>
+      </c>
+      <c r="D44" s="22">
+        <v>0</v>
+      </c>
+      <c r="E44" s="22">
+        <v>0</v>
+      </c>
+      <c r="F44" s="22">
+        <v>1</v>
+      </c>
+      <c r="G44" s="22">
+        <v>0</v>
+      </c>
+      <c r="H44" s="25"/>
+      <c r="I44" s="25"/>
+      <c r="J44" s="25"/>
+      <c r="K44" s="24"/>
+      <c r="L44" s="24"/>
+      <c r="M44" s="23">
+        <v>1</v>
+      </c>
+      <c r="N44" s="23">
+        <v>1</v>
+      </c>
+      <c r="O44" s="24"/>
+      <c r="P44" s="24"/>
+      <c r="Q44" s="24"/>
+      <c r="R44" s="24"/>
+      <c r="S44" s="25"/>
+      <c r="T44" s="25"/>
+      <c r="U44" s="24"/>
+      <c r="V44" s="25"/>
+      <c r="W44" s="24"/>
       <c r="X44" s="7" t="s">
         <v>17</v>
       </c>
@@ -4071,12 +4119,12 @@
         <v>16</v>
       </c>
       <c r="AC44" s="18" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="45" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.3">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="45" spans="1:29" s="9" customFormat="1">
       <c r="A45" s="9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B45" s="10"/>
       <c r="C45" s="10"/>
@@ -4107,15 +4155,15 @@
       <c r="AB45" s="12"/>
       <c r="AC45" s="19"/>
     </row>
-    <row r="46" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:29">
       <c r="A46" s="11" t="s">
         <v>80</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D46" s="8" t="s">
         <v>17</v>
@@ -4148,23 +4196,23 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:29">
       <c r="A47" s="13" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="AB47" s="16">
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:29">
       <c r="A48" s="13" t="s">
-        <v>83</v>
+        <v>165</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D48" s="8" t="s">
         <v>17</v>
@@ -4215,9 +4263,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:28">
       <c r="A49" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E49" s="4"/>
       <c r="F49" s="4"/>
@@ -4246,15 +4294,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:28">
       <c r="A50" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D50" s="8" t="s">
         <v>17</v>
@@ -4305,10 +4353,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:28">
       <c r="A51" s="13" t="s">
-        <v>87</v>
-      </c>
+        <v>86</v>
+      </c>
+      <c r="C51" s="28"/>
       <c r="E51" s="4"/>
       <c r="F51" s="4"/>
       <c r="G51" s="4"/>
@@ -4336,15 +4385,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:28">
       <c r="A52" s="13" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C52" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D52" s="8" t="s">
         <v>17</v>
@@ -4395,9 +4444,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:28">
       <c r="A53" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E53" s="4"/>
       <c r="F53" s="4"/>
@@ -4426,15 +4475,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:28">
       <c r="A54" s="11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C54" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D54" s="8" t="s">
         <v>17</v>
@@ -4485,23 +4534,23 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:28">
       <c r="A55" s="13" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="AB55" s="16">
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:28">
       <c r="A56" s="13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C56" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D56" s="8" t="s">
         <v>17</v>
@@ -4552,23 +4601,23 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:28">
       <c r="A57" s="11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AB57" s="16">
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:28">
       <c r="A58" s="11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B58" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C58" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D58" s="8" t="s">
         <v>17</v>
@@ -4619,23 +4668,23 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:28">
       <c r="A59" s="13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="AB59" s="16">
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:28">
       <c r="A60" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B60" s="6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C60" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D60" s="8" t="s">
         <v>17</v>
@@ -4686,23 +4735,23 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:28">
       <c r="A61" s="11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="AB61" s="16">
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:28">
       <c r="A62" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B62" s="6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C62" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D62" s="8" t="s">
         <v>17</v>
@@ -4753,20 +4802,20 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:28">
       <c r="A63" s="13" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AB63" s="16">
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:28">
       <c r="A64" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B64" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C64" s="5">
         <v>0</v>
@@ -4824,9 +4873,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:29" s="9" customFormat="1">
       <c r="A65" s="9" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B65" s="10"/>
       <c r="C65" s="10"/>
@@ -4857,29 +4906,29 @@
       <c r="AB65" s="12"/>
       <c r="AC65" s="19"/>
     </row>
-    <row r="66" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:29">
       <c r="B66" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="C66" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="C66" s="7" t="s">
+      <c r="X66" s="2">
+        <v>1</v>
+      </c>
+      <c r="Y66" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z66" s="2">
+        <v>1</v>
+      </c>
+      <c r="AB66" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:29">
+      <c r="A67" s="11" t="s">
         <v>124</v>
-      </c>
-      <c r="X66" s="2">
-        <v>1</v>
-      </c>
-      <c r="Y66" s="2">
-        <v>0</v>
-      </c>
-      <c r="Z66" s="2">
-        <v>1</v>
-      </c>
-      <c r="AB66" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A67" s="11" t="s">
-        <v>125</v>
       </c>
       <c r="E67" s="14"/>
       <c r="F67" s="14"/>
@@ -4908,23 +4957,65 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:29">
       <c r="A68" s="11" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B68" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C68" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
+      </c>
+      <c r="D68" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E68" s="3">
+        <v>0</v>
+      </c>
+      <c r="F68" s="3">
+        <v>0</v>
+      </c>
+      <c r="G68" s="3">
+        <v>1</v>
+      </c>
+      <c r="H68" s="2">
+        <v>0</v>
+      </c>
+      <c r="I68" s="2">
+        <v>1</v>
+      </c>
+      <c r="J68" s="2">
+        <v>1</v>
+      </c>
+      <c r="O68" s="3">
+        <v>0</v>
+      </c>
+      <c r="P68" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q68" s="3">
+        <v>0</v>
+      </c>
+      <c r="R68" s="3">
+        <v>0</v>
+      </c>
+      <c r="U68" s="3">
+        <v>1</v>
+      </c>
+      <c r="V68" s="2">
+        <v>1</v>
+      </c>
+      <c r="W68" s="3">
+        <v>1</v>
       </c>
       <c r="AB68" s="16">
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:29">
       <c r="A69" s="13" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E69" s="14"/>
       <c r="F69" s="14"/>
@@ -4953,210 +5044,489 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:29">
       <c r="A70" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="B70" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="C70" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="D70" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E70" s="3">
+        <v>0</v>
+      </c>
+      <c r="F70" s="3">
+        <v>0</v>
+      </c>
+      <c r="G70" s="3">
+        <v>1</v>
+      </c>
+      <c r="H70" s="2">
+        <v>0</v>
+      </c>
+      <c r="I70" s="2">
+        <v>1</v>
+      </c>
+      <c r="J70" s="2">
+        <v>1</v>
+      </c>
+      <c r="O70" s="3">
+        <v>0</v>
+      </c>
+      <c r="P70" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q70" s="3">
+        <v>0</v>
+      </c>
+      <c r="R70" s="3">
+        <v>1</v>
+      </c>
+      <c r="U70" s="3">
+        <v>1</v>
+      </c>
+      <c r="W70" s="3">
+        <v>1</v>
+      </c>
+      <c r="AB70" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:29">
+      <c r="A71" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="AB71" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:29">
+      <c r="A72" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="B72" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="C72" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="H72" s="2">
+        <v>0</v>
+      </c>
+      <c r="I72" s="2">
+        <v>1</v>
+      </c>
+      <c r="J72" s="2">
+        <v>1</v>
+      </c>
+      <c r="O72" s="3">
+        <v>1</v>
+      </c>
+      <c r="P72" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q72" s="3">
+        <v>1</v>
+      </c>
+      <c r="R72" s="3">
+        <v>1</v>
+      </c>
+      <c r="W72" s="3">
+        <v>1</v>
+      </c>
+      <c r="AB72" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:29">
+      <c r="A73" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="AB73" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:29">
+      <c r="A74" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="B74" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="C74" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="D74" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E74" s="3">
+        <v>0</v>
+      </c>
+      <c r="F74" s="3">
+        <v>0</v>
+      </c>
+      <c r="G74" s="3">
+        <v>1</v>
+      </c>
+      <c r="H74" s="2">
+        <v>0</v>
+      </c>
+      <c r="I74" s="2">
+        <v>1</v>
+      </c>
+      <c r="J74" s="2">
+        <v>1</v>
+      </c>
+      <c r="O74" s="3">
+        <v>0</v>
+      </c>
+      <c r="P74" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q74" s="3">
+        <v>0</v>
+      </c>
+      <c r="R74" s="3">
+        <v>1</v>
+      </c>
+      <c r="W74" s="3">
+        <v>1</v>
+      </c>
+      <c r="AB74" s="16">
+        <v>0</v>
+      </c>
+      <c r="AC74" s="18" t="s">
         <v>133</v>
       </c>
-      <c r="B70" s="6" t="s">
-        <v>145</v>
-      </c>
-      <c r="C70" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="AB70" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A71" s="11" t="s">
-        <v>127</v>
-      </c>
-      <c r="AB71" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A72" s="11" t="s">
-        <v>128</v>
-      </c>
-      <c r="B72" s="6" t="s">
+    </row>
+    <row r="75" spans="1:29">
+      <c r="A75" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="AB75" s="16">
+        <v>0</v>
+      </c>
+      <c r="AC75" s="18" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="76" spans="1:29">
+      <c r="A76" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="B76" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="C76" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="D76" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E76" s="3">
+        <v>0</v>
+      </c>
+      <c r="F76" s="3">
+        <v>0</v>
+      </c>
+      <c r="G76" s="3">
+        <v>1</v>
+      </c>
+      <c r="H76" s="2">
+        <v>0</v>
+      </c>
+      <c r="I76" s="2">
+        <v>1</v>
+      </c>
+      <c r="J76" s="2">
+        <v>1</v>
+      </c>
+      <c r="O76" s="3">
+        <v>0</v>
+      </c>
+      <c r="P76" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q76" s="3">
+        <v>1</v>
+      </c>
+      <c r="R76" s="3">
+        <v>0</v>
+      </c>
+      <c r="W76" s="3">
+        <v>1</v>
+      </c>
+      <c r="AB76" s="16">
+        <v>0</v>
+      </c>
+      <c r="AC76" s="18" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="77" spans="1:29">
+      <c r="A77" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="AB77" s="16">
+        <v>0</v>
+      </c>
+      <c r="AC77" s="18" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="78" spans="1:29">
+      <c r="A78" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="B78" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="C78" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="D78" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E78" s="3">
+        <v>0</v>
+      </c>
+      <c r="F78" s="3">
+        <v>0</v>
+      </c>
+      <c r="G78" s="3">
+        <v>1</v>
+      </c>
+      <c r="H78" s="2">
+        <v>0</v>
+      </c>
+      <c r="I78" s="2">
+        <v>1</v>
+      </c>
+      <c r="J78" s="2">
+        <v>1</v>
+      </c>
+      <c r="O78" s="3">
+        <v>0</v>
+      </c>
+      <c r="P78" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q78" s="3">
+        <v>1</v>
+      </c>
+      <c r="R78" s="3">
+        <v>1</v>
+      </c>
+      <c r="W78" s="3">
+        <v>1</v>
+      </c>
+      <c r="AB78" s="16">
+        <v>0</v>
+      </c>
+      <c r="AC78" s="18" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="79" spans="1:29">
+      <c r="A79" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="AB79" s="16">
+        <v>0</v>
+      </c>
+      <c r="AC79" s="18" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="80" spans="1:29">
+      <c r="A80" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="B80" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="C72" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="AB72" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A73" s="13" t="s">
-        <v>129</v>
-      </c>
-      <c r="AB73" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A74" s="13" t="s">
-        <v>134</v>
-      </c>
-      <c r="B74" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="C74" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="AB74" s="16">
-        <v>0</v>
-      </c>
-      <c r="AC74" s="18" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="75" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A75" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="AB75" s="16">
-        <v>0</v>
-      </c>
-      <c r="AC75" s="18" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="76" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A76" s="11" t="s">
-        <v>138</v>
-      </c>
-      <c r="B76" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="C76" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="AB76" s="16">
-        <v>0</v>
-      </c>
-      <c r="AC76" s="18" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="77" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A77" s="13" t="s">
-        <v>136</v>
-      </c>
-      <c r="AB77" s="16">
-        <v>0</v>
-      </c>
-      <c r="AC77" s="18" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="78" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A78" s="13" t="s">
-        <v>137</v>
-      </c>
-      <c r="B78" s="6" t="s">
+      <c r="C80" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="D80" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E80" s="3">
+        <v>0</v>
+      </c>
+      <c r="F80" s="3">
+        <v>0</v>
+      </c>
+      <c r="G80" s="3">
+        <v>1</v>
+      </c>
+      <c r="H80" s="2">
+        <v>0</v>
+      </c>
+      <c r="I80" s="2">
+        <v>1</v>
+      </c>
+      <c r="J80" s="2">
+        <v>1</v>
+      </c>
+      <c r="O80" s="3">
+        <v>1</v>
+      </c>
+      <c r="P80" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q80" s="3">
+        <v>0</v>
+      </c>
+      <c r="R80" s="3">
+        <v>0</v>
+      </c>
+      <c r="W80" s="3">
+        <v>1</v>
+      </c>
+      <c r="AB80" s="16">
+        <v>0</v>
+      </c>
+      <c r="AC80" s="18" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="81" spans="1:29">
+      <c r="A81" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="AB81" s="16">
+        <v>0</v>
+      </c>
+      <c r="AC81" s="18" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="82" spans="1:29">
+      <c r="A82" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="B82" s="6" t="s">
         <v>149</v>
       </c>
-      <c r="C78" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="AB78" s="16">
-        <v>0</v>
-      </c>
-      <c r="AC78" s="18" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="79" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A79" s="11" t="s">
-        <v>139</v>
-      </c>
-      <c r="AB79" s="16">
-        <v>0</v>
-      </c>
-      <c r="AC79" s="18" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="80" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A80" s="11" t="s">
-        <v>140</v>
-      </c>
-      <c r="B80" s="6" t="s">
+      <c r="C82" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="D82" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E82" s="3">
+        <v>0</v>
+      </c>
+      <c r="F82" s="3">
+        <v>0</v>
+      </c>
+      <c r="G82" s="3">
+        <v>1</v>
+      </c>
+      <c r="H82" s="2">
+        <v>0</v>
+      </c>
+      <c r="I82" s="2">
+        <v>1</v>
+      </c>
+      <c r="J82" s="2">
+        <v>1</v>
+      </c>
+      <c r="O82" s="3">
+        <v>1</v>
+      </c>
+      <c r="P82" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q82" s="3">
+        <v>0</v>
+      </c>
+      <c r="R82" s="3">
+        <v>1</v>
+      </c>
+      <c r="W82" s="3">
+        <v>1</v>
+      </c>
+      <c r="AB82" s="16">
+        <v>0</v>
+      </c>
+      <c r="AC82" s="18" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="83" spans="1:29">
+      <c r="A83" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="AB83" s="16">
+        <v>0</v>
+      </c>
+      <c r="AC83" s="18" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="84" spans="1:29">
+      <c r="A84" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="B84" s="6" t="s">
         <v>150</v>
       </c>
-      <c r="C80" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="AB80" s="16">
-        <v>0</v>
-      </c>
-      <c r="AC80" s="18" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="81" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A81" s="13" t="s">
-        <v>141</v>
-      </c>
-      <c r="AB81" s="16">
-        <v>0</v>
-      </c>
-      <c r="AC81" s="18" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="82" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A82" s="13" t="s">
-        <v>142</v>
-      </c>
-      <c r="B82" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="C82" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="AB82" s="16">
-        <v>0</v>
-      </c>
-      <c r="AC82" s="18" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="83" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A83" s="11" t="s">
-        <v>143</v>
-      </c>
-      <c r="AB83" s="16">
-        <v>0</v>
-      </c>
-      <c r="AC83" s="18" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="84" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A84" s="11" t="s">
-        <v>144</v>
-      </c>
-      <c r="B84" s="6" t="s">
-        <v>152</v>
-      </c>
       <c r="C84" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
+      </c>
+      <c r="D84" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E84" s="3">
+        <v>0</v>
+      </c>
+      <c r="F84" s="3">
+        <v>0</v>
+      </c>
+      <c r="G84" s="3">
+        <v>1</v>
+      </c>
+      <c r="H84" s="2">
+        <v>0</v>
+      </c>
+      <c r="I84" s="2">
+        <v>1</v>
+      </c>
+      <c r="J84" s="2">
+        <v>1</v>
+      </c>
+      <c r="O84" s="3">
+        <v>1</v>
+      </c>
+      <c r="P84" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q84" s="3">
+        <v>1</v>
+      </c>
+      <c r="R84" s="3">
+        <v>0</v>
+      </c>
+      <c r="W84" s="3">
+        <v>1</v>
       </c>
       <c r="AB84" s="16">
         <v>0</v>
       </c>
       <c r="AC84" s="18" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="85" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.3">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="85" spans="1:29" s="9" customFormat="1">
       <c r="A85" s="9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B85" s="10"/>
       <c r="C85" s="10"/>
@@ -5187,53 +5557,98 @@
       <c r="AB85" s="12"/>
       <c r="AC85" s="19"/>
     </row>
-    <row r="86" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:29">
       <c r="A86" t="s">
+        <v>100</v>
+      </c>
+      <c r="B86" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="C86" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="D86" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E86" s="3">
+        <v>0</v>
+      </c>
+      <c r="F86" s="3">
+        <v>1</v>
+      </c>
+      <c r="G86" s="3">
+        <v>1</v>
+      </c>
+      <c r="K86" s="3">
+        <v>1</v>
+      </c>
+      <c r="L86" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA86" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB86" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:29">
+      <c r="A87" t="s">
         <v>101</v>
       </c>
-      <c r="B86" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="C86" s="7" t="s">
+      <c r="B87" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="C87" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="S87" s="2">
+        <v>1</v>
+      </c>
+      <c r="T87" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA87" s="3">
+        <v>1</v>
+      </c>
+      <c r="AB87" s="16">
+        <v>0</v>
+      </c>
+      <c r="AC87" s="18" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="88" spans="1:29">
+      <c r="A88" t="s">
+        <v>102</v>
+      </c>
+      <c r="B88" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="AA86" s="3">
-        <v>0</v>
-      </c>
-      <c r="AB86" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="87" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A87" t="s">
-        <v>102</v>
-      </c>
-      <c r="B87" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="C87" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="AA87" s="3">
-        <v>1</v>
-      </c>
-      <c r="AB87" s="16">
-        <v>0</v>
-      </c>
-      <c r="AC87" s="18" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="88" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A88" t="s">
-        <v>103</v>
-      </c>
-      <c r="B88" s="6" t="s">
-        <v>121</v>
-      </c>
       <c r="C88" s="7" t="s">
         <v>16</v>
       </c>
+      <c r="D88" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E88" s="3">
+        <v>0</v>
+      </c>
+      <c r="F88" s="3">
+        <v>1</v>
+      </c>
+      <c r="G88" s="3">
+        <v>1</v>
+      </c>
+      <c r="H88" s="2">
+        <v>1</v>
+      </c>
+      <c r="I88" s="2">
+        <v>0</v>
+      </c>
+      <c r="J88" s="2">
+        <v>1</v>
+      </c>
       <c r="AA88" s="3">
         <v>1</v>
       </c>
@@ -5241,9 +5656,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:29" s="9" customFormat="1">
       <c r="A89" s="9" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B89" s="10"/>
       <c r="C89" s="10"/>
@@ -5274,38 +5689,38 @@
       <c r="AB89" s="12"/>
       <c r="AC89" s="19"/>
     </row>
-    <row r="90" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:29">
       <c r="A90" s="11" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="AB90" s="16">
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:29">
       <c r="A91" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="AB91" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:29">
+      <c r="A92" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="93" spans="1:29">
+      <c r="B93" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="AB93" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:29" s="9" customFormat="1">
+      <c r="A94" s="9" t="s">
         <v>158</v>
-      </c>
-      <c r="AB91" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="92" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A92" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="93" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="B93" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="AB93" s="16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="94" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A94" s="9" t="s">
-        <v>160</v>
       </c>
       <c r="B94" s="10"/>
       <c r="C94" s="10"/>
@@ -5336,27 +5751,99 @@
       <c r="AB94" s="12"/>
       <c r="AC94" s="19"/>
     </row>
-    <row r="95" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A95" t="s">
+    <row r="95" spans="1:29">
+      <c r="A95" s="30" t="s">
+        <v>159</v>
+      </c>
+      <c r="D95" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E95" s="3">
+        <v>1</v>
+      </c>
+      <c r="F95" s="3">
+        <v>1</v>
+      </c>
+      <c r="G95" s="3">
+        <v>1</v>
+      </c>
+      <c r="M95" s="2">
+        <v>0</v>
+      </c>
+      <c r="N95" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:29">
+      <c r="A96" t="s">
+        <v>160</v>
+      </c>
+      <c r="D96" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E96" s="3">
+        <v>0</v>
+      </c>
+      <c r="F96" s="3">
+        <v>0</v>
+      </c>
+      <c r="G96" s="3">
+        <v>1</v>
+      </c>
+      <c r="H96" s="2">
+        <v>0</v>
+      </c>
+      <c r="I96" s="2">
+        <v>1</v>
+      </c>
+      <c r="J96" s="2">
+        <v>1</v>
+      </c>
+      <c r="O96" s="3">
+        <v>0</v>
+      </c>
+      <c r="P96" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q96" s="3">
+        <v>0</v>
+      </c>
+      <c r="R96" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:29">
+      <c r="A97" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="96" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A96" t="s">
+      <c r="C97" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D97" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E97" s="3">
+        <v>0</v>
+      </c>
+      <c r="F97" s="3">
+        <v>1</v>
+      </c>
+      <c r="G97" s="3">
+        <v>1</v>
+      </c>
+      <c r="H97" s="2">
+        <v>0</v>
+      </c>
+      <c r="I97" s="2">
+        <v>0</v>
+      </c>
+      <c r="J97" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:29" s="9" customFormat="1">
+      <c r="A98" s="9" t="s">
         <v>162</v>
-      </c>
-    </row>
-    <row r="97" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A97" t="s">
-        <v>163</v>
-      </c>
-      <c r="C97" s="7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="98" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A98" s="9" t="s">
-        <v>164</v>
       </c>
       <c r="B98" s="10"/>
       <c r="C98" s="10"/>
@@ -5387,13 +5874,19 @@
       <c r="AB98" s="12"/>
       <c r="AC98" s="19"/>
     </row>
-    <row r="99" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:29">
       <c r="A99" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="D2:G2"/>
+    <mergeCell ref="O2:R2"/>
+    <mergeCell ref="S2:T2"/>
+    <mergeCell ref="X2:Z2"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="K2:L2"/>
     <mergeCell ref="D1:G1"/>
     <mergeCell ref="M1:N1"/>
     <mergeCell ref="X1:Z1"/>
@@ -5401,12 +5894,6 @@
     <mergeCell ref="O1:R1"/>
     <mergeCell ref="K1:L1"/>
     <mergeCell ref="H1:J1"/>
-    <mergeCell ref="D2:G2"/>
-    <mergeCell ref="O2:R2"/>
-    <mergeCell ref="S2:T2"/>
-    <mergeCell ref="X2:Z2"/>
-    <mergeCell ref="H2:J2"/>
-    <mergeCell ref="K2:L2"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added ORing for ALU operations for 1 operand
</commit_message>
<xml_diff>
--- a/Microroutines.xlsx
+++ b/Microroutines.xlsx
@@ -1,17 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study\Third Year\arch\PDP11\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{300B9134-D0A6-4D97-A622-1F19B9975E31}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13710" yWindow="3735" windowWidth="9330" windowHeight="8610"/>
+    <workbookView xWindow="13716" yWindow="3732" windowWidth="9324" windowHeight="8616" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -520,7 +526,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -535,7 +541,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -545,7 +551,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF9C0006"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -556,59 +562,59 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="8">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -657,7 +663,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
@@ -726,12 +732,6 @@
     <xf numFmtId="2" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="49" fontId="7" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -739,6 +739,15 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Accent2" xfId="4" builtinId="33"/>
@@ -1015,54 +1024,54 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AC99"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="82" zoomScaleNormal="82" zoomScaleSheetLayoutView="86" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E27" sqref="E27"/>
+      <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A102" sqref="A102"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="47.125" customWidth="1"/>
-    <col min="2" max="2" width="8.75" style="6" customWidth="1"/>
-    <col min="3" max="3" width="7.375" style="7" customWidth="1"/>
-    <col min="4" max="4" width="2.625" style="8" customWidth="1"/>
+    <col min="1" max="1" width="47.109375" customWidth="1"/>
+    <col min="2" max="2" width="8.77734375" style="6" customWidth="1"/>
+    <col min="3" max="3" width="7.33203125" style="7" customWidth="1"/>
+    <col min="4" max="4" width="2.6640625" style="8" customWidth="1"/>
     <col min="5" max="5" width="3" style="3" customWidth="1"/>
-    <col min="6" max="6" width="3.125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="3.75" style="3" customWidth="1"/>
+    <col min="6" max="6" width="3.109375" style="3" customWidth="1"/>
+    <col min="7" max="7" width="3.77734375" style="3" customWidth="1"/>
     <col min="8" max="8" width="3" style="2" customWidth="1"/>
-    <col min="9" max="9" width="3.5" style="2" customWidth="1"/>
-    <col min="10" max="10" width="2.875" style="2" customWidth="1"/>
-    <col min="11" max="11" width="3.25" style="3" customWidth="1"/>
-    <col min="12" max="12" width="3.625" style="3" customWidth="1"/>
-    <col min="13" max="13" width="3.625" style="2" customWidth="1"/>
-    <col min="14" max="14" width="3.125" style="2" customWidth="1"/>
-    <col min="15" max="16" width="3.625" style="3" customWidth="1"/>
-    <col min="17" max="17" width="3.5" style="3" customWidth="1"/>
-    <col min="18" max="18" width="3.375" style="3" customWidth="1"/>
-    <col min="19" max="19" width="3.75" style="2" customWidth="1"/>
-    <col min="20" max="20" width="3.5" style="2" customWidth="1"/>
+    <col min="9" max="9" width="3.44140625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="2.88671875" style="2" customWidth="1"/>
+    <col min="11" max="11" width="3.21875" style="3" customWidth="1"/>
+    <col min="12" max="12" width="3.6640625" style="3" customWidth="1"/>
+    <col min="13" max="13" width="3.6640625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="3.109375" style="2" customWidth="1"/>
+    <col min="15" max="16" width="3.6640625" style="3" customWidth="1"/>
+    <col min="17" max="17" width="3.44140625" style="3" customWidth="1"/>
+    <col min="18" max="18" width="3.33203125" style="3" customWidth="1"/>
+    <col min="19" max="19" width="3.77734375" style="2" customWidth="1"/>
+    <col min="20" max="20" width="3.44140625" style="2" customWidth="1"/>
     <col min="21" max="21" width="3" style="3" customWidth="1"/>
-    <col min="22" max="22" width="3.125" style="2" customWidth="1"/>
-    <col min="23" max="23" width="3.5" style="3" customWidth="1"/>
+    <col min="22" max="22" width="3.109375" style="2" customWidth="1"/>
+    <col min="23" max="23" width="3.44140625" style="3" customWidth="1"/>
     <col min="24" max="24" width="4" style="2" customWidth="1"/>
-    <col min="25" max="25" width="3.5" style="2" customWidth="1"/>
-    <col min="26" max="26" width="3.625" style="2" customWidth="1"/>
-    <col min="27" max="27" width="3.5" style="3" customWidth="1"/>
-    <col min="28" max="28" width="3.5" style="16" customWidth="1"/>
-    <col min="29" max="29" width="30.5" style="18" customWidth="1"/>
+    <col min="25" max="25" width="3.44140625" style="2" customWidth="1"/>
+    <col min="26" max="26" width="3.6640625" style="2" customWidth="1"/>
+    <col min="27" max="27" width="3.44140625" style="3" customWidth="1"/>
+    <col min="28" max="28" width="3.44140625" style="16" customWidth="1"/>
+    <col min="29" max="29" width="30.44140625" style="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1072,35 +1081,35 @@
       <c r="C1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="D1" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="27" t="s">
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="30" t="s">
         <v>52</v>
       </c>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="26" t="s">
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="29" t="s">
         <v>51</v>
       </c>
-      <c r="L1" s="26"/>
-      <c r="M1" s="27" t="s">
+      <c r="L1" s="29"/>
+      <c r="M1" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="N1" s="27"/>
-      <c r="O1" s="26" t="s">
+      <c r="N1" s="30"/>
+      <c r="O1" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="P1" s="26"/>
-      <c r="Q1" s="26"/>
-      <c r="R1" s="26"/>
-      <c r="S1" s="27" t="s">
+      <c r="P1" s="29"/>
+      <c r="Q1" s="29"/>
+      <c r="R1" s="29"/>
+      <c r="S1" s="30" t="s">
         <v>54</v>
       </c>
-      <c r="T1" s="27"/>
+      <c r="T1" s="30"/>
       <c r="U1" s="3" t="s">
         <v>2</v>
       </c>
@@ -1110,11 +1119,11 @@
       <c r="W1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="X1" s="27" t="s">
+      <c r="X1" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="Y1" s="27"/>
-      <c r="Z1" s="27"/>
+      <c r="Y1" s="30"/>
+      <c r="Z1" s="30"/>
       <c r="AA1" s="3" t="s">
         <v>5</v>
       </c>
@@ -1125,27 +1134,27 @@
         <v>128</v>
       </c>
     </row>
-    <row r="2" spans="1:29">
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
-      <c r="J2" s="27"/>
-      <c r="K2" s="26"/>
-      <c r="L2" s="26"/>
-      <c r="O2" s="26"/>
-      <c r="P2" s="26"/>
-      <c r="Q2" s="26"/>
-      <c r="R2" s="26"/>
-      <c r="S2" s="27"/>
-      <c r="T2" s="27"/>
-      <c r="X2" s="27"/>
-      <c r="Y2" s="27"/>
-      <c r="Z2" s="27"/>
-    </row>
-    <row r="3" spans="1:29" s="9" customFormat="1">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="29"/>
+      <c r="L2" s="29"/>
+      <c r="O2" s="29"/>
+      <c r="P2" s="29"/>
+      <c r="Q2" s="29"/>
+      <c r="R2" s="29"/>
+      <c r="S2" s="30"/>
+      <c r="T2" s="30"/>
+      <c r="X2" s="30"/>
+      <c r="Y2" s="30"/>
+      <c r="Z2" s="30"/>
+    </row>
+    <row r="3" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
         <v>82</v>
       </c>
@@ -1178,7 +1187,7 @@
       <c r="AB3" s="12"/>
       <c r="AC3" s="19"/>
     </row>
-    <row r="4" spans="1:29" s="1" customFormat="1">
+    <row r="4" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1265,7 +1274,7 @@
       </c>
       <c r="AC4" s="20"/>
     </row>
-    <row r="5" spans="1:29" s="1" customFormat="1">
+    <row r="5" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -1352,7 +1361,7 @@
       </c>
       <c r="AC5" s="20"/>
     </row>
-    <row r="6" spans="1:29" s="1" customFormat="1">
+    <row r="6" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -1439,7 +1448,7 @@
       </c>
       <c r="AC6" s="20"/>
     </row>
-    <row r="7" spans="1:29" s="1" customFormat="1">
+    <row r="7" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1526,7 +1535,7 @@
       </c>
       <c r="AC7" s="20"/>
     </row>
-    <row r="8" spans="1:29" s="9" customFormat="1">
+    <row r="8" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
         <v>81</v>
       </c>
@@ -1559,12 +1568,12 @@
       <c r="AB8" s="12"/>
       <c r="AC8" s="19"/>
     </row>
-    <row r="9" spans="1:29">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:29">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -1650,7 +1659,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:29">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -1736,14 +1745,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:29">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>22</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="29" t="s">
+      <c r="C12" s="27" t="s">
         <v>47</v>
       </c>
       <c r="D12" s="8" t="s">
@@ -1822,7 +1831,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:29">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>26</v>
       </c>
@@ -1908,7 +1917,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:29">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>23</v>
       </c>
@@ -1994,7 +2003,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:29">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>29</v>
       </c>
@@ -2080,7 +2089,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:29">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>31</v>
       </c>
@@ -2166,7 +2175,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:29">
+    <row r="17" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>22</v>
       </c>
@@ -2252,7 +2261,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:29">
+    <row r="18" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>36</v>
       </c>
@@ -2338,7 +2347,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:29">
+    <row r="19" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>35</v>
       </c>
@@ -2424,7 +2433,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:29">
+    <row r="20" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>38</v>
       </c>
@@ -2510,7 +2519,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:29">
+    <row r="21" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>40</v>
       </c>
@@ -2596,7 +2605,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:29">
+    <row r="22" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>42</v>
       </c>
@@ -2682,7 +2691,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:29">
+    <row r="23" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -2771,7 +2780,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="24" spans="1:29">
+    <row r="24" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>45</v>
       </c>
@@ -2857,7 +2866,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:29">
+    <row r="25" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>22</v>
       </c>
@@ -2943,7 +2952,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:29">
+    <row r="26" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>48</v>
       </c>
@@ -3029,7 +3038,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:29" s="9" customFormat="1">
+    <row r="27" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="9" t="s">
         <v>107</v>
       </c>
@@ -3062,7 +3071,7 @@
       <c r="AB27" s="10"/>
       <c r="AC27" s="19"/>
     </row>
-    <row r="28" spans="1:29">
+    <row r="28" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>64</v>
       </c>
@@ -3120,7 +3129,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="29" spans="1:29">
+    <row r="29" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>57</v>
       </c>
@@ -3178,14 +3187,14 @@
         <v>16</v>
       </c>
     </row>
-    <row r="30" spans="1:29">
+    <row r="30" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>22</v>
       </c>
       <c r="B30" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="29" t="s">
+      <c r="C30" s="27" t="s">
         <v>79</v>
       </c>
       <c r="D30" s="24"/>
@@ -3232,7 +3241,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:29">
+    <row r="31" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>59</v>
       </c>
@@ -3308,7 +3317,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="32" spans="1:29">
+    <row r="32" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>60</v>
       </c>
@@ -3376,7 +3385,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="33" spans="1:29">
+    <row r="33" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>61</v>
       </c>
@@ -3446,7 +3455,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="34" spans="1:29">
+    <row r="34" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>62</v>
       </c>
@@ -3510,7 +3519,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="35" spans="1:29">
+    <row r="35" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>22</v>
       </c>
@@ -3564,7 +3573,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="36" spans="1:29">
+    <row r="36" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>36</v>
       </c>
@@ -3640,7 +3649,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="37" spans="1:29">
+    <row r="37" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>35</v>
       </c>
@@ -3708,7 +3717,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="38" spans="1:29">
+    <row r="38" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>38</v>
       </c>
@@ -3766,7 +3775,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="39" spans="1:29">
+    <row r="39" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>63</v>
       </c>
@@ -3834,7 +3843,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="40" spans="1:29">
+    <row r="40" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>42</v>
       </c>
@@ -3892,7 +3901,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="41" spans="1:29">
+    <row r="41" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>22</v>
       </c>
@@ -3949,7 +3958,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="42" spans="1:29">
+    <row r="42" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>45</v>
       </c>
@@ -4007,7 +4016,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="43" spans="1:29">
+    <row r="43" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>22</v>
       </c>
@@ -4061,7 +4070,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="44" spans="1:29">
+    <row r="44" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>65</v>
       </c>
@@ -4122,7 +4131,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="45" spans="1:29" s="9" customFormat="1">
+    <row r="45" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A45" s="9" t="s">
         <v>104</v>
       </c>
@@ -4155,7 +4164,7 @@
       <c r="AB45" s="12"/>
       <c r="AC45" s="19"/>
     </row>
-    <row r="46" spans="1:29">
+    <row r="46" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A46" s="11" t="s">
         <v>80</v>
       </c>
@@ -4196,7 +4205,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:29">
+    <row r="47" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A47" s="13" t="s">
         <v>84</v>
       </c>
@@ -4204,7 +4213,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:29">
+    <row r="48" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A48" s="13" t="s">
         <v>165</v>
       </c>
@@ -4263,7 +4272,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:28">
+    <row r="49" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A49" s="11" t="s">
         <v>85</v>
       </c>
@@ -4294,7 +4303,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:28">
+    <row r="50" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A50" s="11" t="s">
         <v>83</v>
       </c>
@@ -4353,11 +4362,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:28">
+    <row r="51" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A51" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="C51" s="28"/>
+      <c r="C51" s="26"/>
       <c r="E51" s="4"/>
       <c r="F51" s="4"/>
       <c r="G51" s="4"/>
@@ -4385,7 +4394,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:28">
+    <row r="52" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A52" s="13" t="s">
         <v>89</v>
       </c>
@@ -4444,7 +4453,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:28">
+    <row r="53" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A53" s="11" t="s">
         <v>87</v>
       </c>
@@ -4475,7 +4484,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:28">
+    <row r="54" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A54" s="11" t="s">
         <v>93</v>
       </c>
@@ -4534,7 +4543,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:28">
+    <row r="55" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A55" s="13" t="s">
         <v>88</v>
       </c>
@@ -4542,7 +4551,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:28">
+    <row r="56" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A56" s="13" t="s">
         <v>94</v>
       </c>
@@ -4601,7 +4610,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:28">
+    <row r="57" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A57" s="11" t="s">
         <v>90</v>
       </c>
@@ -4609,7 +4618,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:28">
+    <row r="58" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A58" s="11" t="s">
         <v>95</v>
       </c>
@@ -4668,7 +4677,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:28">
+    <row r="59" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A59" s="13" t="s">
         <v>91</v>
       </c>
@@ -4676,7 +4685,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:28">
+    <row r="60" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A60" s="13" t="s">
         <v>96</v>
       </c>
@@ -4735,7 +4744,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:28">
+    <row r="61" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A61" s="11" t="s">
         <v>92</v>
       </c>
@@ -4743,7 +4752,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:28">
+    <row r="62" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A62" s="11" t="s">
         <v>97</v>
       </c>
@@ -4802,7 +4811,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:28">
+    <row r="63" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A63" s="13" t="s">
         <v>98</v>
       </c>
@@ -4810,7 +4819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:28">
+    <row r="64" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A64" s="13" t="s">
         <v>93</v>
       </c>
@@ -4873,7 +4882,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:29" s="9" customFormat="1">
+    <row r="65" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A65" s="9" t="s">
         <v>151</v>
       </c>
@@ -4906,7 +4915,7 @@
       <c r="AB65" s="12"/>
       <c r="AC65" s="19"/>
     </row>
-    <row r="66" spans="1:29">
+    <row r="66" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B66" s="6" t="s">
         <v>122</v>
       </c>
@@ -4926,7 +4935,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:29">
+    <row r="67" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A67" s="11" t="s">
         <v>124</v>
       </c>
@@ -4957,7 +4966,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:29">
+    <row r="68" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A68" s="11" t="s">
         <v>130</v>
       </c>
@@ -5009,11 +5018,20 @@
       <c r="W68" s="3">
         <v>1</v>
       </c>
+      <c r="X68" s="31">
+        <v>1</v>
+      </c>
+      <c r="Y68" s="31">
+        <v>0</v>
+      </c>
+      <c r="Z68" s="31">
+        <v>0</v>
+      </c>
       <c r="AB68" s="16">
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:29">
+    <row r="69" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A69" s="13" t="s">
         <v>125</v>
       </c>
@@ -5044,7 +5062,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:29">
+    <row r="70" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A70" s="13" t="s">
         <v>131</v>
       </c>
@@ -5093,11 +5111,20 @@
       <c r="W70" s="3">
         <v>1</v>
       </c>
+      <c r="X70" s="31">
+        <v>1</v>
+      </c>
+      <c r="Y70" s="31">
+        <v>0</v>
+      </c>
+      <c r="Z70" s="31">
+        <v>0</v>
+      </c>
       <c r="AB70" s="16">
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:29">
+    <row r="71" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A71" s="11" t="s">
         <v>126</v>
       </c>
@@ -5105,7 +5132,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:29">
+    <row r="72" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A72" s="11" t="s">
         <v>164</v>
       </c>
@@ -5139,11 +5166,20 @@
       <c r="W72" s="3">
         <v>1</v>
       </c>
+      <c r="X72" s="31">
+        <v>1</v>
+      </c>
+      <c r="Y72" s="31">
+        <v>0</v>
+      </c>
+      <c r="Z72" s="31">
+        <v>0</v>
+      </c>
       <c r="AB72" s="16">
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:29">
+    <row r="73" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A73" s="13" t="s">
         <v>127</v>
       </c>
@@ -5151,7 +5187,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:29">
+    <row r="74" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A74" s="13" t="s">
         <v>132</v>
       </c>
@@ -5197,6 +5233,15 @@
       <c r="W74" s="3">
         <v>1</v>
       </c>
+      <c r="X74" s="31">
+        <v>1</v>
+      </c>
+      <c r="Y74" s="31">
+        <v>0</v>
+      </c>
+      <c r="Z74" s="31">
+        <v>0</v>
+      </c>
       <c r="AB74" s="16">
         <v>0</v>
       </c>
@@ -5204,7 +5249,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="75" spans="1:29">
+    <row r="75" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A75" s="11" t="s">
         <v>129</v>
       </c>
@@ -5215,7 +5260,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="76" spans="1:29">
+    <row r="76" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A76" s="11" t="s">
         <v>136</v>
       </c>
@@ -5261,6 +5306,15 @@
       <c r="W76" s="3">
         <v>1</v>
       </c>
+      <c r="X76" s="31">
+        <v>1</v>
+      </c>
+      <c r="Y76" s="31">
+        <v>0</v>
+      </c>
+      <c r="Z76" s="31">
+        <v>0</v>
+      </c>
       <c r="AB76" s="16">
         <v>0</v>
       </c>
@@ -5268,7 +5322,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="77" spans="1:29">
+    <row r="77" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A77" s="13" t="s">
         <v>134</v>
       </c>
@@ -5279,7 +5333,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="78" spans="1:29">
+    <row r="78" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A78" s="13" t="s">
         <v>135</v>
       </c>
@@ -5325,6 +5379,15 @@
       <c r="W78" s="3">
         <v>1</v>
       </c>
+      <c r="X78" s="31">
+        <v>1</v>
+      </c>
+      <c r="Y78" s="31">
+        <v>0</v>
+      </c>
+      <c r="Z78" s="31">
+        <v>0</v>
+      </c>
       <c r="AB78" s="16">
         <v>0</v>
       </c>
@@ -5332,7 +5395,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="79" spans="1:29">
+    <row r="79" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A79" s="11" t="s">
         <v>137</v>
       </c>
@@ -5343,7 +5406,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="80" spans="1:29">
+    <row r="80" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A80" s="11" t="s">
         <v>138</v>
       </c>
@@ -5389,6 +5452,15 @@
       <c r="W80" s="3">
         <v>1</v>
       </c>
+      <c r="X80" s="31">
+        <v>1</v>
+      </c>
+      <c r="Y80" s="31">
+        <v>0</v>
+      </c>
+      <c r="Z80" s="31">
+        <v>0</v>
+      </c>
       <c r="AB80" s="16">
         <v>0</v>
       </c>
@@ -5396,7 +5468,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="81" spans="1:29">
+    <row r="81" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A81" s="13" t="s">
         <v>139</v>
       </c>
@@ -5407,7 +5479,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="82" spans="1:29">
+    <row r="82" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A82" s="13" t="s">
         <v>140</v>
       </c>
@@ -5453,6 +5525,15 @@
       <c r="W82" s="3">
         <v>1</v>
       </c>
+      <c r="X82" s="31">
+        <v>1</v>
+      </c>
+      <c r="Y82" s="31">
+        <v>0</v>
+      </c>
+      <c r="Z82" s="31">
+        <v>0</v>
+      </c>
       <c r="AB82" s="16">
         <v>0</v>
       </c>
@@ -5460,7 +5541,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="83" spans="1:29">
+    <row r="83" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A83" s="11" t="s">
         <v>141</v>
       </c>
@@ -5471,7 +5552,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="84" spans="1:29">
+    <row r="84" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A84" s="11" t="s">
         <v>142</v>
       </c>
@@ -5517,6 +5598,15 @@
       <c r="W84" s="3">
         <v>1</v>
       </c>
+      <c r="X84" s="31">
+        <v>1</v>
+      </c>
+      <c r="Y84" s="31">
+        <v>0</v>
+      </c>
+      <c r="Z84" s="31">
+        <v>0</v>
+      </c>
       <c r="AB84" s="16">
         <v>0</v>
       </c>
@@ -5524,7 +5614,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="85" spans="1:29" s="9" customFormat="1">
+    <row r="85" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A85" s="9" t="s">
         <v>99</v>
       </c>
@@ -5557,7 +5647,7 @@
       <c r="AB85" s="12"/>
       <c r="AC85" s="19"/>
     </row>
-    <row r="86" spans="1:29">
+    <row r="86" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>100</v>
       </c>
@@ -5592,7 +5682,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:29">
+    <row r="87" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>101</v>
       </c>
@@ -5618,7 +5708,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="88" spans="1:29">
+    <row r="88" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>102</v>
       </c>
@@ -5656,7 +5746,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:29" s="9" customFormat="1">
+    <row r="89" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A89" s="9" t="s">
         <v>152</v>
       </c>
@@ -5689,7 +5779,7 @@
       <c r="AB89" s="12"/>
       <c r="AC89" s="19"/>
     </row>
-    <row r="90" spans="1:29">
+    <row r="90" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A90" s="11" t="s">
         <v>155</v>
       </c>
@@ -5697,7 +5787,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:29">
+    <row r="91" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A91" s="11" t="s">
         <v>156</v>
       </c>
@@ -5705,12 +5795,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:29">
+    <row r="92" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="93" spans="1:29">
+    <row r="93" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B93" s="6" t="s">
         <v>153</v>
       </c>
@@ -5718,7 +5808,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:29" s="9" customFormat="1">
+    <row r="94" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A94" s="9" t="s">
         <v>158</v>
       </c>
@@ -5751,8 +5841,8 @@
       <c r="AB94" s="12"/>
       <c r="AC94" s="19"/>
     </row>
-    <row r="95" spans="1:29">
-      <c r="A95" s="30" t="s">
+    <row r="95" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A95" s="28" t="s">
         <v>159</v>
       </c>
       <c r="D95" s="8" t="s">
@@ -5774,7 +5864,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:29">
+    <row r="96" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>160</v>
       </c>
@@ -5812,7 +5902,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:29">
+    <row r="97" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>161</v>
       </c>
@@ -5841,7 +5931,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:29" s="9" customFormat="1">
+    <row r="98" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A98" s="9" t="s">
         <v>162</v>
       </c>
@@ -5874,19 +5964,13 @@
       <c r="AB98" s="12"/>
       <c r="AC98" s="19"/>
     </row>
-    <row r="99" spans="1:29">
+    <row r="99" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>163</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="D2:G2"/>
-    <mergeCell ref="O2:R2"/>
-    <mergeCell ref="S2:T2"/>
-    <mergeCell ref="X2:Z2"/>
-    <mergeCell ref="H2:J2"/>
-    <mergeCell ref="K2:L2"/>
     <mergeCell ref="D1:G1"/>
     <mergeCell ref="M1:N1"/>
     <mergeCell ref="X1:Z1"/>
@@ -5894,6 +5978,12 @@
     <mergeCell ref="O1:R1"/>
     <mergeCell ref="K1:L1"/>
     <mergeCell ref="H1:J1"/>
+    <mergeCell ref="D2:G2"/>
+    <mergeCell ref="O2:R2"/>
+    <mergeCell ref="S2:T2"/>
+    <mergeCell ref="X2:Z2"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="K2:L2"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fix the next address field of the last microinst. of IRET
</commit_message>
<xml_diff>
--- a/Microroutines.xlsx
+++ b/Microroutines.xlsx
@@ -882,14 +882,14 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Accent2" xfId="4" builtinId="33"/>
@@ -1177,8 +1177,8 @@
   <dimension ref="A1:AD126"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="86" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A112" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C125" sqref="C125"/>
+      <pane ySplit="1" topLeftCell="A111" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C126" sqref="C126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1224,35 +1224,35 @@
       <c r="C1" s="8" t="s">
         <v>201</v>
       </c>
-      <c r="D1" s="32" t="s">
+      <c r="D1" s="34" t="s">
         <v>48</v>
       </c>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="33" t="s">
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="35" t="s">
         <v>51</v>
       </c>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
-      <c r="K1" s="32" t="s">
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="34" t="s">
         <v>50</v>
       </c>
-      <c r="L1" s="32"/>
-      <c r="M1" s="33" t="s">
+      <c r="L1" s="34"/>
+      <c r="M1" s="35" t="s">
         <v>49</v>
       </c>
-      <c r="N1" s="33"/>
-      <c r="O1" s="32" t="s">
+      <c r="N1" s="35"/>
+      <c r="O1" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="P1" s="32"/>
-      <c r="Q1" s="32"/>
-      <c r="R1" s="32"/>
-      <c r="S1" s="33" t="s">
+      <c r="P1" s="34"/>
+      <c r="Q1" s="34"/>
+      <c r="R1" s="34"/>
+      <c r="S1" s="35" t="s">
         <v>53</v>
       </c>
-      <c r="T1" s="33"/>
+      <c r="T1" s="35"/>
       <c r="U1" s="3" t="s">
         <v>1</v>
       </c>
@@ -1262,11 +1262,11 @@
       <c r="W1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="X1" s="33" t="s">
+      <c r="X1" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="Y1" s="33"/>
-      <c r="Z1" s="33"/>
+      <c r="Y1" s="35"/>
+      <c r="Z1" s="35"/>
       <c r="AA1" s="3" t="s">
         <v>4</v>
       </c>
@@ -1281,24 +1281,24 @@
       </c>
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="33"/>
-      <c r="I2" s="33"/>
-      <c r="J2" s="33"/>
-      <c r="K2" s="32"/>
-      <c r="L2" s="32"/>
-      <c r="O2" s="32"/>
-      <c r="P2" s="32"/>
-      <c r="Q2" s="32"/>
-      <c r="R2" s="32"/>
-      <c r="S2" s="33"/>
-      <c r="T2" s="33"/>
-      <c r="X2" s="33"/>
-      <c r="Y2" s="33"/>
-      <c r="Z2" s="33"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="35"/>
+      <c r="J2" s="35"/>
+      <c r="K2" s="34"/>
+      <c r="L2" s="34"/>
+      <c r="O2" s="34"/>
+      <c r="P2" s="34"/>
+      <c r="Q2" s="34"/>
+      <c r="R2" s="34"/>
+      <c r="S2" s="35"/>
+      <c r="T2" s="35"/>
+      <c r="X2" s="35"/>
+      <c r="Y2" s="35"/>
+      <c r="Z2" s="35"/>
     </row>
     <row r="3" spans="1:30" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
@@ -7654,7 +7654,7 @@
       </c>
     </row>
     <row r="123" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A123" s="34" t="s">
+      <c r="A123" s="32" t="s">
         <v>203</v>
       </c>
       <c r="B123" s="6" t="s">
@@ -7687,27 +7687,18 @@
       </c>
     </row>
     <row r="126" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A126" s="35" t="s">
+      <c r="A126" s="33" t="s">
         <v>204</v>
       </c>
       <c r="B126" s="6" t="s">
         <v>210</v>
       </c>
       <c r="C126" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="AA126" s="3">
-        <v>1</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="D2:G2"/>
-    <mergeCell ref="O2:R2"/>
-    <mergeCell ref="S2:T2"/>
-    <mergeCell ref="X2:Z2"/>
-    <mergeCell ref="H2:J2"/>
-    <mergeCell ref="K2:L2"/>
     <mergeCell ref="D1:G1"/>
     <mergeCell ref="M1:N1"/>
     <mergeCell ref="X1:Z1"/>
@@ -7715,6 +7706,12 @@
     <mergeCell ref="O1:R1"/>
     <mergeCell ref="K1:L1"/>
     <mergeCell ref="H1:J1"/>
+    <mergeCell ref="D2:G2"/>
+    <mergeCell ref="O2:R2"/>
+    <mergeCell ref="S2:T2"/>
+    <mergeCell ref="X2:Z2"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="K2:L2"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add OR_INT signal and the interrupt hardware
</commit_message>
<xml_diff>
--- a/Microroutines.xlsx
+++ b/Microroutines.xlsx
@@ -41,13 +41,7 @@
     <t>F11</t>
   </si>
   <si>
-    <t xml:space="preserve">PC_out, MAR_in, Z_in, Read, Clear_Y, Carry_in, Add </t>
-  </si>
-  <si>
     <t>PLA_out</t>
-  </si>
-  <si>
-    <t>PC_in, Z_out</t>
   </si>
   <si>
     <t>IR_in, MDR_out</t>
@@ -703,6 +697,12 @@
   </si>
   <si>
     <t>FLAGs_in MDR_out FLAGS_CH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PC_out, MAR_in, Z_in, Clear_Y, Carry_in, Add </t>
+  </si>
+  <si>
+    <t>PC_in, Z_out, Read</t>
   </si>
 </sst>
 </file>
@@ -1197,8 +1197,8 @@
   <dimension ref="A1:AE129"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="86" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A110" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AA129" sqref="AA129"/>
+      <pane ySplit="1" topLeftCell="A109" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Y129" sqref="Y129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1240,38 +1240,38 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D1" s="36" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E1" s="36"/>
       <c r="F1" s="36"/>
       <c r="G1" s="36"/>
       <c r="H1" s="37" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="I1" s="37"/>
       <c r="J1" s="37"/>
       <c r="K1" s="36" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="L1" s="36"/>
       <c r="M1" s="37" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="N1" s="37"/>
       <c r="O1" s="36" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="P1" s="36"/>
       <c r="Q1" s="36"/>
       <c r="R1" s="36"/>
       <c r="S1" s="37" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="T1" s="37"/>
       <c r="U1" s="3" t="s">
@@ -1284,7 +1284,7 @@
         <v>3</v>
       </c>
       <c r="X1" s="37" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="Y1" s="37"/>
       <c r="Z1" s="37"/>
@@ -1292,16 +1292,16 @@
         <v>4</v>
       </c>
       <c r="AB1" s="16" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="AC1" s="28" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="AD1" s="35" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="AE1" s="17" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.3">
@@ -1326,7 +1326,7 @@
     </row>
     <row r="3" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B3" s="10"/>
       <c r="C3" s="10"/>
@@ -1361,16 +1361,16 @@
     </row>
     <row r="4" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>213</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E4" s="3">
         <v>0</v>
@@ -1454,16 +1454,16 @@
     </row>
     <row r="5" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>214</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E5" s="3">
         <v>0</v>
@@ -1547,16 +1547,16 @@
     </row>
     <row r="6" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E6" s="3">
         <v>0</v>
@@ -1640,16 +1640,16 @@
     </row>
     <row r="7" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E7" s="3">
         <v>0</v>
@@ -1733,7 +1733,7 @@
     </row>
     <row r="8" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B8" s="10"/>
       <c r="C8" s="10"/>
@@ -1772,7 +1772,7 @@
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="AC9" s="34">
         <v>0</v>
@@ -1783,7 +1783,7 @@
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B10" s="6">
         <v>101</v>
@@ -1792,79 +1792,79 @@
         <v>201</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J10" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="K10" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="L10" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="M10" s="7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="N10" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="O10" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="P10" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="Q10" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="R10" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="S10" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="T10" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="U10" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="V10" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="W10" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="X10" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="Y10" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="Z10" s="7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="AA10" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="AB10" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="AC10" s="34">
         <v>0</v>
@@ -1875,16 +1875,16 @@
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E11" s="3">
         <v>1</v>
@@ -1967,16 +1967,16 @@
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C12" s="26" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E12" s="3">
         <v>0</v>
@@ -2059,16 +2059,16 @@
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E13" s="3">
         <v>1</v>
@@ -2151,16 +2151,16 @@
     </row>
     <row r="14" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="6" t="s">
-        <v>24</v>
-      </c>
       <c r="C14" s="7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E14" s="3">
         <v>0</v>
@@ -2243,16 +2243,16 @@
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B15" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="7" t="s">
-        <v>29</v>
-      </c>
       <c r="D15" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E15" s="3">
         <v>1</v>
@@ -2335,13 +2335,13 @@
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B16" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" s="7" t="s">
         <v>29</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>31</v>
       </c>
       <c r="D16" s="3">
         <v>0</v>
@@ -2427,13 +2427,13 @@
     </row>
     <row r="17" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D17" s="3">
         <v>0</v>
@@ -2519,16 +2519,16 @@
     </row>
     <row r="18" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E18" s="3">
         <v>0</v>
@@ -2611,16 +2611,16 @@
     </row>
     <row r="19" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B19" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>36</v>
-      </c>
       <c r="D19" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E19" s="3">
         <v>0</v>
@@ -2703,16 +2703,16 @@
     </row>
     <row r="20" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B20" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C20" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C20" s="7" t="s">
-        <v>38</v>
-      </c>
       <c r="D20" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E20" s="3">
         <v>0</v>
@@ -2795,16 +2795,16 @@
     </row>
     <row r="21" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B21" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="C21" s="7" t="s">
-        <v>40</v>
-      </c>
       <c r="D21" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E21" s="3">
         <v>1</v>
@@ -2887,16 +2887,16 @@
     </row>
     <row r="22" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E22" s="3">
         <v>0</v>
@@ -2979,16 +2979,16 @@
     </row>
     <row r="23" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E23" s="3">
         <v>0</v>
@@ -3069,21 +3069,21 @@
         <v>0</v>
       </c>
       <c r="AE23" s="18" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="24" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E24" s="3">
         <v>0</v>
@@ -3166,16 +3166,16 @@
     </row>
     <row r="25" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E25" s="3">
         <v>0</v>
@@ -3258,16 +3258,16 @@
     </row>
     <row r="26" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E26" s="3">
         <v>0</v>
@@ -3350,7 +3350,7 @@
     </row>
     <row r="27" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="9" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B27" s="10"/>
       <c r="C27" s="10"/>
@@ -3389,13 +3389,13 @@
     </row>
     <row r="28" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D28" s="22">
         <v>0</v>
@@ -3458,19 +3458,19 @@
         <v>0</v>
       </c>
       <c r="X28" s="7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="Y28" s="7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="Z28" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="AA28" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="AB28" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="AC28" s="34">
         <v>0</v>
@@ -3481,16 +3481,16 @@
     </row>
     <row r="29" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B29" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C29" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="C29" s="7" t="s">
-        <v>57</v>
-      </c>
       <c r="D29" s="24" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E29" s="22">
         <v>1</v>
@@ -3550,19 +3550,19 @@
         <v>0</v>
       </c>
       <c r="X29" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="Y29" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="Z29" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="AA29" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="AB29" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="AC29" s="34">
         <v>0</v>
@@ -3573,13 +3573,13 @@
     </row>
     <row r="30" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C30" s="26" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D30" s="22">
         <v>0</v>
@@ -3642,19 +3642,19 @@
         <v>0</v>
       </c>
       <c r="X30" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="Y30" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="Z30" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="AA30" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="AB30" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="AC30" s="34">
         <v>0</v>
@@ -3665,13 +3665,13 @@
     </row>
     <row r="31" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D31" s="22">
         <v>0</v>
@@ -3734,19 +3734,19 @@
         <v>0</v>
       </c>
       <c r="X31" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="Y31" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="Z31" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="AA31" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="AB31" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="AC31" s="34">
         <v>0</v>
@@ -3757,13 +3757,13 @@
     </row>
     <row r="32" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D32" s="22">
         <v>0</v>
@@ -3826,19 +3826,19 @@
         <v>0</v>
       </c>
       <c r="X32" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="Y32" s="7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="Z32" s="7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="AA32" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="AB32" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="AC32" s="34">
         <v>0</v>
@@ -3849,13 +3849,13 @@
     </row>
     <row r="33" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D33" s="22">
         <v>0</v>
@@ -3918,19 +3918,19 @@
         <v>0</v>
       </c>
       <c r="X33" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="Y33" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="Z33" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="AA33" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="AB33" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="AC33" s="34">
         <v>0</v>
@@ -3941,13 +3941,13 @@
     </row>
     <row r="34" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D34" s="22">
         <v>0</v>
@@ -4010,19 +4010,19 @@
         <v>0</v>
       </c>
       <c r="X34" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="Y34" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="Z34" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="AA34" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="AB34" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="AC34" s="34">
         <v>0</v>
@@ -4033,13 +4033,13 @@
     </row>
     <row r="35" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D35" s="22">
         <v>0</v>
@@ -4102,19 +4102,19 @@
         <v>0</v>
       </c>
       <c r="X35" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="Y35" s="7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="Z35" s="7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="AA35" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="AB35" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="AC35" s="34">
         <v>0</v>
@@ -4125,13 +4125,13 @@
     </row>
     <row r="36" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D36" s="22">
         <v>0</v>
@@ -4194,19 +4194,19 @@
         <v>0</v>
       </c>
       <c r="X36" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="Y36" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="Z36" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="AA36" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="AB36" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="AC36" s="34">
         <v>0</v>
@@ -4217,13 +4217,13 @@
     </row>
     <row r="37" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D37" s="22">
         <v>0</v>
@@ -4286,19 +4286,19 @@
         <v>0</v>
       </c>
       <c r="X37" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="Y37" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="Z37" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="AA37" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="AB37" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="AC37" s="34">
         <v>0</v>
@@ -4309,13 +4309,13 @@
     </row>
     <row r="38" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D38" s="22">
         <v>0</v>
@@ -4378,19 +4378,19 @@
         <v>0</v>
       </c>
       <c r="X38" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="Y38" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="Z38" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="AA38" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="AB38" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="AC38" s="34">
         <v>0</v>
@@ -4401,13 +4401,13 @@
     </row>
     <row r="39" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D39" s="22">
         <v>0</v>
@@ -4470,19 +4470,19 @@
         <v>0</v>
       </c>
       <c r="X39" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="Y39" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="Z39" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="AA39" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="AB39" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="AC39" s="34">
         <v>0</v>
@@ -4493,13 +4493,13 @@
     </row>
     <row r="40" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D40" s="22">
         <v>0</v>
@@ -4562,19 +4562,19 @@
         <v>0</v>
       </c>
       <c r="X40" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="Y40" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="Z40" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="AA40" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="AB40" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="AC40" s="34">
         <v>0</v>
@@ -4585,13 +4585,13 @@
     </row>
     <row r="41" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D41" s="22">
         <v>0</v>
@@ -4654,19 +4654,19 @@
         <v>0</v>
       </c>
       <c r="X41" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="Y41" s="7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="Z41" s="7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="AA41" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="AB41" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="AC41" s="34">
         <v>0</v>
@@ -4675,18 +4675,18 @@
         <v>0</v>
       </c>
       <c r="AE41" s="18" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="42" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D42" s="22">
         <v>0</v>
@@ -4749,19 +4749,19 @@
         <v>0</v>
       </c>
       <c r="X42" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="Y42" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="Z42" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="AA42" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="AB42" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="AC42" s="34">
         <v>0</v>
@@ -4772,13 +4772,13 @@
     </row>
     <row r="43" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D43" s="22">
         <v>0</v>
@@ -4841,19 +4841,19 @@
         <v>0</v>
       </c>
       <c r="X43" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="Y43" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="Z43" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="AA43" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="AB43" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="AC43" s="34">
         <v>0</v>
@@ -4864,13 +4864,13 @@
     </row>
     <row r="44" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D44" s="22">
         <v>0</v>
@@ -4933,19 +4933,19 @@
         <v>0</v>
       </c>
       <c r="X44" s="7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="Y44" s="7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="Z44" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="AA44" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="AB44" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="AC44" s="34">
         <v>0</v>
@@ -4954,12 +4954,12 @@
         <v>0</v>
       </c>
       <c r="AE44" s="18" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="45" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A45" s="9" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B45" s="10"/>
       <c r="C45" s="10"/>
@@ -4998,16 +4998,16 @@
     </row>
     <row r="46" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A46" s="11" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E46" s="3">
         <v>0</v>
@@ -5048,7 +5048,7 @@
     </row>
     <row r="47" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A47" s="13" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="AA47" s="34">
         <v>0</v>
@@ -5065,16 +5065,16 @@
     </row>
     <row r="48" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A48" s="13" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B48" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="C48" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="C48" s="7" t="s">
-        <v>109</v>
-      </c>
       <c r="D48" s="8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E48" s="3">
         <v>0</v>
@@ -5133,7 +5133,7 @@
     </row>
     <row r="49" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A49" s="11" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E49" s="4"/>
       <c r="F49" s="4"/>
@@ -5172,16 +5172,16 @@
     </row>
     <row r="50" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A50" s="11" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D50" s="8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E50" s="3">
         <v>0</v>
@@ -5240,7 +5240,7 @@
     </row>
     <row r="51" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A51" s="13" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C51" s="25"/>
       <c r="E51" s="4"/>
@@ -5280,16 +5280,16 @@
     </row>
     <row r="52" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A52" s="13" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C52" s="7" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D52" s="8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E52" s="21">
         <v>0</v>
@@ -5348,7 +5348,7 @@
     </row>
     <row r="53" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A53" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E53" s="4"/>
       <c r="F53" s="4"/>
@@ -5387,16 +5387,16 @@
     </row>
     <row r="54" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A54" s="11" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C54" s="7" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D54" s="8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E54" s="21">
         <v>0</v>
@@ -5455,7 +5455,7 @@
     </row>
     <row r="55" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A55" s="13" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="AA55" s="34">
         <v>0</v>
@@ -5472,16 +5472,16 @@
     </row>
     <row r="56" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A56" s="13" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C56" s="7" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D56" s="8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E56" s="21">
         <v>0</v>
@@ -5540,7 +5540,7 @@
     </row>
     <row r="57" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A57" s="11" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="AA57" s="34">
         <v>0</v>
@@ -5557,16 +5557,16 @@
     </row>
     <row r="58" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A58" s="11" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B58" s="6" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C58" s="7" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D58" s="8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E58" s="21">
         <v>0</v>
@@ -5625,7 +5625,7 @@
     </row>
     <row r="59" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A59" s="13" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="AA59" s="34">
         <v>0</v>
@@ -5642,16 +5642,16 @@
     </row>
     <row r="60" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A60" s="13" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B60" s="6" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C60" s="7" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D60" s="8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E60" s="21">
         <v>0</v>
@@ -5710,7 +5710,7 @@
     </row>
     <row r="61" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A61" s="11" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="AA61" s="34">
         <v>0</v>
@@ -5727,16 +5727,16 @@
     </row>
     <row r="62" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A62" s="11" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B62" s="6" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C62" s="7" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D62" s="8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E62" s="21">
         <v>0</v>
@@ -5795,7 +5795,7 @@
     </row>
     <row r="63" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A63" s="13" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="AA63" s="34">
         <v>0</v>
@@ -5812,16 +5812,16 @@
     </row>
     <row r="64" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A64" s="13" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B64" s="6" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C64" s="5">
         <v>0</v>
       </c>
       <c r="D64" s="8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E64" s="21">
         <v>0</v>
@@ -5865,13 +5865,13 @@
         <v>1</v>
       </c>
       <c r="X64" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y64" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z64" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA64" s="3">
         <v>0</v>
@@ -5888,7 +5888,7 @@
     </row>
     <row r="65" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A65" s="9" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B65" s="10"/>
       <c r="C65" s="10"/>
@@ -5927,10 +5927,10 @@
     </row>
     <row r="66" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B66" s="6" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C66" s="7" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="X66" s="2">
         <v>1</v>
@@ -5953,7 +5953,7 @@
     </row>
     <row r="67" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A67" s="11" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E67" s="14"/>
       <c r="F67" s="14"/>
@@ -5990,16 +5990,16 @@
     </row>
     <row r="68" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A68" s="11" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B68" s="6" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C68" s="7" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D68" s="8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E68" s="3">
         <v>0</v>
@@ -6061,7 +6061,7 @@
     </row>
     <row r="69" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A69" s="13" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E69" s="14"/>
       <c r="F69" s="14"/>
@@ -6098,16 +6098,16 @@
     </row>
     <row r="70" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A70" s="13" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B70" s="6" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C70" s="7" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D70" s="8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E70" s="3">
         <v>0</v>
@@ -6166,7 +6166,7 @@
     </row>
     <row r="71" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A71" s="11" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="AB71" s="16">
         <v>0</v>
@@ -6180,13 +6180,13 @@
     </row>
     <row r="72" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A72" s="11" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B72" s="6" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C72" s="7" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="H72" s="2">
         <v>0</v>
@@ -6233,7 +6233,7 @@
     </row>
     <row r="73" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A73" s="13" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="AB73" s="16">
         <v>0</v>
@@ -6247,16 +6247,16 @@
     </row>
     <row r="74" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A74" s="13" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B74" s="6" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C74" s="7" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D74" s="8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E74" s="3">
         <v>0</v>
@@ -6310,12 +6310,12 @@
         <v>0</v>
       </c>
       <c r="AE74" s="18" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="75" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A75" s="11" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="AB75" s="16">
         <v>0</v>
@@ -6327,21 +6327,21 @@
         <v>0</v>
       </c>
       <c r="AE75" s="18" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="76" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A76" s="11" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B76" s="6" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C76" s="7" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D76" s="8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E76" s="3">
         <v>0</v>
@@ -6395,12 +6395,12 @@
         <v>0</v>
       </c>
       <c r="AE76" s="18" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="77" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A77" s="13" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="AB77" s="16">
         <v>0</v>
@@ -6412,21 +6412,21 @@
         <v>0</v>
       </c>
       <c r="AE77" s="18" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="78" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A78" s="13" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B78" s="6" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C78" s="7" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D78" s="8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E78" s="3">
         <v>0</v>
@@ -6480,12 +6480,12 @@
         <v>0</v>
       </c>
       <c r="AE78" s="18" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="79" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A79" s="11" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="AB79" s="16">
         <v>0</v>
@@ -6497,21 +6497,21 @@
         <v>0</v>
       </c>
       <c r="AE79" s="18" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="80" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A80" s="11" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B80" s="6" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C80" s="7" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D80" s="8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E80" s="3">
         <v>0</v>
@@ -6565,12 +6565,12 @@
         <v>0</v>
       </c>
       <c r="AE80" s="18" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="81" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A81" s="13" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="AB81" s="16">
         <v>0</v>
@@ -6582,21 +6582,21 @@
         <v>0</v>
       </c>
       <c r="AE81" s="18" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="82" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A82" s="13" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B82" s="6" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C82" s="7" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D82" s="8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E82" s="3">
         <v>0</v>
@@ -6650,12 +6650,12 @@
         <v>0</v>
       </c>
       <c r="AE82" s="18" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="83" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A83" s="11" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="AB83" s="16">
         <v>0</v>
@@ -6667,21 +6667,21 @@
         <v>0</v>
       </c>
       <c r="AE83" s="18" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="84" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A84" s="11" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B84" s="6" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C84" s="7" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D84" s="8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E84" s="3">
         <v>0</v>
@@ -6735,12 +6735,12 @@
         <v>0</v>
       </c>
       <c r="AE84" s="18" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="85" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A85" s="9" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B85" s="10"/>
       <c r="C85" s="10"/>
@@ -6779,16 +6779,16 @@
     </row>
     <row r="86" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B86" s="6" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C86" s="7" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D86" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E86" s="3">
         <v>0</v>
@@ -6820,48 +6820,57 @@
     </row>
     <row r="87" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
+        <v>98</v>
+      </c>
+      <c r="B87" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="C87" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="S87" s="2">
+        <v>1</v>
+      </c>
+      <c r="T87" s="2">
+        <v>0</v>
+      </c>
+      <c r="X87" s="2">
+        <v>1</v>
+      </c>
+      <c r="Y87" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z87" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA87" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB87" s="16">
+        <v>0</v>
+      </c>
+      <c r="AC87" s="34">
+        <v>0</v>
+      </c>
+      <c r="AD87" s="35">
+        <v>0</v>
+      </c>
+      <c r="AE87" s="18" t="s">
         <v>100</v>
-      </c>
-      <c r="B87" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="C87" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="S87" s="2">
-        <v>1</v>
-      </c>
-      <c r="T87" s="2">
-        <v>0</v>
-      </c>
-      <c r="AA87" s="3">
-        <v>0</v>
-      </c>
-      <c r="AB87" s="16">
-        <v>0</v>
-      </c>
-      <c r="AC87" s="34">
-        <v>0</v>
-      </c>
-      <c r="AD87" s="35">
-        <v>0</v>
-      </c>
-      <c r="AE87" s="18" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="88" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B88" s="6" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C88" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D88" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E88" s="3">
         <v>0</v>
@@ -6879,6 +6888,15 @@
         <v>0</v>
       </c>
       <c r="J88" s="2">
+        <v>1</v>
+      </c>
+      <c r="X88" s="2">
+        <v>1</v>
+      </c>
+      <c r="Y88" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z88" s="2">
         <v>1</v>
       </c>
       <c r="AA88" s="3">
@@ -6896,7 +6914,7 @@
     </row>
     <row r="89" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A89" s="9" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B89" s="10"/>
       <c r="C89" s="10"/>
@@ -6935,7 +6953,7 @@
     </row>
     <row r="90" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A90" s="11" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="AB90" s="16">
         <v>0</v>
@@ -6949,7 +6967,7 @@
     </row>
     <row r="91" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A91" s="11" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="AB91" s="16">
         <v>0</v>
@@ -6963,7 +6981,7 @@
     </row>
     <row r="92" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="AC92" s="34">
         <v>0</v>
@@ -6974,7 +6992,7 @@
     </row>
     <row r="93" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B93" s="6" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="AB93" s="16">
         <v>1</v>
@@ -6988,7 +7006,7 @@
     </row>
     <row r="94" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A94" s="9" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B94" s="10"/>
       <c r="C94" s="10"/>
@@ -7027,10 +7045,10 @@
     </row>
     <row r="95" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A95" s="27" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D95" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E95" s="3">
         <v>1</v>
@@ -7056,10 +7074,10 @@
     </row>
     <row r="96" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D96" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E96" s="3">
         <v>0</v>
@@ -7100,13 +7118,13 @@
     </row>
     <row r="97" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C97" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D97" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E97" s="3">
         <v>0</v>
@@ -7124,6 +7142,15 @@
         <v>0</v>
       </c>
       <c r="J97" s="2">
+        <v>1</v>
+      </c>
+      <c r="X97" s="2">
+        <v>1</v>
+      </c>
+      <c r="Y97" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z97" s="2">
         <v>1</v>
       </c>
       <c r="AC97" s="34">
@@ -7135,7 +7162,7 @@
     </row>
     <row r="98" spans="1:31" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A98" s="9" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B98" s="10"/>
       <c r="C98" s="10"/>
@@ -7174,7 +7201,7 @@
     </row>
     <row r="99" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="AC99" s="34">
         <v>0</v>
@@ -7185,16 +7212,16 @@
     </row>
     <row r="100" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A100" s="11" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B100" s="6" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C100" s="7" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D100" s="8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E100" s="3">
         <v>0</v>
@@ -7277,16 +7304,16 @@
     </row>
     <row r="101" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A101" s="11" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B101" s="6" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C101" s="7" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D101" s="8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E101" s="3">
         <v>0</v>
@@ -7369,16 +7396,16 @@
     </row>
     <row r="102" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A102" s="11" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B102" s="6" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C102" s="7" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D102" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E102" s="3">
         <v>0</v>
@@ -7461,16 +7488,16 @@
     </row>
     <row r="103" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A103" s="11" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B103" s="6" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C103" s="7" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D103" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E103" s="3">
         <v>1</v>
@@ -7553,16 +7580,16 @@
     </row>
     <row r="104" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A104" s="11" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B104" s="6" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C104" s="7" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D104" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E104" s="3">
         <v>0</v>
@@ -7645,16 +7672,16 @@
     </row>
     <row r="105" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A105" s="11" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B105" s="6" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C105" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D105" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E105" s="3">
         <v>1</v>
@@ -7714,13 +7741,13 @@
         <v>0</v>
       </c>
       <c r="X105" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y105" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z105" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA105" s="3">
         <v>0</v>
@@ -7737,7 +7764,7 @@
     </row>
     <row r="106" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A106" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="AC106" s="34">
         <v>0</v>
@@ -7748,16 +7775,16 @@
     </row>
     <row r="107" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A107" s="11" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B107" s="6" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C107" s="7" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D107" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E107" s="3">
         <v>1</v>
@@ -7840,16 +7867,16 @@
     </row>
     <row r="108" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A108" s="11" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B108" s="6" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C108" s="7" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D108" s="8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E108" s="3">
         <v>0</v>
@@ -7932,16 +7959,16 @@
     </row>
     <row r="109" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A109" s="11" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B109" s="6" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C109" s="7" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D109" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E109" s="3">
         <v>0</v>
@@ -8024,16 +8051,16 @@
     </row>
     <row r="110" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A110" s="11" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B110" s="6" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C110" s="7" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D110" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E110" s="3">
         <v>0</v>
@@ -8116,13 +8143,13 @@
     </row>
     <row r="111" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A111" s="11" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B111" s="6" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C111" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E111" s="32"/>
       <c r="F111" s="32"/>
@@ -8143,9 +8170,15 @@
       <c r="U111" s="32"/>
       <c r="V111" s="33"/>
       <c r="W111" s="32"/>
-      <c r="X111" s="33"/>
-      <c r="Y111" s="33"/>
-      <c r="Z111" s="33"/>
+      <c r="X111" s="33">
+        <v>1</v>
+      </c>
+      <c r="Y111" s="33">
+        <v>1</v>
+      </c>
+      <c r="Z111" s="33">
+        <v>1</v>
+      </c>
       <c r="AA111" s="32">
         <v>0</v>
       </c>
@@ -8159,7 +8192,7 @@
     </row>
     <row r="112" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A112" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="AC112" s="34">
         <v>0</v>
@@ -8170,16 +8203,16 @@
     </row>
     <row r="113" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A113" s="11" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B113" s="6" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C113" s="7" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D113" s="8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E113" s="3">
         <v>0</v>
@@ -8262,16 +8295,16 @@
     </row>
     <row r="114" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A114" s="11" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B114" s="6" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C114" s="7" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D114" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E114" s="3">
         <v>0</v>
@@ -8354,16 +8387,16 @@
     </row>
     <row r="115" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A115" s="11" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B115" s="6" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C115" s="7" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D115" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E115" s="3">
         <v>0</v>
@@ -8446,16 +8479,16 @@
     </row>
     <row r="116" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A116" s="11" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B116" s="6" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C116" s="7" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D116" s="8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E116" s="3">
         <v>0</v>
@@ -8538,16 +8571,16 @@
     </row>
     <row r="117" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A117" s="11" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B117" s="6" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C117" s="7" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D117" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E117" s="3">
         <v>0</v>
@@ -8630,16 +8663,16 @@
     </row>
     <row r="118" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A118" s="11" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B118" s="6" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C118" s="7" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D118" s="8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E118" s="3">
         <v>0</v>
@@ -8722,16 +8755,16 @@
     </row>
     <row r="119" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A119" s="11" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B119" s="6" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C119" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D119" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E119" s="3">
         <v>0</v>
@@ -8791,13 +8824,13 @@
         <v>0</v>
       </c>
       <c r="X119" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y119" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z119" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA119" s="3">
         <v>0</v>
@@ -8814,7 +8847,7 @@
     </row>
     <row r="120" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A120" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="AD120" s="35">
         <v>0</v>
@@ -8822,7 +8855,7 @@
     </row>
     <row r="121" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A121" s="11" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="AD121" s="35">
         <v>0</v>
@@ -8830,16 +8863,16 @@
     </row>
     <row r="122" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A122" s="11" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B122" s="6" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C122" s="7" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D122" s="8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E122" s="3">
         <v>0</v>
@@ -8889,13 +8922,13 @@
     </row>
     <row r="123" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A123" s="11" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B123" s="6" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C123" s="7" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="K123" s="3">
         <v>1</v>
@@ -8915,16 +8948,16 @@
     </row>
     <row r="124" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A124" s="11" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B124" s="6" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C124" s="7" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D124" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E124" s="32">
         <v>0</v>
@@ -8969,16 +9002,16 @@
     </row>
     <row r="125" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A125" s="11" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B125" s="6" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C125" s="7" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D125" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E125" s="3">
         <v>0</v>
@@ -8998,16 +9031,16 @@
     </row>
     <row r="126" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A126" s="11" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B126" s="6" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C126" s="7" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D126" s="8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E126" s="34">
         <v>0</v>
@@ -9058,13 +9091,13 @@
     </row>
     <row r="127" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A127" s="11" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B127" s="6" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C127" s="7" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="K127" s="3">
         <v>1</v>
@@ -9081,16 +9114,16 @@
     </row>
     <row r="128" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A128" s="11" t="s">
+        <v>207</v>
+      </c>
+      <c r="B128" s="6" t="s">
         <v>209</v>
       </c>
-      <c r="B128" s="6" t="s">
-        <v>211</v>
-      </c>
       <c r="C128" s="7" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D128" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E128" s="34">
         <v>0</v>
@@ -9132,16 +9165,16 @@
     </row>
     <row r="129" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A129" s="31" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B129" s="6" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C129" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D129" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E129" s="3">
         <v>0</v>
@@ -9159,6 +9192,15 @@
         <v>0</v>
       </c>
       <c r="J129" s="2">
+        <v>1</v>
+      </c>
+      <c r="X129" s="2">
+        <v>1</v>
+      </c>
+      <c r="Y129" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z129" s="2">
         <v>1</v>
       </c>
       <c r="AA129" s="3">
@@ -9167,12 +9209,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="D2:G2"/>
-    <mergeCell ref="O2:R2"/>
-    <mergeCell ref="S2:T2"/>
-    <mergeCell ref="X2:Z2"/>
-    <mergeCell ref="H2:J2"/>
-    <mergeCell ref="K2:L2"/>
     <mergeCell ref="D1:G1"/>
     <mergeCell ref="M1:N1"/>
     <mergeCell ref="X1:Z1"/>
@@ -9180,6 +9216,12 @@
     <mergeCell ref="O1:R1"/>
     <mergeCell ref="K1:L1"/>
     <mergeCell ref="H1:J1"/>
+    <mergeCell ref="D2:G2"/>
+    <mergeCell ref="O2:R2"/>
+    <mergeCell ref="S2:T2"/>
+    <mergeCell ref="X2:Z2"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="K2:L2"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Checking JSR & INT
</commit_message>
<xml_diff>
--- a/Microroutines.xlsx
+++ b/Microroutines.xlsx
@@ -1,22 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\college\arch\Project\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="13716" yWindow="3732" windowWidth="9324" windowHeight="8616"/>
+    <workbookView xWindow="13710" yWindow="3735" windowWidth="9330" windowHeight="8610"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="207">
   <si>
     <t>Micro instruction</t>
   </si>
@@ -513,7 +508,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
+        <rFont val="Arial"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -528,7 +523,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
+        <rFont val="Arial"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -538,7 +533,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF9C0006"/>
-        <rFont val="Calibri"/>
+        <rFont val="Arial"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -564,9 +559,6 @@
     <t>602</t>
   </si>
   <si>
-    <t>603</t>
-  </si>
-  <si>
     <t>640</t>
   </si>
   <si>
@@ -687,59 +679,59 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1150,56 +1142,56 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AE126"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="86" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A94" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L102" sqref="L102"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="86" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A104" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A124" sqref="A124"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="47.109375" customWidth="1"/>
-    <col min="2" max="2" width="8.77734375" style="5" customWidth="1"/>
-    <col min="3" max="3" width="7.33203125" style="6" customWidth="1"/>
-    <col min="4" max="4" width="2.6640625" style="7" customWidth="1"/>
+    <col min="1" max="1" width="47.125" customWidth="1"/>
+    <col min="2" max="2" width="8.75" style="5" customWidth="1"/>
+    <col min="3" max="3" width="7.375" style="6" customWidth="1"/>
+    <col min="4" max="4" width="2.625" style="7" customWidth="1"/>
     <col min="5" max="5" width="3" style="2" customWidth="1"/>
-    <col min="6" max="6" width="3.109375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="3.77734375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="3.125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="3.75" style="2" customWidth="1"/>
     <col min="8" max="8" width="3" style="30" customWidth="1"/>
-    <col min="9" max="9" width="3.44140625" style="30" customWidth="1"/>
-    <col min="10" max="10" width="2.88671875" style="30" customWidth="1"/>
-    <col min="11" max="11" width="3.21875" style="2" customWidth="1"/>
-    <col min="12" max="12" width="3.6640625" style="2" customWidth="1"/>
-    <col min="13" max="13" width="3.6640625" style="30" customWidth="1"/>
-    <col min="14" max="14" width="3.109375" style="30" customWidth="1"/>
-    <col min="15" max="16" width="3.6640625" style="2" customWidth="1"/>
-    <col min="17" max="17" width="3.44140625" style="2" customWidth="1"/>
-    <col min="18" max="18" width="3.33203125" style="2" customWidth="1"/>
-    <col min="19" max="19" width="3.77734375" style="30" customWidth="1"/>
-    <col min="20" max="20" width="3.44140625" style="30" customWidth="1"/>
+    <col min="9" max="9" width="3.5" style="30" customWidth="1"/>
+    <col min="10" max="10" width="2.875" style="30" customWidth="1"/>
+    <col min="11" max="11" width="3.25" style="2" customWidth="1"/>
+    <col min="12" max="12" width="3.625" style="2" customWidth="1"/>
+    <col min="13" max="13" width="3.625" style="30" customWidth="1"/>
+    <col min="14" max="14" width="3.125" style="30" customWidth="1"/>
+    <col min="15" max="16" width="3.625" style="2" customWidth="1"/>
+    <col min="17" max="17" width="3.5" style="2" customWidth="1"/>
+    <col min="18" max="18" width="3.375" style="2" customWidth="1"/>
+    <col min="19" max="19" width="3.75" style="30" customWidth="1"/>
+    <col min="20" max="20" width="3.5" style="30" customWidth="1"/>
     <col min="21" max="21" width="3" style="2" customWidth="1"/>
-    <col min="22" max="22" width="3.109375" style="30" customWidth="1"/>
-    <col min="23" max="23" width="3.44140625" style="2" customWidth="1"/>
+    <col min="22" max="22" width="3.125" style="30" customWidth="1"/>
+    <col min="23" max="23" width="3.5" style="2" customWidth="1"/>
     <col min="24" max="24" width="4" style="30" customWidth="1"/>
-    <col min="25" max="25" width="3.44140625" style="30" customWidth="1"/>
-    <col min="26" max="26" width="3.6640625" style="30" customWidth="1"/>
-    <col min="27" max="27" width="3.44140625" style="2" customWidth="1"/>
-    <col min="28" max="28" width="3.44140625" style="30" customWidth="1"/>
-    <col min="29" max="29" width="3.44140625" style="25" customWidth="1"/>
-    <col min="30" max="30" width="3.44140625" style="30" customWidth="1"/>
-    <col min="31" max="31" width="30.44140625" style="15" customWidth="1"/>
+    <col min="25" max="25" width="3.5" style="30" customWidth="1"/>
+    <col min="26" max="26" width="3.625" style="30" customWidth="1"/>
+    <col min="27" max="27" width="3.5" style="2" customWidth="1"/>
+    <col min="28" max="28" width="3.5" style="30" customWidth="1"/>
+    <col min="29" max="29" width="3.5" style="25" customWidth="1"/>
+    <col min="30" max="30" width="3.5" style="30" customWidth="1"/>
+    <col min="31" max="31" width="30.5" style="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:31">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1207,7 +1199,7 @@
         <v>7</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D1" s="31" t="s">
         <v>46</v>
@@ -1259,16 +1251,16 @@
         <v>154</v>
       </c>
       <c r="AC1" s="25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="AD1" s="30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="AE1" s="14" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:31">
       <c r="D2" s="31"/>
       <c r="E2" s="31"/>
       <c r="F2" s="31"/>
@@ -1288,7 +1280,7 @@
       <c r="Y2" s="32"/>
       <c r="Z2" s="32"/>
     </row>
-    <row r="3" spans="1:31" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:31" s="8" customFormat="1">
       <c r="A3" s="8" t="s">
         <v>79</v>
       </c>
@@ -1323,9 +1315,9 @@
       <c r="AD3" s="30"/>
       <c r="AE3" s="16"/>
     </row>
-    <row r="4" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:31" s="1" customFormat="1">
       <c r="A4" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>9</v>
@@ -1416,9 +1408,9 @@
       </c>
       <c r="AE4" s="17"/>
     </row>
-    <row r="5" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:31" s="1" customFormat="1">
       <c r="A5" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>10</v>
@@ -1509,7 +1501,7 @@
       </c>
       <c r="AE5" s="17"/>
     </row>
-    <row r="6" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:31" s="1" customFormat="1">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -1602,7 +1594,7 @@
       </c>
       <c r="AE6" s="17"/>
     </row>
-    <row r="7" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:31" s="1" customFormat="1">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1695,7 +1687,7 @@
       </c>
       <c r="AE7" s="17"/>
     </row>
-    <row r="8" spans="1:31" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:31" s="8" customFormat="1">
       <c r="A8" s="8" t="s">
         <v>78</v>
       </c>
@@ -1734,7 +1726,7 @@
       </c>
       <c r="AE8" s="16"/>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:31">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1745,7 +1737,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:31">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -1837,7 +1829,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:31">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -1929,7 +1921,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:31">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -2021,7 +2013,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:31">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -2113,7 +2105,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:31">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -2205,7 +2197,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:31">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -2297,7 +2289,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:31">
       <c r="A16" t="s">
         <v>28</v>
       </c>
@@ -2389,7 +2381,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:31">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -2481,7 +2473,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:31">
       <c r="A18" t="s">
         <v>33</v>
       </c>
@@ -2573,7 +2565,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:31">
       <c r="A19" t="s">
         <v>32</v>
       </c>
@@ -2665,7 +2657,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:31">
       <c r="A20" t="s">
         <v>35</v>
       </c>
@@ -2757,7 +2749,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:31">
       <c r="A21" t="s">
         <v>37</v>
       </c>
@@ -2849,7 +2841,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:31">
       <c r="A22" t="s">
         <v>39</v>
       </c>
@@ -2941,7 +2933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:31">
       <c r="A23" t="s">
         <v>19</v>
       </c>
@@ -3036,7 +3028,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="24" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:31">
       <c r="A24" t="s">
         <v>42</v>
       </c>
@@ -3128,7 +3120,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:31">
       <c r="A25" t="s">
         <v>19</v>
       </c>
@@ -3220,7 +3212,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:31">
       <c r="A26" t="s">
         <v>45</v>
       </c>
@@ -3312,7 +3304,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:31" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:31" s="8" customFormat="1">
       <c r="A27" s="8" t="s">
         <v>104</v>
       </c>
@@ -3351,7 +3343,7 @@
       </c>
       <c r="AE27" s="16"/>
     </row>
-    <row r="28" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:31">
       <c r="A28" t="s">
         <v>61</v>
       </c>
@@ -3443,7 +3435,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:31">
       <c r="A29" t="s">
         <v>54</v>
       </c>
@@ -3535,7 +3527,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:31">
       <c r="A30" t="s">
         <v>19</v>
       </c>
@@ -3627,7 +3619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:31">
       <c r="A31" t="s">
         <v>56</v>
       </c>
@@ -3719,7 +3711,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:31">
       <c r="A32" t="s">
         <v>57</v>
       </c>
@@ -3811,7 +3803,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:31">
       <c r="A33" t="s">
         <v>58</v>
       </c>
@@ -3903,7 +3895,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:31">
       <c r="A34" t="s">
         <v>59</v>
       </c>
@@ -3995,7 +3987,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:31">
       <c r="A35" t="s">
         <v>19</v>
       </c>
@@ -4087,7 +4079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:31">
       <c r="A36" t="s">
         <v>33</v>
       </c>
@@ -4179,7 +4171,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:31">
       <c r="A37" t="s">
         <v>32</v>
       </c>
@@ -4271,7 +4263,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:31">
       <c r="A38" t="s">
         <v>35</v>
       </c>
@@ -4363,7 +4355,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:31">
       <c r="A39" t="s">
         <v>60</v>
       </c>
@@ -4455,7 +4447,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:31">
       <c r="A40" t="s">
         <v>39</v>
       </c>
@@ -4547,7 +4539,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:31">
       <c r="A41" t="s">
         <v>19</v>
       </c>
@@ -4642,7 +4634,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="42" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:31">
       <c r="A42" t="s">
         <v>42</v>
       </c>
@@ -4734,7 +4726,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:31">
       <c r="A43" t="s">
         <v>19</v>
       </c>
@@ -4826,7 +4818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:31">
       <c r="A44" t="s">
         <v>62</v>
       </c>
@@ -4921,7 +4913,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="45" spans="1:31" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:31" s="8" customFormat="1">
       <c r="A45" s="8" t="s">
         <v>101</v>
       </c>
@@ -4960,7 +4952,7 @@
       </c>
       <c r="AE45" s="16"/>
     </row>
-    <row r="46" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:31">
       <c r="A46" s="10" t="s">
         <v>77</v>
       </c>
@@ -5010,7 +5002,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:31">
       <c r="A47" s="12" t="s">
         <v>81</v>
       </c>
@@ -5027,7 +5019,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:31">
       <c r="A48" s="12" t="s">
         <v>161</v>
       </c>
@@ -5095,7 +5087,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:30">
       <c r="A49" s="10" t="s">
         <v>82</v>
       </c>
@@ -5123,7 +5115,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:30">
       <c r="A50" s="10" t="s">
         <v>80</v>
       </c>
@@ -5191,7 +5183,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:30">
       <c r="A51" s="12" t="s">
         <v>83</v>
       </c>
@@ -5220,7 +5212,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:30">
       <c r="A52" s="12" t="s">
         <v>86</v>
       </c>
@@ -5288,7 +5280,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:30">
       <c r="A53" s="10" t="s">
         <v>84</v>
       </c>
@@ -5316,7 +5308,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:30">
       <c r="A54" s="10" t="s">
         <v>90</v>
       </c>
@@ -5384,7 +5376,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:30">
       <c r="A55" s="12" t="s">
         <v>85</v>
       </c>
@@ -5401,7 +5393,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:30">
       <c r="A56" s="12" t="s">
         <v>91</v>
       </c>
@@ -5469,7 +5461,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:30">
       <c r="A57" s="10" t="s">
         <v>87</v>
       </c>
@@ -5486,7 +5478,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:30">
       <c r="A58" s="10" t="s">
         <v>92</v>
       </c>
@@ -5554,7 +5546,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:30">
       <c r="A59" s="12" t="s">
         <v>88</v>
       </c>
@@ -5571,7 +5563,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:30">
       <c r="A60" s="12" t="s">
         <v>93</v>
       </c>
@@ -5639,7 +5631,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:30">
       <c r="A61" s="10" t="s">
         <v>89</v>
       </c>
@@ -5656,7 +5648,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:30">
       <c r="A62" s="10" t="s">
         <v>94</v>
       </c>
@@ -5724,7 +5716,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:30">
       <c r="A63" s="12" t="s">
         <v>95</v>
       </c>
@@ -5741,7 +5733,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:30">
       <c r="A64" s="12" t="s">
         <v>90</v>
       </c>
@@ -5812,7 +5804,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:31" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:31" s="8" customFormat="1">
       <c r="A65" s="8" t="s">
         <v>148</v>
       </c>
@@ -5851,7 +5843,7 @@
       </c>
       <c r="AE65" s="16"/>
     </row>
-    <row r="66" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:31">
       <c r="B66" s="5" t="s">
         <v>119</v>
       </c>
@@ -5877,7 +5869,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:31">
       <c r="A67" s="10" t="s">
         <v>121</v>
       </c>
@@ -5903,7 +5895,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:31">
       <c r="A68" s="10" t="s">
         <v>127</v>
       </c>
@@ -5974,7 +5966,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:31">
       <c r="A69" s="12" t="s">
         <v>122</v>
       </c>
@@ -6000,7 +5992,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:31">
       <c r="A70" s="12" t="s">
         <v>128</v>
       </c>
@@ -6068,7 +6060,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:31">
       <c r="A71" s="10" t="s">
         <v>123</v>
       </c>
@@ -6082,7 +6074,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:31">
       <c r="A72" s="10" t="s">
         <v>160</v>
       </c>
@@ -6135,7 +6127,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:31">
       <c r="A73" s="12" t="s">
         <v>124</v>
       </c>
@@ -6149,7 +6141,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:31">
       <c r="A74" s="12" t="s">
         <v>129</v>
       </c>
@@ -6217,7 +6209,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="75" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:31">
       <c r="A75" s="10" t="s">
         <v>126</v>
       </c>
@@ -6234,7 +6226,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="76" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:31">
       <c r="A76" s="10" t="s">
         <v>133</v>
       </c>
@@ -6302,7 +6294,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="77" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:31">
       <c r="A77" s="12" t="s">
         <v>131</v>
       </c>
@@ -6319,7 +6311,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="78" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:31">
       <c r="A78" s="12" t="s">
         <v>132</v>
       </c>
@@ -6387,7 +6379,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="79" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:31">
       <c r="A79" s="10" t="s">
         <v>134</v>
       </c>
@@ -6404,7 +6396,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="80" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:31">
       <c r="A80" s="10" t="s">
         <v>135</v>
       </c>
@@ -6472,7 +6464,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="81" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:31">
       <c r="A81" s="12" t="s">
         <v>136</v>
       </c>
@@ -6489,7 +6481,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="82" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:31">
       <c r="A82" s="12" t="s">
         <v>137</v>
       </c>
@@ -6557,7 +6549,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="83" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:31">
       <c r="A83" s="10" t="s">
         <v>138</v>
       </c>
@@ -6574,7 +6566,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="84" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:31">
       <c r="A84" s="10" t="s">
         <v>139</v>
       </c>
@@ -6642,7 +6634,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="85" spans="1:31" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:31" s="8" customFormat="1">
       <c r="A85" s="8" t="s">
         <v>96</v>
       </c>
@@ -6681,7 +6673,7 @@
       </c>
       <c r="AE85" s="16"/>
     </row>
-    <row r="86" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:31">
       <c r="A86" t="s">
         <v>97</v>
       </c>
@@ -6722,7 +6714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:31">
       <c r="A87" t="s">
         <v>98</v>
       </c>
@@ -6763,7 +6755,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="88" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:31">
       <c r="A88" t="s">
         <v>99</v>
       </c>
@@ -6816,7 +6808,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:31" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:31" s="8" customFormat="1">
       <c r="A89" s="8" t="s">
         <v>149</v>
       </c>
@@ -6855,7 +6847,7 @@
       </c>
       <c r="AE89" s="16"/>
     </row>
-    <row r="90" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:31">
       <c r="A90" s="10" t="s">
         <v>152</v>
       </c>
@@ -6869,7 +6861,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:31">
       <c r="A91" s="10" t="s">
         <v>153</v>
       </c>
@@ -6883,7 +6875,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:31">
       <c r="A92" t="s">
         <v>151</v>
       </c>
@@ -6894,7 +6886,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:31">
       <c r="B93" s="5" t="s">
         <v>150</v>
       </c>
@@ -6908,7 +6900,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:31" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:31" s="8" customFormat="1">
       <c r="A94" s="8" t="s">
         <v>155</v>
       </c>
@@ -6947,7 +6939,7 @@
       </c>
       <c r="AE94" s="16"/>
     </row>
-    <row r="95" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:31">
       <c r="A95" s="24" t="s">
         <v>156</v>
       </c>
@@ -6976,7 +6968,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:31">
       <c r="A96" t="s">
         <v>157</v>
       </c>
@@ -7020,7 +7012,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:31">
       <c r="A97" t="s">
         <v>158</v>
       </c>
@@ -7064,7 +7056,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:31" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:31" s="8" customFormat="1">
       <c r="A98" s="8" t="s">
         <v>159</v>
       </c>
@@ -7103,9 +7095,9 @@
       </c>
       <c r="AE98" s="16"/>
     </row>
-    <row r="99" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:31">
       <c r="A99" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="AC99" s="28">
         <v>0</v>
@@ -7114,7 +7106,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:31">
       <c r="A100" s="10" t="s">
         <v>164</v>
       </c>
@@ -7125,13 +7117,13 @@
         <v>163</v>
       </c>
       <c r="D100" s="29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E100" s="2">
         <v>0</v>
       </c>
       <c r="F100" s="29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G100" s="29">
         <v>0</v>
@@ -7140,10 +7132,10 @@
         <v>0</v>
       </c>
       <c r="I100" s="30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J100" s="30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K100" s="29">
         <v>0</v>
@@ -7167,7 +7159,7 @@
         <v>0</v>
       </c>
       <c r="R100" s="29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S100" s="30">
         <v>0</v>
@@ -7176,7 +7168,7 @@
         <v>0</v>
       </c>
       <c r="U100" s="29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V100" s="30">
         <v>0</v>
@@ -7206,7 +7198,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:31">
       <c r="A101" s="10" t="s">
         <v>165</v>
       </c>
@@ -7223,16 +7215,16 @@
         <v>0</v>
       </c>
       <c r="F101" s="29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G101" s="29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H101" s="30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I101" s="30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J101" s="30">
         <v>0</v>
@@ -7241,7 +7233,7 @@
         <v>0</v>
       </c>
       <c r="L101" s="29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M101" s="30">
         <v>0</v>
@@ -7298,9 +7290,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:31">
       <c r="A102" s="10" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B102" s="5" t="s">
         <v>166</v>
@@ -7318,7 +7310,7 @@
         <v>0</v>
       </c>
       <c r="G102" s="29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H102" s="30">
         <v>0</v>
@@ -7330,7 +7322,7 @@
         <v>0</v>
       </c>
       <c r="K102" s="29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L102" s="29">
         <v>0</v>
@@ -7390,392 +7382,392 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:31">
       <c r="A103" s="10" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B103" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="C103" s="6" t="s">
+      <c r="C103" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="D103" s="29">
+        <v>1</v>
+      </c>
+      <c r="E103" s="29">
+        <v>0</v>
+      </c>
+      <c r="F103" s="29">
+        <v>0</v>
+      </c>
+      <c r="G103" s="29">
+        <v>1</v>
+      </c>
+      <c r="H103" s="30">
+        <v>0</v>
+      </c>
+      <c r="I103" s="30">
+        <v>0</v>
+      </c>
+      <c r="J103" s="30">
+        <v>1</v>
+      </c>
+      <c r="K103" s="29">
+        <v>0</v>
+      </c>
+      <c r="L103" s="29">
+        <v>0</v>
+      </c>
+      <c r="M103" s="30">
+        <v>0</v>
+      </c>
+      <c r="N103" s="30">
+        <v>0</v>
+      </c>
+      <c r="O103" s="29">
+        <v>0</v>
+      </c>
+      <c r="P103" s="29">
+        <v>0</v>
+      </c>
+      <c r="Q103" s="29">
+        <v>0</v>
+      </c>
+      <c r="R103" s="29">
+        <v>0</v>
+      </c>
+      <c r="S103" s="30">
+        <v>1</v>
+      </c>
+      <c r="T103" s="30">
+        <v>0</v>
+      </c>
+      <c r="U103" s="29">
+        <v>0</v>
+      </c>
+      <c r="V103" s="30">
+        <v>0</v>
+      </c>
+      <c r="W103" s="29">
+        <v>0</v>
+      </c>
+      <c r="X103" s="30">
+        <v>1</v>
+      </c>
+      <c r="Y103" s="30">
+        <v>1</v>
+      </c>
+      <c r="Z103" s="30">
+        <v>1</v>
+      </c>
+      <c r="AA103" s="29">
+        <v>0</v>
+      </c>
+      <c r="AB103" s="30">
+        <v>0</v>
+      </c>
+      <c r="AC103" s="29">
+        <v>0</v>
+      </c>
+      <c r="AD103" s="30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:31">
+      <c r="A104" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="AC104" s="28">
+        <v>0</v>
+      </c>
+      <c r="AD104" s="30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:31">
+      <c r="A105" s="10" t="s">
+        <v>171</v>
+      </c>
+      <c r="B105" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="D103" s="29">
-        <v>0</v>
-      </c>
-      <c r="E103" s="29">
-        <v>0</v>
-      </c>
-      <c r="F103" s="29">
-        <v>0</v>
-      </c>
-      <c r="G103" s="29">
-        <v>0</v>
-      </c>
-      <c r="H103" s="30">
-        <v>0</v>
-      </c>
-      <c r="I103" s="30">
-        <v>0</v>
-      </c>
-      <c r="J103" s="30">
-        <v>0</v>
-      </c>
-      <c r="K103" s="29">
-        <v>0</v>
-      </c>
-      <c r="L103" s="29">
-        <v>0</v>
-      </c>
-      <c r="M103" s="30">
-        <v>0</v>
-      </c>
-      <c r="N103" s="30">
-        <v>0</v>
-      </c>
-      <c r="O103" s="29">
-        <v>0</v>
-      </c>
-      <c r="P103" s="29">
-        <v>0</v>
-      </c>
-      <c r="Q103" s="29">
-        <v>0</v>
-      </c>
-      <c r="R103" s="29">
-        <v>0</v>
-      </c>
-      <c r="S103" s="30">
-        <v>0</v>
-      </c>
-      <c r="T103" s="30">
-        <v>0</v>
-      </c>
-      <c r="U103" s="29">
-        <v>0</v>
-      </c>
-      <c r="V103" s="30">
-        <v>0</v>
-      </c>
-      <c r="W103" s="29">
-        <v>0</v>
-      </c>
-      <c r="X103" s="30">
-        <v>0</v>
-      </c>
-      <c r="Y103" s="30">
-        <v>0</v>
-      </c>
-      <c r="Z103" s="30">
-        <v>0</v>
-      </c>
-      <c r="AA103" s="29">
-        <v>0</v>
-      </c>
-      <c r="AB103" s="30">
-        <v>0</v>
-      </c>
-      <c r="AC103" s="29">
-        <v>0</v>
-      </c>
-      <c r="AD103" s="30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="104" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A104" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="AC104" s="28">
-        <v>0</v>
-      </c>
-      <c r="AD104" s="30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="105" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A105" s="10" t="s">
+      <c r="C105" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="D105" s="29">
+        <v>1</v>
+      </c>
+      <c r="E105" s="2">
+        <v>0</v>
+      </c>
+      <c r="F105" s="29">
+        <v>1</v>
+      </c>
+      <c r="G105" s="29">
+        <v>0</v>
+      </c>
+      <c r="H105" s="30">
+        <v>0</v>
+      </c>
+      <c r="I105" s="30">
+        <v>1</v>
+      </c>
+      <c r="J105" s="30">
+        <v>1</v>
+      </c>
+      <c r="K105" s="29">
+        <v>0</v>
+      </c>
+      <c r="L105" s="29">
+        <v>1</v>
+      </c>
+      <c r="M105" s="30">
+        <v>0</v>
+      </c>
+      <c r="N105" s="30">
+        <v>0</v>
+      </c>
+      <c r="O105" s="29">
+        <v>0</v>
+      </c>
+      <c r="P105" s="29">
+        <v>0</v>
+      </c>
+      <c r="Q105" s="29">
+        <v>0</v>
+      </c>
+      <c r="R105" s="29">
+        <v>0</v>
+      </c>
+      <c r="S105" s="30">
+        <v>0</v>
+      </c>
+      <c r="T105" s="30">
+        <v>0</v>
+      </c>
+      <c r="U105" s="29">
+        <v>1</v>
+      </c>
+      <c r="V105" s="30">
+        <v>1</v>
+      </c>
+      <c r="W105" s="29">
+        <v>0</v>
+      </c>
+      <c r="X105" s="30">
+        <v>0</v>
+      </c>
+      <c r="Y105" s="30">
+        <v>0</v>
+      </c>
+      <c r="Z105" s="30">
+        <v>0</v>
+      </c>
+      <c r="AA105" s="29">
+        <v>0</v>
+      </c>
+      <c r="AB105" s="30">
+        <v>0</v>
+      </c>
+      <c r="AC105" s="29">
+        <v>0</v>
+      </c>
+      <c r="AD105" s="30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:31">
+      <c r="A106" s="10" t="s">
         <v>172</v>
       </c>
-      <c r="B105" s="5" t="s">
-        <v>169</v>
-      </c>
-      <c r="C105" s="6" t="s">
+      <c r="B106" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="C106" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="D105" s="29">
-        <v>0</v>
-      </c>
-      <c r="E105" s="2">
-        <v>0</v>
-      </c>
-      <c r="F105" s="29">
-        <v>0</v>
-      </c>
-      <c r="G105" s="29">
-        <v>0</v>
-      </c>
-      <c r="H105" s="30">
-        <v>0</v>
-      </c>
-      <c r="I105" s="30">
-        <v>0</v>
-      </c>
-      <c r="J105" s="30">
-        <v>0</v>
-      </c>
-      <c r="K105" s="29">
-        <v>0</v>
-      </c>
-      <c r="L105" s="29">
-        <v>0</v>
-      </c>
-      <c r="M105" s="30">
-        <v>0</v>
-      </c>
-      <c r="N105" s="30">
-        <v>0</v>
-      </c>
-      <c r="O105" s="29">
-        <v>0</v>
-      </c>
-      <c r="P105" s="29">
-        <v>0</v>
-      </c>
-      <c r="Q105" s="29">
-        <v>0</v>
-      </c>
-      <c r="R105" s="29">
-        <v>0</v>
-      </c>
-      <c r="S105" s="30">
-        <v>0</v>
-      </c>
-      <c r="T105" s="30">
-        <v>0</v>
-      </c>
-      <c r="U105" s="29">
-        <v>0</v>
-      </c>
-      <c r="V105" s="30">
-        <v>0</v>
-      </c>
-      <c r="W105" s="29">
-        <v>0</v>
-      </c>
-      <c r="X105" s="30">
-        <v>0</v>
-      </c>
-      <c r="Y105" s="30">
-        <v>0</v>
-      </c>
-      <c r="Z105" s="30">
-        <v>0</v>
-      </c>
-      <c r="AA105" s="29">
-        <v>0</v>
-      </c>
-      <c r="AB105" s="30">
-        <v>0</v>
-      </c>
-      <c r="AC105" s="29">
-        <v>0</v>
-      </c>
-      <c r="AD105" s="30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="106" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A106" s="10" t="s">
-        <v>173</v>
-      </c>
-      <c r="B106" s="5" t="s">
+      <c r="D106" s="29">
+        <v>0</v>
+      </c>
+      <c r="E106" s="29">
+        <v>0</v>
+      </c>
+      <c r="F106" s="29">
+        <v>0</v>
+      </c>
+      <c r="G106" s="29">
+        <v>0</v>
+      </c>
+      <c r="H106" s="30">
+        <v>0</v>
+      </c>
+      <c r="I106" s="30">
+        <v>0</v>
+      </c>
+      <c r="J106" s="30">
+        <v>0</v>
+      </c>
+      <c r="K106" s="29">
+        <v>1</v>
+      </c>
+      <c r="L106" s="29">
+        <v>0</v>
+      </c>
+      <c r="M106" s="30">
+        <v>0</v>
+      </c>
+      <c r="N106" s="30">
+        <v>0</v>
+      </c>
+      <c r="O106" s="29">
+        <v>0</v>
+      </c>
+      <c r="P106" s="29">
+        <v>0</v>
+      </c>
+      <c r="Q106" s="29">
+        <v>0</v>
+      </c>
+      <c r="R106" s="29">
+        <v>0</v>
+      </c>
+      <c r="S106" s="30">
+        <v>0</v>
+      </c>
+      <c r="T106" s="30">
+        <v>1</v>
+      </c>
+      <c r="U106" s="29">
+        <v>0</v>
+      </c>
+      <c r="V106" s="30">
+        <v>0</v>
+      </c>
+      <c r="W106" s="29">
+        <v>0</v>
+      </c>
+      <c r="X106" s="30">
+        <v>0</v>
+      </c>
+      <c r="Y106" s="30">
+        <v>0</v>
+      </c>
+      <c r="Z106" s="30">
+        <v>0</v>
+      </c>
+      <c r="AA106" s="29">
+        <v>0</v>
+      </c>
+      <c r="AB106" s="30">
+        <v>0</v>
+      </c>
+      <c r="AC106" s="29">
+        <v>0</v>
+      </c>
+      <c r="AD106" s="30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:31">
+      <c r="A107" s="10" t="s">
+        <v>192</v>
+      </c>
+      <c r="B107" s="5" t="s">
         <v>174</v>
       </c>
-      <c r="C106" s="6" t="s">
+      <c r="C107" s="6" t="s">
         <v>175</v>
       </c>
-      <c r="D106" s="29">
-        <v>0</v>
-      </c>
-      <c r="E106" s="29">
-        <v>0</v>
-      </c>
-      <c r="F106" s="29">
-        <v>0</v>
-      </c>
-      <c r="G106" s="29">
-        <v>0</v>
-      </c>
-      <c r="H106" s="30">
-        <v>0</v>
-      </c>
-      <c r="I106" s="30">
-        <v>0</v>
-      </c>
-      <c r="J106" s="30">
-        <v>0</v>
-      </c>
-      <c r="K106" s="29">
-        <v>0</v>
-      </c>
-      <c r="L106" s="29">
-        <v>0</v>
-      </c>
-      <c r="M106" s="30">
-        <v>0</v>
-      </c>
-      <c r="N106" s="30">
-        <v>0</v>
-      </c>
-      <c r="O106" s="29">
-        <v>0</v>
-      </c>
-      <c r="P106" s="29">
-        <v>0</v>
-      </c>
-      <c r="Q106" s="29">
-        <v>0</v>
-      </c>
-      <c r="R106" s="29">
-        <v>0</v>
-      </c>
-      <c r="S106" s="30">
-        <v>0</v>
-      </c>
-      <c r="T106" s="30">
-        <v>0</v>
-      </c>
-      <c r="U106" s="29">
-        <v>0</v>
-      </c>
-      <c r="V106" s="30">
-        <v>0</v>
-      </c>
-      <c r="W106" s="29">
-        <v>0</v>
-      </c>
-      <c r="X106" s="30">
-        <v>0</v>
-      </c>
-      <c r="Y106" s="30">
-        <v>0</v>
-      </c>
-      <c r="Z106" s="30">
-        <v>0</v>
-      </c>
-      <c r="AA106" s="29">
-        <v>0</v>
-      </c>
-      <c r="AB106" s="30">
-        <v>0</v>
-      </c>
-      <c r="AC106" s="29">
-        <v>0</v>
-      </c>
-      <c r="AD106" s="30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="107" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A107" s="10" t="s">
-        <v>193</v>
-      </c>
-      <c r="B107" s="5" t="s">
+      <c r="D107" s="29">
+        <v>0</v>
+      </c>
+      <c r="E107" s="29">
+        <v>0</v>
+      </c>
+      <c r="F107" s="29">
+        <v>1</v>
+      </c>
+      <c r="G107" s="29">
+        <v>0</v>
+      </c>
+      <c r="H107" s="30">
+        <v>0</v>
+      </c>
+      <c r="I107" s="30">
+        <v>0</v>
+      </c>
+      <c r="J107" s="30">
+        <v>1</v>
+      </c>
+      <c r="K107" s="29">
+        <v>0</v>
+      </c>
+      <c r="L107" s="29">
+        <v>0</v>
+      </c>
+      <c r="M107" s="30">
+        <v>0</v>
+      </c>
+      <c r="N107" s="30">
+        <v>0</v>
+      </c>
+      <c r="O107" s="29">
+        <v>0</v>
+      </c>
+      <c r="P107" s="29">
+        <v>0</v>
+      </c>
+      <c r="Q107" s="29">
+        <v>0</v>
+      </c>
+      <c r="R107" s="29">
+        <v>0</v>
+      </c>
+      <c r="S107" s="30">
+        <v>0</v>
+      </c>
+      <c r="T107" s="30">
+        <v>0</v>
+      </c>
+      <c r="U107" s="29">
+        <v>0</v>
+      </c>
+      <c r="V107" s="30">
+        <v>0</v>
+      </c>
+      <c r="W107" s="29">
+        <v>0</v>
+      </c>
+      <c r="X107" s="30">
+        <v>0</v>
+      </c>
+      <c r="Y107" s="30">
+        <v>0</v>
+      </c>
+      <c r="Z107" s="30">
+        <v>0</v>
+      </c>
+      <c r="AA107" s="29">
+        <v>0</v>
+      </c>
+      <c r="AB107" s="30">
+        <v>0</v>
+      </c>
+      <c r="AC107" s="29">
+        <v>0</v>
+      </c>
+      <c r="AD107" s="30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:31">
+      <c r="A108" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="B108" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="C107" s="6" t="s">
-        <v>176</v>
-      </c>
-      <c r="D107" s="29">
-        <v>0</v>
-      </c>
-      <c r="E107" s="29">
-        <v>0</v>
-      </c>
-      <c r="F107" s="29">
-        <v>0</v>
-      </c>
-      <c r="G107" s="29">
-        <v>0</v>
-      </c>
-      <c r="H107" s="30">
-        <v>0</v>
-      </c>
-      <c r="I107" s="30">
-        <v>0</v>
-      </c>
-      <c r="J107" s="30">
-        <v>0</v>
-      </c>
-      <c r="K107" s="29">
-        <v>0</v>
-      </c>
-      <c r="L107" s="29">
-        <v>0</v>
-      </c>
-      <c r="M107" s="30">
-        <v>0</v>
-      </c>
-      <c r="N107" s="30">
-        <v>0</v>
-      </c>
-      <c r="O107" s="29">
-        <v>0</v>
-      </c>
-      <c r="P107" s="29">
-        <v>0</v>
-      </c>
-      <c r="Q107" s="29">
-        <v>0</v>
-      </c>
-      <c r="R107" s="29">
-        <v>0</v>
-      </c>
-      <c r="S107" s="30">
-        <v>0</v>
-      </c>
-      <c r="T107" s="30">
-        <v>0</v>
-      </c>
-      <c r="U107" s="29">
-        <v>0</v>
-      </c>
-      <c r="V107" s="30">
-        <v>0</v>
-      </c>
-      <c r="W107" s="29">
-        <v>0</v>
-      </c>
-      <c r="X107" s="30">
-        <v>0</v>
-      </c>
-      <c r="Y107" s="30">
-        <v>0</v>
-      </c>
-      <c r="Z107" s="30">
-        <v>0</v>
-      </c>
-      <c r="AA107" s="29">
-        <v>0</v>
-      </c>
-      <c r="AB107" s="30">
-        <v>0</v>
-      </c>
-      <c r="AC107" s="29">
-        <v>0</v>
-      </c>
-      <c r="AD107" s="30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="108" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A108" s="10" t="s">
-        <v>200</v>
-      </c>
-      <c r="B108" s="5" t="s">
-        <v>176</v>
-      </c>
       <c r="C108" s="6" t="s">
         <v>13</v>
       </c>
@@ -7786,16 +7778,16 @@
         <v>0</v>
       </c>
       <c r="F108" s="29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G108" s="29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H108" s="30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I108" s="30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J108" s="30">
         <v>0</v>
@@ -7840,13 +7832,13 @@
         <v>0</v>
       </c>
       <c r="X108" s="30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y108" s="30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z108" s="30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA108" s="29">
         <v>0</v>
@@ -7861,9 +7853,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:31">
       <c r="A109" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="AC109" s="28">
         <v>0</v>
@@ -7872,15 +7864,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:31">
       <c r="A110" s="10" t="s">
         <v>164</v>
       </c>
       <c r="B110" s="5" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C110" s="6" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D110" s="7" t="s">
         <v>14</v>
@@ -7964,199 +7956,199 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:31">
       <c r="A111" s="10" t="s">
         <v>165</v>
       </c>
       <c r="B111" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="C111" s="6" t="s">
         <v>184</v>
       </c>
-      <c r="C111" s="6" t="s">
+      <c r="D111" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E111" s="2">
+        <v>0</v>
+      </c>
+      <c r="F111" s="2">
+        <v>1</v>
+      </c>
+      <c r="G111" s="2">
+        <v>1</v>
+      </c>
+      <c r="H111" s="30">
+        <v>1</v>
+      </c>
+      <c r="I111" s="30">
+        <v>1</v>
+      </c>
+      <c r="J111" s="30">
+        <v>0</v>
+      </c>
+      <c r="K111" s="2">
+        <v>0</v>
+      </c>
+      <c r="L111" s="2">
+        <v>1</v>
+      </c>
+      <c r="M111" s="30">
+        <v>0</v>
+      </c>
+      <c r="N111" s="30">
+        <v>0</v>
+      </c>
+      <c r="O111" s="2">
+        <v>0</v>
+      </c>
+      <c r="P111" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q111" s="2">
+        <v>0</v>
+      </c>
+      <c r="R111" s="2">
+        <v>0</v>
+      </c>
+      <c r="S111" s="30">
+        <v>0</v>
+      </c>
+      <c r="T111" s="30">
+        <v>0</v>
+      </c>
+      <c r="U111" s="2">
+        <v>0</v>
+      </c>
+      <c r="V111" s="30">
+        <v>0</v>
+      </c>
+      <c r="W111" s="2">
+        <v>0</v>
+      </c>
+      <c r="X111" s="30">
+        <v>0</v>
+      </c>
+      <c r="Y111" s="30">
+        <v>0</v>
+      </c>
+      <c r="Z111" s="30">
+        <v>0</v>
+      </c>
+      <c r="AA111" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB111" s="30">
+        <v>0</v>
+      </c>
+      <c r="AC111" s="28">
+        <v>0</v>
+      </c>
+      <c r="AD111" s="30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:31">
+      <c r="A112" s="10" t="s">
+        <v>180</v>
+      </c>
+      <c r="B112" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="C112" s="6" t="s">
         <v>185</v>
       </c>
-      <c r="D111" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E111" s="2">
-        <v>0</v>
-      </c>
-      <c r="F111" s="2">
-        <v>1</v>
-      </c>
-      <c r="G111" s="2">
-        <v>1</v>
-      </c>
-      <c r="H111" s="30">
-        <v>1</v>
-      </c>
-      <c r="I111" s="30">
-        <v>1</v>
-      </c>
-      <c r="J111" s="30">
-        <v>0</v>
-      </c>
-      <c r="K111" s="2">
-        <v>0</v>
-      </c>
-      <c r="L111" s="2">
-        <v>1</v>
-      </c>
-      <c r="M111" s="30">
-        <v>0</v>
-      </c>
-      <c r="N111" s="30">
-        <v>0</v>
-      </c>
-      <c r="O111" s="2">
-        <v>0</v>
-      </c>
-      <c r="P111" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q111" s="2">
-        <v>0</v>
-      </c>
-      <c r="R111" s="2">
-        <v>0</v>
-      </c>
-      <c r="S111" s="30">
-        <v>0</v>
-      </c>
-      <c r="T111" s="30">
-        <v>0</v>
-      </c>
-      <c r="U111" s="2">
-        <v>0</v>
-      </c>
-      <c r="V111" s="30">
-        <v>0</v>
-      </c>
-      <c r="W111" s="2">
-        <v>0</v>
-      </c>
-      <c r="X111" s="30">
-        <v>0</v>
-      </c>
-      <c r="Y111" s="30">
-        <v>0</v>
-      </c>
-      <c r="Z111" s="30">
-        <v>0</v>
-      </c>
-      <c r="AA111" s="2">
-        <v>0</v>
-      </c>
-      <c r="AB111" s="30">
-        <v>0</v>
-      </c>
-      <c r="AC111" s="28">
-        <v>0</v>
-      </c>
-      <c r="AD111" s="30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="112" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A112" s="10" t="s">
+      <c r="D112" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E112" s="2">
+        <v>0</v>
+      </c>
+      <c r="F112" s="2">
+        <v>0</v>
+      </c>
+      <c r="G112" s="2">
+        <v>1</v>
+      </c>
+      <c r="H112" s="30">
+        <v>0</v>
+      </c>
+      <c r="I112" s="30">
+        <v>0</v>
+      </c>
+      <c r="J112" s="30">
+        <v>0</v>
+      </c>
+      <c r="K112" s="2">
+        <v>1</v>
+      </c>
+      <c r="L112" s="2">
+        <v>0</v>
+      </c>
+      <c r="M112" s="30">
+        <v>0</v>
+      </c>
+      <c r="N112" s="30">
+        <v>0</v>
+      </c>
+      <c r="O112" s="2">
+        <v>0</v>
+      </c>
+      <c r="P112" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q112" s="2">
+        <v>0</v>
+      </c>
+      <c r="R112" s="2">
+        <v>0</v>
+      </c>
+      <c r="S112" s="30">
+        <v>0</v>
+      </c>
+      <c r="T112" s="30">
+        <v>0</v>
+      </c>
+      <c r="U112" s="2">
+        <v>0</v>
+      </c>
+      <c r="V112" s="30">
+        <v>0</v>
+      </c>
+      <c r="W112" s="2">
+        <v>0</v>
+      </c>
+      <c r="X112" s="30">
+        <v>0</v>
+      </c>
+      <c r="Y112" s="30">
+        <v>0</v>
+      </c>
+      <c r="Z112" s="30">
+        <v>0</v>
+      </c>
+      <c r="AA112" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB112" s="30">
+        <v>0</v>
+      </c>
+      <c r="AC112" s="28">
+        <v>0</v>
+      </c>
+      <c r="AD112" s="30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:30">
+      <c r="A113" s="10" t="s">
         <v>181</v>
       </c>
-      <c r="B112" s="5" t="s">
+      <c r="B113" s="5" t="s">
         <v>185</v>
       </c>
-      <c r="C112" s="6" t="s">
+      <c r="C113" s="6" t="s">
         <v>186</v>
-      </c>
-      <c r="D112" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E112" s="2">
-        <v>0</v>
-      </c>
-      <c r="F112" s="2">
-        <v>0</v>
-      </c>
-      <c r="G112" s="2">
-        <v>1</v>
-      </c>
-      <c r="H112" s="30">
-        <v>0</v>
-      </c>
-      <c r="I112" s="30">
-        <v>0</v>
-      </c>
-      <c r="J112" s="30">
-        <v>0</v>
-      </c>
-      <c r="K112" s="2">
-        <v>1</v>
-      </c>
-      <c r="L112" s="2">
-        <v>0</v>
-      </c>
-      <c r="M112" s="30">
-        <v>0</v>
-      </c>
-      <c r="N112" s="30">
-        <v>0</v>
-      </c>
-      <c r="O112" s="2">
-        <v>0</v>
-      </c>
-      <c r="P112" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q112" s="2">
-        <v>0</v>
-      </c>
-      <c r="R112" s="2">
-        <v>0</v>
-      </c>
-      <c r="S112" s="30">
-        <v>0</v>
-      </c>
-      <c r="T112" s="30">
-        <v>0</v>
-      </c>
-      <c r="U112" s="2">
-        <v>0</v>
-      </c>
-      <c r="V112" s="30">
-        <v>0</v>
-      </c>
-      <c r="W112" s="2">
-        <v>0</v>
-      </c>
-      <c r="X112" s="30">
-        <v>0</v>
-      </c>
-      <c r="Y112" s="30">
-        <v>0</v>
-      </c>
-      <c r="Z112" s="30">
-        <v>0</v>
-      </c>
-      <c r="AA112" s="2">
-        <v>0</v>
-      </c>
-      <c r="AB112" s="30">
-        <v>0</v>
-      </c>
-      <c r="AC112" s="28">
-        <v>0</v>
-      </c>
-      <c r="AD112" s="30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="113" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A113" s="10" t="s">
-        <v>182</v>
-      </c>
-      <c r="B113" s="5" t="s">
-        <v>186</v>
-      </c>
-      <c r="C113" s="6" t="s">
-        <v>187</v>
       </c>
       <c r="D113" s="7" t="s">
         <v>14</v>
@@ -8240,107 +8232,107 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:30">
       <c r="A114" s="10" t="s">
         <v>165</v>
       </c>
       <c r="B114" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="C114" s="6" t="s">
         <v>187</v>
       </c>
-      <c r="C114" s="6" t="s">
+      <c r="D114" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E114" s="2">
+        <v>0</v>
+      </c>
+      <c r="F114" s="2">
+        <v>1</v>
+      </c>
+      <c r="G114" s="2">
+        <v>1</v>
+      </c>
+      <c r="H114" s="30">
+        <v>1</v>
+      </c>
+      <c r="I114" s="30">
+        <v>1</v>
+      </c>
+      <c r="J114" s="30">
+        <v>0</v>
+      </c>
+      <c r="K114" s="2">
+        <v>0</v>
+      </c>
+      <c r="L114" s="2">
+        <v>1</v>
+      </c>
+      <c r="M114" s="30">
+        <v>0</v>
+      </c>
+      <c r="N114" s="30">
+        <v>0</v>
+      </c>
+      <c r="O114" s="2">
+        <v>0</v>
+      </c>
+      <c r="P114" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q114" s="2">
+        <v>0</v>
+      </c>
+      <c r="R114" s="2">
+        <v>0</v>
+      </c>
+      <c r="S114" s="30">
+        <v>0</v>
+      </c>
+      <c r="T114" s="30">
+        <v>0</v>
+      </c>
+      <c r="U114" s="2">
+        <v>0</v>
+      </c>
+      <c r="V114" s="30">
+        <v>0</v>
+      </c>
+      <c r="W114" s="2">
+        <v>0</v>
+      </c>
+      <c r="X114" s="30">
+        <v>0</v>
+      </c>
+      <c r="Y114" s="30">
+        <v>0</v>
+      </c>
+      <c r="Z114" s="30">
+        <v>0</v>
+      </c>
+      <c r="AA114" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB114" s="30">
+        <v>0</v>
+      </c>
+      <c r="AC114" s="28">
+        <v>0</v>
+      </c>
+      <c r="AD114" s="30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:30">
+      <c r="A115" s="10" t="s">
+        <v>179</v>
+      </c>
+      <c r="B115" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="C115" s="6" t="s">
         <v>188</v>
-      </c>
-      <c r="D114" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E114" s="2">
-        <v>0</v>
-      </c>
-      <c r="F114" s="2">
-        <v>1</v>
-      </c>
-      <c r="G114" s="2">
-        <v>1</v>
-      </c>
-      <c r="H114" s="30">
-        <v>1</v>
-      </c>
-      <c r="I114" s="30">
-        <v>1</v>
-      </c>
-      <c r="J114" s="30">
-        <v>0</v>
-      </c>
-      <c r="K114" s="2">
-        <v>0</v>
-      </c>
-      <c r="L114" s="2">
-        <v>1</v>
-      </c>
-      <c r="M114" s="30">
-        <v>0</v>
-      </c>
-      <c r="N114" s="30">
-        <v>0</v>
-      </c>
-      <c r="O114" s="2">
-        <v>0</v>
-      </c>
-      <c r="P114" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q114" s="2">
-        <v>0</v>
-      </c>
-      <c r="R114" s="2">
-        <v>0</v>
-      </c>
-      <c r="S114" s="30">
-        <v>0</v>
-      </c>
-      <c r="T114" s="30">
-        <v>0</v>
-      </c>
-      <c r="U114" s="2">
-        <v>0</v>
-      </c>
-      <c r="V114" s="30">
-        <v>0</v>
-      </c>
-      <c r="W114" s="2">
-        <v>0</v>
-      </c>
-      <c r="X114" s="30">
-        <v>0</v>
-      </c>
-      <c r="Y114" s="30">
-        <v>0</v>
-      </c>
-      <c r="Z114" s="30">
-        <v>0</v>
-      </c>
-      <c r="AA114" s="2">
-        <v>0</v>
-      </c>
-      <c r="AB114" s="30">
-        <v>0</v>
-      </c>
-      <c r="AC114" s="28">
-        <v>0</v>
-      </c>
-      <c r="AD114" s="30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="115" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A115" s="10" t="s">
-        <v>180</v>
-      </c>
-      <c r="B115" s="5" t="s">
-        <v>188</v>
-      </c>
-      <c r="C115" s="6" t="s">
-        <v>189</v>
       </c>
       <c r="D115" s="7" t="s">
         <v>14</v>
@@ -8424,12 +8416,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:30">
       <c r="A116" s="10" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B116" s="5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C116" s="6" t="s">
         <v>13</v>
@@ -8516,31 +8508,31 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:30">
       <c r="A117" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="AD117" s="30">
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:30">
       <c r="A118" s="10" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="AD118" s="30">
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:30">
       <c r="A119" s="10" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B119" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="C119" s="6" t="s">
         <v>194</v>
-      </c>
-      <c r="C119" s="6" t="s">
-        <v>195</v>
       </c>
       <c r="D119" s="7" t="s">
         <v>14</v>
@@ -8591,41 +8583,41 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:30">
       <c r="A120" s="10" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B120" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="C120" s="6" t="s">
         <v>195</v>
       </c>
-      <c r="C120" s="6" t="s">
+      <c r="K120" s="2">
+        <v>1</v>
+      </c>
+      <c r="L120" s="2">
+        <v>0</v>
+      </c>
+      <c r="S120" s="30">
+        <v>0</v>
+      </c>
+      <c r="T120" s="30">
+        <v>1</v>
+      </c>
+      <c r="AD120" s="30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:30">
+      <c r="A121" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="B121" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="C121" s="6" t="s">
         <v>196</v>
-      </c>
-      <c r="K120" s="2">
-        <v>1</v>
-      </c>
-      <c r="L120" s="2">
-        <v>0</v>
-      </c>
-      <c r="S120" s="30">
-        <v>0</v>
-      </c>
-      <c r="T120" s="30">
-        <v>1</v>
-      </c>
-      <c r="AD120" s="30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="121" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A121" s="10" t="s">
-        <v>200</v>
-      </c>
-      <c r="B121" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="C121" s="6" t="s">
-        <v>197</v>
       </c>
       <c r="D121" s="7" t="s">
         <v>13</v>
@@ -8662,44 +8654,44 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:30">
       <c r="A122" s="10" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B122" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="C122" s="6" t="s">
         <v>197</v>
       </c>
-      <c r="C122" s="6" t="s">
+      <c r="D122" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E122" s="2">
+        <v>0</v>
+      </c>
+      <c r="F122" s="2">
+        <v>1</v>
+      </c>
+      <c r="G122" s="2">
+        <v>0</v>
+      </c>
+      <c r="W122" s="2">
+        <v>1</v>
+      </c>
+      <c r="AD122" s="30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="1:30">
+      <c r="A123" s="10" t="s">
+        <v>171</v>
+      </c>
+      <c r="B123" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="C123" s="6" t="s">
         <v>198</v>
-      </c>
-      <c r="D122" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E122" s="2">
-        <v>0</v>
-      </c>
-      <c r="F122" s="2">
-        <v>1</v>
-      </c>
-      <c r="G122" s="2">
-        <v>0</v>
-      </c>
-      <c r="W122" s="2">
-        <v>1</v>
-      </c>
-      <c r="AD122" s="30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="123" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A123" s="10" t="s">
-        <v>172</v>
-      </c>
-      <c r="B123" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="C123" s="6" t="s">
-        <v>199</v>
       </c>
       <c r="D123" s="7" t="s">
         <v>14</v>
@@ -8747,38 +8739,38 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:30">
       <c r="A124" s="10" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B124" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="C124" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="K124" s="2">
+        <v>1</v>
+      </c>
+      <c r="L124" s="2">
+        <v>0</v>
+      </c>
+      <c r="S124" s="30">
+        <v>0</v>
+      </c>
+      <c r="T124" s="30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="125" spans="1:30">
+      <c r="A125" s="10" t="s">
         <v>199</v>
       </c>
-      <c r="C124" s="6" t="s">
+      <c r="B125" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="C125" s="6" t="s">
         <v>201</v>
-      </c>
-      <c r="K124" s="2">
-        <v>1</v>
-      </c>
-      <c r="L124" s="2">
-        <v>0</v>
-      </c>
-      <c r="S124" s="30">
-        <v>0</v>
-      </c>
-      <c r="T124" s="30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="125" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A125" s="10" t="s">
-        <v>200</v>
-      </c>
-      <c r="B125" s="5" t="s">
-        <v>201</v>
-      </c>
-      <c r="C125" s="6" t="s">
-        <v>202</v>
       </c>
       <c r="D125" s="7" t="s">
         <v>13</v>
@@ -8812,12 +8804,12 @@
       <c r="AA125" s="27"/>
       <c r="AC125" s="27"/>
     </row>
-    <row r="126" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:30">
       <c r="A126" s="26" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B126" s="5" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C126" s="6" t="s">
         <v>13</v>
@@ -8858,12 +8850,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="D2:G2"/>
-    <mergeCell ref="O2:R2"/>
-    <mergeCell ref="S2:T2"/>
-    <mergeCell ref="X2:Z2"/>
-    <mergeCell ref="H2:J2"/>
-    <mergeCell ref="K2:L2"/>
     <mergeCell ref="D1:G1"/>
     <mergeCell ref="M1:N1"/>
     <mergeCell ref="X1:Z1"/>
@@ -8871,6 +8857,12 @@
     <mergeCell ref="O1:R1"/>
     <mergeCell ref="K1:L1"/>
     <mergeCell ref="H1:J1"/>
+    <mergeCell ref="D2:G2"/>
+    <mergeCell ref="O2:R2"/>
+    <mergeCell ref="S2:T2"/>
+    <mergeCell ref="X2:Z2"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="K2:L2"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add: program to add two numbers.
</commit_message>
<xml_diff>
--- a/Microroutines.xlsx
+++ b/Microroutines.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Years\3rd Year\Online\ARC\Project\PDP11\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\college\arch\PDP11\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{443B8BD4-3B02-4854-9948-128F2D5C3B33}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="218">
   <si>
     <t>Micro instruction</t>
   </si>
@@ -676,9 +675,6 @@
     <t xml:space="preserve">PC_out, MAR_in, Z_in, Clear_Y, Carry_in, Add </t>
   </si>
   <si>
-    <t>PC_in, Z_out, Read</t>
-  </si>
-  <si>
     <t>PC_in DEST_out  write</t>
   </si>
   <si>
@@ -689,12 +685,39 @@
   </si>
   <si>
     <t>007</t>
+  </si>
+  <si>
+    <t>35-27</t>
+  </si>
+  <si>
+    <t>26-23</t>
+  </si>
+  <si>
+    <t>22-20</t>
+  </si>
+  <si>
+    <t>19-18</t>
+  </si>
+  <si>
+    <t>17-16</t>
+  </si>
+  <si>
+    <t>15-12</t>
+  </si>
+  <si>
+    <t>11-10</t>
+  </si>
+  <si>
+    <t>6-4</t>
+  </si>
+  <si>
+    <t>PC_in, Z_out, Read, MDR_in</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -795,7 +818,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
@@ -885,6 +908,18 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="2" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="16" fontId="1" fillId="2" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -1170,48 +1205,48 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE126"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="86" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q15" sqref="Q15"/>
+      <selection pane="bottomLeft" activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="47.140625" customWidth="1"/>
-    <col min="2" max="2" width="8.7109375" style="5" customWidth="1"/>
-    <col min="3" max="3" width="7.42578125" style="6" customWidth="1"/>
-    <col min="4" max="4" width="2.5703125" style="7" customWidth="1"/>
+    <col min="1" max="1" width="47.109375" customWidth="1"/>
+    <col min="2" max="2" width="8.6640625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="7.44140625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="2.5546875" style="7" customWidth="1"/>
     <col min="5" max="5" width="3" style="2" customWidth="1"/>
-    <col min="6" max="6" width="3.140625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="3.7109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="3.109375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="3.6640625" style="2" customWidth="1"/>
     <col min="8" max="8" width="3" style="30" customWidth="1"/>
-    <col min="9" max="9" width="3.42578125" style="30" customWidth="1"/>
-    <col min="10" max="10" width="2.85546875" style="30" customWidth="1"/>
-    <col min="11" max="11" width="3.28515625" style="2" customWidth="1"/>
-    <col min="12" max="12" width="3.5703125" style="2" customWidth="1"/>
-    <col min="13" max="13" width="3.5703125" style="30" customWidth="1"/>
-    <col min="14" max="14" width="3.140625" style="30" customWidth="1"/>
-    <col min="15" max="16" width="3.5703125" style="2" customWidth="1"/>
-    <col min="17" max="18" width="3.42578125" style="2" customWidth="1"/>
-    <col min="19" max="19" width="3.7109375" style="30" customWidth="1"/>
-    <col min="20" max="20" width="3.42578125" style="30" customWidth="1"/>
+    <col min="9" max="9" width="3.44140625" style="30" customWidth="1"/>
+    <col min="10" max="10" width="2.88671875" style="30" customWidth="1"/>
+    <col min="11" max="11" width="3.33203125" style="2" customWidth="1"/>
+    <col min="12" max="12" width="3.5546875" style="2" customWidth="1"/>
+    <col min="13" max="13" width="3.5546875" style="30" customWidth="1"/>
+    <col min="14" max="14" width="3.109375" style="30" customWidth="1"/>
+    <col min="15" max="16" width="3.5546875" style="2" customWidth="1"/>
+    <col min="17" max="18" width="3.44140625" style="2" customWidth="1"/>
+    <col min="19" max="19" width="3.6640625" style="30" customWidth="1"/>
+    <col min="20" max="20" width="3.44140625" style="30" customWidth="1"/>
     <col min="21" max="21" width="3" style="2" customWidth="1"/>
-    <col min="22" max="22" width="3.140625" style="30" customWidth="1"/>
-    <col min="23" max="23" width="3.42578125" style="2" customWidth="1"/>
+    <col min="22" max="22" width="3.109375" style="30" customWidth="1"/>
+    <col min="23" max="23" width="3.44140625" style="2" customWidth="1"/>
     <col min="24" max="24" width="4" style="30" customWidth="1"/>
-    <col min="25" max="25" width="3.42578125" style="30" customWidth="1"/>
-    <col min="26" max="26" width="3.5703125" style="30" customWidth="1"/>
-    <col min="27" max="27" width="3.42578125" style="2" customWidth="1"/>
-    <col min="28" max="28" width="3.42578125" style="30" customWidth="1"/>
-    <col min="29" max="29" width="3.42578125" style="25" customWidth="1"/>
-    <col min="30" max="30" width="3.42578125" style="30" customWidth="1"/>
-    <col min="31" max="31" width="30.42578125" style="15" customWidth="1"/>
+    <col min="25" max="25" width="3.44140625" style="30" customWidth="1"/>
+    <col min="26" max="26" width="3.5546875" style="30" customWidth="1"/>
+    <col min="27" max="27" width="3.44140625" style="2" customWidth="1"/>
+    <col min="28" max="28" width="3.44140625" style="30" customWidth="1"/>
+    <col min="29" max="29" width="3.44140625" style="25" customWidth="1"/>
+    <col min="30" max="30" width="3.44140625" style="30" customWidth="1"/>
+    <col min="31" max="31" width="30.44140625" style="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1280,27 +1315,67 @@
         <v>125</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="D2" s="33"/>
+    <row r="2" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="C2" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="D2" s="33" t="s">
+        <v>210</v>
+      </c>
       <c r="E2" s="33"/>
       <c r="F2" s="33"/>
       <c r="G2" s="33"/>
-      <c r="H2" s="34"/>
+      <c r="H2" s="34" t="s">
+        <v>211</v>
+      </c>
       <c r="I2" s="34"/>
       <c r="J2" s="34"/>
-      <c r="K2" s="33"/>
+      <c r="K2" s="37" t="s">
+        <v>212</v>
+      </c>
       <c r="L2" s="33"/>
-      <c r="O2" s="33"/>
+      <c r="M2" s="36" t="s">
+        <v>213</v>
+      </c>
+      <c r="N2" s="35"/>
+      <c r="O2" s="33" t="s">
+        <v>214</v>
+      </c>
       <c r="P2" s="33"/>
       <c r="Q2" s="33"/>
       <c r="R2" s="33"/>
-      <c r="S2" s="34"/>
+      <c r="S2" s="38" t="s">
+        <v>215</v>
+      </c>
       <c r="T2" s="34"/>
-      <c r="X2" s="34"/>
+      <c r="U2" s="2">
+        <v>9</v>
+      </c>
+      <c r="V2" s="30">
+        <v>8</v>
+      </c>
+      <c r="W2" s="2">
+        <v>7</v>
+      </c>
+      <c r="X2" s="38" t="s">
+        <v>216</v>
+      </c>
       <c r="Y2" s="34"/>
       <c r="Z2" s="34"/>
-    </row>
-    <row r="3" spans="1:31" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AA2" s="2">
+        <v>3</v>
+      </c>
+      <c r="AB2" s="30">
+        <v>2</v>
+      </c>
+      <c r="AC2" s="25">
+        <v>1</v>
+      </c>
+      <c r="AD2" s="30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>79</v>
       </c>
@@ -1335,7 +1410,7 @@
       <c r="AD3" s="11"/>
       <c r="AE3" s="16"/>
     </row>
-    <row r="4" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>204</v>
       </c>
@@ -1428,9 +1503,9 @@
       </c>
       <c r="AE4" s="17"/>
     </row>
-    <row r="5" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>205</v>
+        <v>217</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>10</v>
@@ -1460,7 +1535,7 @@
         <v>1</v>
       </c>
       <c r="K5" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L5" s="2">
         <v>0</v>
@@ -1521,7 +1596,7 @@
       </c>
       <c r="AE5" s="17"/>
     </row>
-    <row r="6" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -1614,7 +1689,7 @@
       </c>
       <c r="AE6" s="17"/>
     </row>
-    <row r="7" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1707,7 +1782,7 @@
       </c>
       <c r="AE7" s="17"/>
     </row>
-    <row r="8" spans="1:31" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:31" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
         <v>78</v>
       </c>
@@ -1742,7 +1817,7 @@
       <c r="AD8" s="11"/>
       <c r="AE8" s="16"/>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1753,7 +1828,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -1845,7 +1920,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -1937,7 +2012,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -2029,7 +2104,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -2121,7 +2196,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -2213,7 +2288,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -2305,7 +2380,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>28</v>
       </c>
@@ -2397,7 +2472,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -2489,7 +2564,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>33</v>
       </c>
@@ -2581,7 +2656,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>32</v>
       </c>
@@ -2673,7 +2748,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>35</v>
       </c>
@@ -2765,7 +2840,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>37</v>
       </c>
@@ -2857,7 +2932,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>39</v>
       </c>
@@ -2949,7 +3024,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>19</v>
       </c>
@@ -3044,7 +3119,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="24" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>42</v>
       </c>
@@ -3136,7 +3211,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>19</v>
       </c>
@@ -3228,7 +3303,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>45</v>
       </c>
@@ -3320,7 +3395,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:31" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:31" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="8" t="s">
         <v>104</v>
       </c>
@@ -3355,7 +3430,7 @@
       <c r="AD27" s="9"/>
       <c r="AE27" s="16"/>
     </row>
-    <row r="28" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>61</v>
       </c>
@@ -3447,7 +3522,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>54</v>
       </c>
@@ -3539,7 +3614,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>19</v>
       </c>
@@ -3631,7 +3706,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>56</v>
       </c>
@@ -3723,7 +3798,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>57</v>
       </c>
@@ -3815,7 +3890,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>58</v>
       </c>
@@ -3907,7 +3982,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>59</v>
       </c>
@@ -3999,7 +4074,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>19</v>
       </c>
@@ -4091,7 +4166,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>33</v>
       </c>
@@ -4183,7 +4258,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>32</v>
       </c>
@@ -4275,7 +4350,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>35</v>
       </c>
@@ -4367,7 +4442,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>60</v>
       </c>
@@ -4459,7 +4534,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>39</v>
       </c>
@@ -4551,7 +4626,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>19</v>
       </c>
@@ -4646,7 +4721,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="42" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>42</v>
       </c>
@@ -4738,7 +4813,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>19</v>
       </c>
@@ -4830,7 +4905,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>62</v>
       </c>
@@ -4925,7 +5000,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="45" spans="1:31" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:31" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A45" s="8" t="s">
         <v>101</v>
       </c>
@@ -4960,7 +5035,7 @@
       <c r="AD45" s="11"/>
       <c r="AE45" s="16"/>
     </row>
-    <row r="46" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A46" s="10" t="s">
         <v>77</v>
       </c>
@@ -5052,7 +5127,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A47" s="12" t="s">
         <v>81</v>
       </c>
@@ -5069,7 +5144,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A48" s="12" t="s">
         <v>161</v>
       </c>
@@ -5161,7 +5236,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A49" s="10" t="s">
         <v>82</v>
       </c>
@@ -5189,7 +5264,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A50" s="10" t="s">
         <v>80</v>
       </c>
@@ -5281,7 +5356,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A51" s="12" t="s">
         <v>83</v>
       </c>
@@ -5310,7 +5385,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A52" s="12" t="s">
         <v>86</v>
       </c>
@@ -5402,7 +5477,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A53" s="10" t="s">
         <v>84</v>
       </c>
@@ -5430,7 +5505,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A54" s="10" t="s">
         <v>90</v>
       </c>
@@ -5522,7 +5597,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A55" s="12" t="s">
         <v>85</v>
       </c>
@@ -5539,7 +5614,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A56" s="12" t="s">
         <v>91</v>
       </c>
@@ -5631,7 +5706,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A57" s="10" t="s">
         <v>87</v>
       </c>
@@ -5648,7 +5723,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A58" s="10" t="s">
         <v>92</v>
       </c>
@@ -5740,7 +5815,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A59" s="12" t="s">
         <v>88</v>
       </c>
@@ -5757,7 +5832,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A60" s="12" t="s">
         <v>93</v>
       </c>
@@ -5849,7 +5924,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A61" s="10" t="s">
         <v>89</v>
       </c>
@@ -5866,7 +5941,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A62" s="10" t="s">
         <v>94</v>
       </c>
@@ -5958,7 +6033,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A63" s="12" t="s">
         <v>95</v>
       </c>
@@ -5975,7 +6050,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A64" s="12" t="s">
         <v>90</v>
       </c>
@@ -6067,7 +6142,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:31" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:31" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A65" s="8" t="s">
         <v>148</v>
       </c>
@@ -6102,7 +6177,7 @@
       <c r="AD65" s="9"/>
       <c r="AE65" s="16"/>
     </row>
-    <row r="66" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B66" s="5" t="s">
         <v>119</v>
       </c>
@@ -6128,7 +6203,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A67" s="10" t="s">
         <v>121</v>
       </c>
@@ -6154,7 +6229,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A68" s="10" t="s">
         <v>127</v>
       </c>
@@ -6246,7 +6321,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A69" s="12" t="s">
         <v>122</v>
       </c>
@@ -6272,7 +6347,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A70" s="12" t="s">
         <v>128</v>
       </c>
@@ -6364,7 +6439,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A71" s="10" t="s">
         <v>123</v>
       </c>
@@ -6378,7 +6453,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A72" s="10" t="s">
         <v>160</v>
       </c>
@@ -6470,7 +6545,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A73" s="12" t="s">
         <v>124</v>
       </c>
@@ -6484,7 +6559,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A74" s="12" t="s">
         <v>129</v>
       </c>
@@ -6579,7 +6654,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="75" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A75" s="10" t="s">
         <v>126</v>
       </c>
@@ -6596,7 +6671,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="76" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A76" s="10" t="s">
         <v>133</v>
       </c>
@@ -6691,7 +6766,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="77" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A77" s="12" t="s">
         <v>131</v>
       </c>
@@ -6708,7 +6783,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="78" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A78" s="12" t="s">
         <v>132</v>
       </c>
@@ -6803,7 +6878,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="79" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A79" s="10" t="s">
         <v>134</v>
       </c>
@@ -6820,7 +6895,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="80" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A80" s="10" t="s">
         <v>135</v>
       </c>
@@ -6915,7 +6990,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="81" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A81" s="12" t="s">
         <v>136</v>
       </c>
@@ -6932,7 +7007,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="82" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A82" s="12" t="s">
         <v>137</v>
       </c>
@@ -7027,7 +7102,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="83" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A83" s="10" t="s">
         <v>138</v>
       </c>
@@ -7044,7 +7119,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="84" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A84" s="10" t="s">
         <v>139</v>
       </c>
@@ -7139,7 +7214,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="85" spans="1:31" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:31" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A85" s="8" t="s">
         <v>96</v>
       </c>
@@ -7174,7 +7249,7 @@
       <c r="AD85" s="11"/>
       <c r="AE85" s="16"/>
     </row>
-    <row r="86" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>97</v>
       </c>
@@ -7266,7 +7341,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>98</v>
       </c>
@@ -7361,7 +7436,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="88" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>99</v>
       </c>
@@ -7453,7 +7528,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:31" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:31" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A89" s="8" t="s">
         <v>149</v>
       </c>
@@ -7488,7 +7563,7 @@
       <c r="AD89" s="11"/>
       <c r="AE89" s="16"/>
     </row>
-    <row r="90" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A90" s="10" t="s">
         <v>152</v>
       </c>
@@ -7502,7 +7577,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A91" s="10" t="s">
         <v>153</v>
       </c>
@@ -7516,7 +7591,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>151</v>
       </c>
@@ -7527,7 +7602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B93" s="5" t="s">
         <v>150</v>
       </c>
@@ -7541,7 +7616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:31" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:31" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A94" s="8" t="s">
         <v>155</v>
       </c>
@@ -7576,16 +7651,16 @@
       <c r="AD94" s="9"/>
       <c r="AE94" s="16"/>
     </row>
-    <row r="95" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A95" s="24" t="s">
         <v>156</v>
       </c>
       <c r="B95" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="C95" s="6" t="s">
         <v>207</v>
       </c>
-      <c r="C95" s="6" t="s">
-        <v>208</v>
-      </c>
       <c r="D95" s="7" t="s">
         <v>13</v>
       </c>
@@ -7668,16 +7743,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>157</v>
       </c>
       <c r="B96" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="C96" s="6" t="s">
         <v>208</v>
       </c>
-      <c r="C96" s="6" t="s">
-        <v>209</v>
-      </c>
       <c r="D96" s="7" t="s">
         <v>13</v>
       </c>
@@ -7760,12 +7835,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>158</v>
       </c>
       <c r="B97" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C97" s="6" t="s">
         <v>13</v>
@@ -7852,7 +7927,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:31" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:31" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A98" s="8" t="s">
         <v>159</v>
       </c>
@@ -7887,7 +7962,7 @@
       <c r="AD98" s="11"/>
       <c r="AE98" s="16"/>
     </row>
-    <row r="99" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
         <v>170</v>
       </c>
@@ -7898,7 +7973,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A100" s="10" t="s">
         <v>164</v>
       </c>
@@ -7990,7 +8065,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A101" s="10" t="s">
         <v>165</v>
       </c>
@@ -8082,7 +8157,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A102" s="10" t="s">
         <v>180</v>
       </c>
@@ -8174,9 +8249,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A103" s="10" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B103" s="5" t="s">
         <v>167</v>
@@ -8266,7 +8341,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="s">
         <v>169</v>
       </c>
@@ -8299,7 +8374,7 @@
       <c r="AC104" s="5"/>
       <c r="AD104" s="5"/>
     </row>
-    <row r="105" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A105" s="10" t="s">
         <v>171</v>
       </c>
@@ -8391,7 +8466,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A106" s="10" t="s">
         <v>172</v>
       </c>
@@ -8483,7 +8558,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A107" s="10" t="s">
         <v>192</v>
       </c>
@@ -8575,7 +8650,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A108" s="10" t="s">
         <v>199</v>
       </c>
@@ -8667,7 +8742,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A109" s="1" t="s">
         <v>178</v>
       </c>
@@ -8700,7 +8775,7 @@
       <c r="AC109" s="5"/>
       <c r="AD109" s="5"/>
     </row>
-    <row r="110" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A110" s="10" t="s">
         <v>164</v>
       </c>
@@ -8792,7 +8867,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A111" s="10" t="s">
         <v>165</v>
       </c>
@@ -8884,7 +8959,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A112" s="10" t="s">
         <v>180</v>
       </c>
@@ -8976,7 +9051,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A113" s="10" t="s">
         <v>181</v>
       </c>
@@ -9068,7 +9143,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A114" s="10" t="s">
         <v>165</v>
       </c>
@@ -9160,7 +9235,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A115" s="10" t="s">
         <v>179</v>
       </c>
@@ -9252,7 +9327,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A116" s="10" t="s">
         <v>182</v>
       </c>
@@ -9344,7 +9419,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A117" s="1" t="s">
         <v>176</v>
       </c>
@@ -9377,7 +9452,7 @@
       <c r="AC117" s="5"/>
       <c r="AD117" s="5"/>
     </row>
-    <row r="118" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A118" s="10" t="s">
         <v>191</v>
       </c>
@@ -9408,7 +9483,7 @@
       <c r="AC118" s="7"/>
       <c r="AD118" s="7"/>
     </row>
-    <row r="119" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A119" s="10" t="s">
         <v>171</v>
       </c>
@@ -9500,7 +9575,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A120" s="10" t="s">
         <v>172</v>
       </c>
@@ -9586,7 +9661,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A121" s="10" t="s">
         <v>199</v>
       </c>
@@ -9678,7 +9753,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A122" s="10" t="s">
         <v>203</v>
       </c>
@@ -9770,7 +9845,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A123" s="10" t="s">
         <v>171</v>
       </c>
@@ -9862,7 +9937,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A124" s="10" t="s">
         <v>172</v>
       </c>
@@ -9954,7 +10029,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A125" s="10" t="s">
         <v>199</v>
       </c>
@@ -10046,7 +10121,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A126" s="26" t="s">
         <v>192</v>
       </c>
@@ -10139,7 +10214,14 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="14">
+    <mergeCell ref="D2:G2"/>
+    <mergeCell ref="O2:R2"/>
+    <mergeCell ref="S2:T2"/>
+    <mergeCell ref="X2:Z2"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
     <mergeCell ref="D1:G1"/>
     <mergeCell ref="M1:N1"/>
     <mergeCell ref="X1:Z1"/>
@@ -10147,12 +10229,6 @@
     <mergeCell ref="O1:R1"/>
     <mergeCell ref="K1:L1"/>
     <mergeCell ref="H1:J1"/>
-    <mergeCell ref="D2:G2"/>
-    <mergeCell ref="O2:R2"/>
-    <mergeCell ref="S2:T2"/>
-    <mergeCell ref="X2:Z2"/>
-    <mergeCell ref="H2:J2"/>
-    <mergeCell ref="K2:L2"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add: c3 and c4 test cases.
</commit_message>
<xml_diff>
--- a/Microroutines.xlsx
+++ b/Microroutines.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="219">
   <si>
     <t>Micro instruction</t>
   </si>
@@ -294,9 +294,6 @@
   </si>
   <si>
     <t>XOR:</t>
-  </si>
-  <si>
-    <t>DEST_out sub Z_in FLAGS_in</t>
   </si>
   <si>
     <t>DEST_out sbc Z_in FLAGS_in</t>
@@ -712,6 +709,12 @@
   </si>
   <si>
     <t>PC_in, Z_out, Read, MDR_in</t>
+  </si>
+  <si>
+    <t>DEST_out sub Z_in Carry in FLAGS_in</t>
+  </si>
+  <si>
+    <t>DEST_out sub Carry_in Z_in FLAGS_in</t>
   </si>
 </sst>
 </file>
@@ -907,20 +910,20 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="16" fontId="1" fillId="2" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="20" fontId="2" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="20" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="20" fontId="2" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="16" fontId="1" fillId="2" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1209,8 +1212,8 @@
   <dimension ref="A1:AE126"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="86" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L5" sqref="L5"/>
+      <pane ySplit="1" topLeftCell="A78" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A90" sqref="A90:XFD90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1254,7 +1257,7 @@
         <v>7</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D1" s="33" t="s">
         <v>46</v>
@@ -1262,29 +1265,29 @@
       <c r="E1" s="33"/>
       <c r="F1" s="33"/>
       <c r="G1" s="33"/>
-      <c r="H1" s="34" t="s">
+      <c r="H1" s="35" t="s">
         <v>49</v>
       </c>
-      <c r="I1" s="34"/>
-      <c r="J1" s="34"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
       <c r="K1" s="33" t="s">
         <v>48</v>
       </c>
       <c r="L1" s="33"/>
-      <c r="M1" s="34" t="s">
+      <c r="M1" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="N1" s="34"/>
+      <c r="N1" s="35"/>
       <c r="O1" s="33" t="s">
         <v>50</v>
       </c>
       <c r="P1" s="33"/>
       <c r="Q1" s="33"/>
       <c r="R1" s="33"/>
-      <c r="S1" s="34" t="s">
+      <c r="S1" s="35" t="s">
         <v>51</v>
       </c>
-      <c r="T1" s="34"/>
+      <c r="T1" s="35"/>
       <c r="U1" s="2" t="s">
         <v>1</v>
       </c>
@@ -1294,60 +1297,60 @@
       <c r="W1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="X1" s="34" t="s">
+      <c r="X1" s="35" t="s">
         <v>52</v>
       </c>
-      <c r="Y1" s="34"/>
-      <c r="Z1" s="34"/>
+      <c r="Y1" s="35"/>
+      <c r="Z1" s="35"/>
       <c r="AA1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="AB1" s="30" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AC1" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="AD1" s="30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="AE1" s="14" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.3">
       <c r="C2" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="D2" s="33" t="s">
         <v>209</v>
-      </c>
-      <c r="D2" s="33" t="s">
-        <v>210</v>
       </c>
       <c r="E2" s="33"/>
       <c r="F2" s="33"/>
       <c r="G2" s="33"/>
-      <c r="H2" s="34" t="s">
+      <c r="H2" s="35" t="s">
+        <v>210</v>
+      </c>
+      <c r="I2" s="35"/>
+      <c r="J2" s="35"/>
+      <c r="K2" s="36" t="s">
         <v>211</v>
       </c>
-      <c r="I2" s="34"/>
-      <c r="J2" s="34"/>
-      <c r="K2" s="37" t="s">
+      <c r="L2" s="33"/>
+      <c r="M2" s="37" t="s">
         <v>212</v>
       </c>
-      <c r="L2" s="33"/>
-      <c r="M2" s="36" t="s">
+      <c r="N2" s="38"/>
+      <c r="O2" s="33" t="s">
         <v>213</v>
-      </c>
-      <c r="N2" s="35"/>
-      <c r="O2" s="33" t="s">
-        <v>214</v>
       </c>
       <c r="P2" s="33"/>
       <c r="Q2" s="33"/>
       <c r="R2" s="33"/>
-      <c r="S2" s="38" t="s">
-        <v>215</v>
-      </c>
-      <c r="T2" s="34"/>
+      <c r="S2" s="34" t="s">
+        <v>214</v>
+      </c>
+      <c r="T2" s="35"/>
       <c r="U2" s="2">
         <v>9</v>
       </c>
@@ -1357,11 +1360,11 @@
       <c r="W2" s="2">
         <v>7</v>
       </c>
-      <c r="X2" s="38" t="s">
-        <v>216</v>
-      </c>
-      <c r="Y2" s="34"/>
-      <c r="Z2" s="34"/>
+      <c r="X2" s="34" t="s">
+        <v>215</v>
+      </c>
+      <c r="Y2" s="35"/>
+      <c r="Z2" s="35"/>
       <c r="AA2" s="2">
         <v>3</v>
       </c>
@@ -1412,7 +1415,7 @@
     </row>
     <row r="4" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>9</v>
@@ -1505,7 +1508,7 @@
     </row>
     <row r="5" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>10</v>
@@ -3116,7 +3119,7 @@
         <v>0</v>
       </c>
       <c r="AE23" s="15" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="24" spans="1:31" x14ac:dyDescent="0.3">
@@ -3397,7 +3400,7 @@
     </row>
     <row r="27" spans="1:31" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B27" s="9"/>
       <c r="C27" s="9"/>
@@ -3438,7 +3441,7 @@
         <v>43</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D28" s="19">
         <v>0</v>
@@ -4718,7 +4721,7 @@
         <v>0</v>
       </c>
       <c r="AE41" s="15" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="42" spans="1:31" x14ac:dyDescent="0.3">
@@ -4913,7 +4916,7 @@
         <v>76</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D44" s="19">
         <v>0</v>
@@ -4997,12 +5000,12 @@
         <v>0</v>
       </c>
       <c r="AE44" s="15" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="45" spans="1:31" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A45" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B45" s="9"/>
       <c r="C45" s="9"/>
@@ -5040,10 +5043,10 @@
         <v>77</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D46" s="7" t="s">
         <v>14</v>
@@ -5146,13 +5149,13 @@
     </row>
     <row r="48" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A48" s="12" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D48" s="7" t="s">
         <v>14</v>
@@ -5269,10 +5272,10 @@
         <v>80</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D50" s="7" t="s">
         <v>14</v>
@@ -5390,10 +5393,10 @@
         <v>86</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C52" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D52" s="7" t="s">
         <v>14</v>
@@ -5507,13 +5510,13 @@
     </row>
     <row r="54" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A54" s="10" t="s">
-        <v>90</v>
+        <v>217</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C54" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D54" s="7" t="s">
         <v>14</v>
@@ -5570,7 +5573,7 @@
         <v>0</v>
       </c>
       <c r="V54" s="32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W54" s="2">
         <v>1</v>
@@ -5616,13 +5619,13 @@
     </row>
     <row r="56" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A56" s="12" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C56" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D56" s="7" t="s">
         <v>14</v>
@@ -5725,13 +5728,13 @@
     </row>
     <row r="58" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A58" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C58" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D58" s="7" t="s">
         <v>14</v>
@@ -5834,13 +5837,13 @@
     </row>
     <row r="60" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A60" s="12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C60" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D60" s="7" t="s">
         <v>14</v>
@@ -5943,13 +5946,13 @@
     </row>
     <row r="62" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A62" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C62" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D62" s="7" t="s">
         <v>14</v>
@@ -6035,7 +6038,7 @@
     </row>
     <row r="63" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A63" s="12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="AA63" s="28">
         <v>0</v>
@@ -6052,10 +6055,10 @@
     </row>
     <row r="64" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A64" s="12" t="s">
-        <v>90</v>
+        <v>218</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C64" s="4">
         <v>0</v>
@@ -6115,7 +6118,7 @@
         <v>0</v>
       </c>
       <c r="V64" s="32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W64" s="3">
         <v>1</v>
@@ -6144,7 +6147,7 @@
     </row>
     <row r="65" spans="1:31" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A65" s="8" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B65" s="9"/>
       <c r="C65" s="9"/>
@@ -6179,10 +6182,10 @@
     </row>
     <row r="66" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B66" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="C66" s="6" t="s">
         <v>119</v>
-      </c>
-      <c r="C66" s="6" t="s">
-        <v>120</v>
       </c>
       <c r="X66" s="30">
         <v>1</v>
@@ -6205,7 +6208,7 @@
     </row>
     <row r="67" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A67" s="10" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E67" s="13"/>
       <c r="F67" s="13"/>
@@ -6231,13 +6234,13 @@
     </row>
     <row r="68" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A68" s="10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C68" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D68" s="7" t="s">
         <v>14</v>
@@ -6323,7 +6326,7 @@
     </row>
     <row r="69" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A69" s="12" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E69" s="13"/>
       <c r="F69" s="13"/>
@@ -6349,13 +6352,13 @@
     </row>
     <row r="70" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A70" s="12" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C70" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D70" s="7" t="s">
         <v>14</v>
@@ -6441,7 +6444,7 @@
     </row>
     <row r="71" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A71" s="10" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="AB71" s="30">
         <v>0</v>
@@ -6455,13 +6458,13 @@
     </row>
     <row r="72" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A72" s="10" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B72" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C72" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D72" s="7" t="s">
         <v>13</v>
@@ -6547,7 +6550,7 @@
     </row>
     <row r="73" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A73" s="12" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="AB73" s="30">
         <v>0</v>
@@ -6561,13 +6564,13 @@
     </row>
     <row r="74" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A74" s="12" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B74" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C74" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D74" s="7" t="s">
         <v>14</v>
@@ -6651,12 +6654,12 @@
         <v>0</v>
       </c>
       <c r="AE74" s="15" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="75" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A75" s="10" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="AB75" s="30">
         <v>0</v>
@@ -6668,18 +6671,18 @@
         <v>0</v>
       </c>
       <c r="AE75" s="15" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="76" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A76" s="10" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B76" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C76" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D76" s="7" t="s">
         <v>14</v>
@@ -6763,12 +6766,12 @@
         <v>0</v>
       </c>
       <c r="AE76" s="15" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="77" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A77" s="12" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AB77" s="30">
         <v>0</v>
@@ -6780,18 +6783,18 @@
         <v>0</v>
       </c>
       <c r="AE77" s="15" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="78" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A78" s="12" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B78" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C78" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D78" s="7" t="s">
         <v>14</v>
@@ -6875,12 +6878,12 @@
         <v>0</v>
       </c>
       <c r="AE78" s="15" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="79" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A79" s="10" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="AB79" s="30">
         <v>0</v>
@@ -6892,18 +6895,18 @@
         <v>0</v>
       </c>
       <c r="AE79" s="15" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="80" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A80" s="10" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B80" s="5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C80" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D80" s="7" t="s">
         <v>14</v>
@@ -6987,12 +6990,12 @@
         <v>0</v>
       </c>
       <c r="AE80" s="15" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="81" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A81" s="12" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="AB81" s="30">
         <v>0</v>
@@ -7004,18 +7007,18 @@
         <v>0</v>
       </c>
       <c r="AE81" s="15" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="82" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A82" s="12" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B82" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C82" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D82" s="7" t="s">
         <v>14</v>
@@ -7099,12 +7102,12 @@
         <v>0</v>
       </c>
       <c r="AE82" s="15" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="83" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A83" s="10" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="AB83" s="30">
         <v>0</v>
@@ -7116,18 +7119,18 @@
         <v>0</v>
       </c>
       <c r="AE83" s="15" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="84" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A84" s="10" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B84" s="5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C84" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D84" s="7" t="s">
         <v>14</v>
@@ -7211,12 +7214,12 @@
         <v>0</v>
       </c>
       <c r="AE84" s="15" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="85" spans="1:31" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A85" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B85" s="9"/>
       <c r="C85" s="9"/>
@@ -7251,13 +7254,13 @@
     </row>
     <row r="86" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B86" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C86" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D86" s="7" t="s">
         <v>13</v>
@@ -7343,10 +7346,10 @@
     </row>
     <row r="87" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B87" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C87" s="6" t="s">
         <v>13</v>
@@ -7433,15 +7436,15 @@
         <v>0</v>
       </c>
       <c r="AE87" s="15" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="88" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B88" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C88" s="6" t="s">
         <v>13</v>
@@ -7530,7 +7533,7 @@
     </row>
     <row r="89" spans="1:31" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A89" s="8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B89" s="9"/>
       <c r="C89" s="9"/>
@@ -7565,7 +7568,7 @@
     </row>
     <row r="90" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A90" s="10" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="AB90" s="30">
         <v>0</v>
@@ -7579,7 +7582,7 @@
     </row>
     <row r="91" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A91" s="10" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AB91" s="30">
         <v>0</v>
@@ -7593,7 +7596,7 @@
     </row>
     <row r="92" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="AC92" s="28">
         <v>0</v>
@@ -7604,7 +7607,7 @@
     </row>
     <row r="93" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B93" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="AB93" s="30">
         <v>1</v>
@@ -7618,7 +7621,7 @@
     </row>
     <row r="94" spans="1:31" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A94" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B94" s="9"/>
       <c r="C94" s="9"/>
@@ -7653,13 +7656,13 @@
     </row>
     <row r="95" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A95" s="24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B95" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="C95" s="6" t="s">
         <v>206</v>
-      </c>
-      <c r="C95" s="6" t="s">
-        <v>207</v>
       </c>
       <c r="D95" s="7" t="s">
         <v>13</v>
@@ -7745,13 +7748,13 @@
     </row>
     <row r="96" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B96" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="C96" s="6" t="s">
         <v>207</v>
-      </c>
-      <c r="C96" s="6" t="s">
-        <v>208</v>
       </c>
       <c r="D96" s="7" t="s">
         <v>13</v>
@@ -7837,10 +7840,10 @@
     </row>
     <row r="97" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B97" s="5" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C97" s="6" t="s">
         <v>13</v>
@@ -7929,7 +7932,7 @@
     </row>
     <row r="98" spans="1:31" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A98" s="8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B98" s="9"/>
       <c r="C98" s="9"/>
@@ -7964,7 +7967,7 @@
     </row>
     <row r="99" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="AC99" s="28">
         <v>0</v>
@@ -7975,13 +7978,13 @@
     </row>
     <row r="100" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A100" s="10" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B100" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="C100" s="6" t="s">
         <v>162</v>
-      </c>
-      <c r="C100" s="6" t="s">
-        <v>163</v>
       </c>
       <c r="D100" s="29">
         <v>1</v>
@@ -8067,13 +8070,13 @@
     </row>
     <row r="101" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A101" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="B101" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C101" s="6" t="s">
         <v>165</v>
-      </c>
-      <c r="B101" s="5" t="s">
-        <v>163</v>
-      </c>
-      <c r="C101" s="6" t="s">
-        <v>166</v>
       </c>
       <c r="D101" s="29">
         <v>0</v>
@@ -8159,13 +8162,13 @@
     </row>
     <row r="102" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A102" s="10" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B102" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="C102" s="6" t="s">
         <v>166</v>
-      </c>
-      <c r="C102" s="6" t="s">
-        <v>167</v>
       </c>
       <c r="D102" s="29">
         <v>0</v>
@@ -8251,10 +8254,10 @@
     </row>
     <row r="103" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A103" s="10" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B103" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C103" s="23" t="s">
         <v>13</v>
@@ -8343,7 +8346,7 @@
     </row>
     <row r="104" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C104" s="5"/>
       <c r="D104" s="5"/>
@@ -8376,13 +8379,13 @@
     </row>
     <row r="105" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A105" s="10" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B105" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C105" s="6" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D105" s="29">
         <v>1</v>
@@ -8468,13 +8471,13 @@
     </row>
     <row r="106" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A106" s="10" t="s">
+        <v>171</v>
+      </c>
+      <c r="B106" s="5" t="s">
         <v>172</v>
       </c>
-      <c r="B106" s="5" t="s">
+      <c r="C106" s="6" t="s">
         <v>173</v>
-      </c>
-      <c r="C106" s="6" t="s">
-        <v>174</v>
       </c>
       <c r="D106" s="29">
         <v>0</v>
@@ -8560,13 +8563,13 @@
     </row>
     <row r="107" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A107" s="10" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B107" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="C107" s="6" t="s">
         <v>174</v>
-      </c>
-      <c r="C107" s="6" t="s">
-        <v>175</v>
       </c>
       <c r="D107" s="29">
         <v>0</v>
@@ -8652,10 +8655,10 @@
     </row>
     <row r="108" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A108" s="10" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B108" s="5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C108" s="6" t="s">
         <v>13</v>
@@ -8744,7 +8747,7 @@
     </row>
     <row r="109" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A109" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C109" s="5"/>
       <c r="D109" s="5"/>
@@ -8777,13 +8780,13 @@
     </row>
     <row r="110" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A110" s="10" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B110" s="5" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C110" s="6" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D110" s="7" t="s">
         <v>14</v>
@@ -8869,13 +8872,13 @@
     </row>
     <row r="111" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A111" s="10" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B111" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="C111" s="6" t="s">
         <v>183</v>
-      </c>
-      <c r="C111" s="6" t="s">
-        <v>184</v>
       </c>
       <c r="D111" s="7" t="s">
         <v>13</v>
@@ -8961,13 +8964,13 @@
     </row>
     <row r="112" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A112" s="10" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B112" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="C112" s="6" t="s">
         <v>184</v>
-      </c>
-      <c r="C112" s="6" t="s">
-        <v>185</v>
       </c>
       <c r="D112" s="7" t="s">
         <v>13</v>
@@ -9053,13 +9056,13 @@
     </row>
     <row r="113" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A113" s="10" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B113" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="C113" s="6" t="s">
         <v>185</v>
-      </c>
-      <c r="C113" s="6" t="s">
-        <v>186</v>
       </c>
       <c r="D113" s="7" t="s">
         <v>14</v>
@@ -9145,13 +9148,13 @@
     </row>
     <row r="114" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A114" s="10" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B114" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="C114" s="6" t="s">
         <v>186</v>
-      </c>
-      <c r="C114" s="6" t="s">
-        <v>187</v>
       </c>
       <c r="D114" s="7" t="s">
         <v>13</v>
@@ -9237,13 +9240,13 @@
     </row>
     <row r="115" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A115" s="10" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B115" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="C115" s="6" t="s">
         <v>187</v>
-      </c>
-      <c r="C115" s="6" t="s">
-        <v>188</v>
       </c>
       <c r="D115" s="7" t="s">
         <v>14</v>
@@ -9329,10 +9332,10 @@
     </row>
     <row r="116" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A116" s="10" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B116" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C116" s="6" t="s">
         <v>13</v>
@@ -9421,7 +9424,7 @@
     </row>
     <row r="117" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A117" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C117" s="5"/>
       <c r="D117" s="5"/>
@@ -9454,7 +9457,7 @@
     </row>
     <row r="118" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A118" s="10" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E118" s="7"/>
       <c r="F118" s="7"/>
@@ -9485,13 +9488,13 @@
     </row>
     <row r="119" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A119" s="10" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B119" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="C119" s="6" t="s">
         <v>193</v>
-      </c>
-      <c r="C119" s="6" t="s">
-        <v>194</v>
       </c>
       <c r="D119" s="7" t="s">
         <v>14</v>
@@ -9577,13 +9580,13 @@
     </row>
     <row r="120" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A120" s="10" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B120" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="C120" s="6" t="s">
         <v>194</v>
-      </c>
-      <c r="C120" s="6" t="s">
-        <v>195</v>
       </c>
       <c r="E120" s="31">
         <v>0</v>
@@ -9663,13 +9666,13 @@
     </row>
     <row r="121" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A121" s="10" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B121" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="C121" s="6" t="s">
         <v>195</v>
-      </c>
-      <c r="C121" s="6" t="s">
-        <v>196</v>
       </c>
       <c r="D121" s="7" t="s">
         <v>13</v>
@@ -9755,13 +9758,13 @@
     </row>
     <row r="122" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A122" s="10" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B122" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="C122" s="6" t="s">
         <v>196</v>
-      </c>
-      <c r="C122" s="6" t="s">
-        <v>197</v>
       </c>
       <c r="D122" s="7" t="s">
         <v>13</v>
@@ -9847,13 +9850,13 @@
     </row>
     <row r="123" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A123" s="10" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B123" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="C123" s="6" t="s">
         <v>197</v>
-      </c>
-      <c r="C123" s="6" t="s">
-        <v>198</v>
       </c>
       <c r="D123" s="7" t="s">
         <v>14</v>
@@ -9939,13 +9942,13 @@
     </row>
     <row r="124" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A124" s="10" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B124" s="5" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C124" s="6" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D124" s="7" t="s">
         <v>13</v>
@@ -10031,13 +10034,13 @@
     </row>
     <row r="125" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A125" s="10" t="s">
+        <v>198</v>
+      </c>
+      <c r="B125" s="5" t="s">
         <v>199</v>
       </c>
-      <c r="B125" s="5" t="s">
+      <c r="C125" s="6" t="s">
         <v>200</v>
-      </c>
-      <c r="C125" s="6" t="s">
-        <v>201</v>
       </c>
       <c r="D125" s="7" t="s">
         <v>13</v>
@@ -10123,10 +10126,10 @@
     </row>
     <row r="126" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A126" s="26" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B126" s="5" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C126" s="6" t="s">
         <v>13</v>
@@ -10215,6 +10218,13 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="D1:G1"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="X1:Z1"/>
+    <mergeCell ref="S1:T1"/>
+    <mergeCell ref="O1:R1"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="H1:J1"/>
     <mergeCell ref="D2:G2"/>
     <mergeCell ref="O2:R2"/>
     <mergeCell ref="S2:T2"/>
@@ -10222,13 +10232,6 @@
     <mergeCell ref="H2:J2"/>
     <mergeCell ref="K2:L2"/>
     <mergeCell ref="M2:N2"/>
-    <mergeCell ref="D1:G1"/>
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="X1:Z1"/>
-    <mergeCell ref="S1:T1"/>
-    <mergeCell ref="O1:R1"/>
-    <mergeCell ref="K1:L1"/>
-    <mergeCell ref="H1:J1"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>